<commit_message>
Add validation for ABG assessment and update documentation
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Pulse\engine\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0364D484-1C7B-485C-8DEB-D9CD21BF3B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24AE0C5-D465-4C32-A1B9-F63E20425075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -23,12 +23,23 @@
     <sheet name="Respiratory" sheetId="35" r:id="rId8"/>
     <sheet name="Tissue" sheetId="34" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3978" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="1080">
   <si>
     <t>Output</t>
   </si>
@@ -3382,6 +3393,15 @@
   </si>
   <si>
     <t>Equal to System Property / Molar Mass * Valence</t>
+  </si>
+  <si>
+    <t>ArterialBloodGasTest</t>
+  </si>
+  <si>
+    <t>ABG@</t>
+  </si>
+  <si>
+    <t>8f</t>
   </si>
 </sst>
 </file>
@@ -5071,25 +5091,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1796875" style="51" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" style="52" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.28515625" style="51" customWidth="1"/>
+    <col min="8" max="8" width="49.26953125" style="51" customWidth="1"/>
     <col min="9" max="9" width="36" style="51" customWidth="1"/>
-    <col min="10" max="11" width="28.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="52" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="10" max="11" width="28.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="52" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
@@ -5714,7 +5734,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="56.25">
+    <row r="22" spans="1:12" ht="42">
       <c r="A22" s="109" t="s">
         <v>886</v>
       </c>
@@ -5744,7 +5764,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="22.5">
+    <row r="23" spans="1:12" ht="21">
       <c r="A23" s="15" t="s">
         <v>887</v>
       </c>
@@ -6547,10 +6567,10 @@
       <c r="H48" s="64"/>
       <c r="I48" s="64"/>
       <c r="J48" s="184" t="s">
-        <v>403</v>
+        <v>1077</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>411</v>
+        <v>1078</v>
       </c>
       <c r="L48" s="184" t="s">
         <v>966</v>
@@ -6581,10 +6601,10 @@
       <c r="H49" s="64"/>
       <c r="I49" s="64"/>
       <c r="J49" s="184" t="s">
-        <v>403</v>
+        <v>1077</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>411</v>
+        <v>1078</v>
       </c>
       <c r="L49" s="184" t="s">
         <v>966</v>
@@ -6615,10 +6635,10 @@
       <c r="H50" s="64"/>
       <c r="I50" s="64"/>
       <c r="J50" s="184" t="s">
-        <v>403</v>
+        <v>1077</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>411</v>
+        <v>1078</v>
       </c>
       <c r="L50" s="184" t="s">
         <v>966</v>
@@ -6649,10 +6669,10 @@
       <c r="H51" s="64"/>
       <c r="I51" s="64"/>
       <c r="J51" s="184" t="s">
-        <v>403</v>
+        <v>1077</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>411</v>
+        <v>1078</v>
       </c>
       <c r="L51" s="184" t="s">
         <v>966</v>
@@ -6681,10 +6701,10 @@
       <c r="H52" s="64"/>
       <c r="I52" s="64"/>
       <c r="J52" s="184" t="s">
-        <v>403</v>
+        <v>1077</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>411</v>
+        <v>1078</v>
       </c>
       <c r="L52" s="184" t="s">
         <v>966</v>
@@ -6792,7 +6812,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15">
+    <row r="56" spans="1:12" ht="14.5">
       <c r="A56" s="80" t="s">
         <v>431</v>
       </c>
@@ -6883,10 +6903,10 @@
         <v>410</v>
       </c>
       <c r="L58" s="151" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="12.75">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="12.5">
       <c r="A59" s="80" t="s">
         <v>434</v>
       </c>
@@ -8207,21 +8227,21 @@
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="29" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" style="28" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" style="107" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="52" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="5"/>
+    <col min="6" max="6" width="21.7265625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="32.7265625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="36.26953125" style="107" customWidth="1"/>
+    <col min="9" max="9" width="29.54296875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="27.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="52" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -8376,7 +8396,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="60">
+    <row r="6" spans="1:12" ht="48">
       <c r="A6" s="172" t="s">
         <v>170</v>
       </c>
@@ -8706,7 +8726,7 @@
       <c r="K17" s="184"/>
       <c r="L17" s="184"/>
     </row>
-    <row r="18" spans="1:12" s="51" customFormat="1" ht="60">
+    <row r="18" spans="1:12" s="51" customFormat="1" ht="48">
       <c r="A18" s="170" t="s">
         <v>169</v>
       </c>
@@ -8738,7 +8758,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="51" customFormat="1" ht="24">
+    <row r="19" spans="1:12" s="51" customFormat="1">
       <c r="A19" s="170" t="s">
         <v>202</v>
       </c>
@@ -8952,7 +8972,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="51" customFormat="1" ht="24">
+    <row r="27" spans="1:12" s="51" customFormat="1">
       <c r="A27" s="170" t="s">
         <v>903</v>
       </c>
@@ -9014,7 +9034,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="51" customFormat="1" ht="48">
+    <row r="29" spans="1:12" s="51" customFormat="1" ht="36">
       <c r="A29" s="170" t="s">
         <v>177</v>
       </c>
@@ -9524,7 +9544,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="36">
+    <row r="46" spans="1:12" ht="24">
       <c r="A46" s="170" t="s">
         <v>623</v>
       </c>
@@ -9786,7 +9806,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="36">
+    <row r="55" spans="1:12" ht="24">
       <c r="A55" s="170" t="s">
         <v>626</v>
       </c>
@@ -9844,7 +9864,7 @@
       <c r="K56" s="184"/>
       <c r="L56" s="184"/>
     </row>
-    <row r="57" spans="1:12" ht="24">
+    <row r="57" spans="1:12">
       <c r="A57" s="170" t="s">
         <v>647</v>
       </c>
@@ -9902,7 +9922,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="24">
+    <row r="59" spans="1:12">
       <c r="A59" s="170" t="s">
         <v>649</v>
       </c>
@@ -9960,7 +9980,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="24">
+    <row r="61" spans="1:12">
       <c r="A61" s="170" t="s">
         <v>651</v>
       </c>
@@ -10018,7 +10038,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="24">
+    <row r="63" spans="1:12">
       <c r="A63" s="170" t="s">
         <v>627</v>
       </c>
@@ -10196,7 +10216,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="24">
+    <row r="69" spans="1:12">
       <c r="A69" s="170" t="s">
         <v>653</v>
       </c>
@@ -10314,7 +10334,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="24">
+    <row r="73" spans="1:12">
       <c r="A73" s="170" t="s">
         <v>656</v>
       </c>
@@ -10404,7 +10424,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="24">
+    <row r="76" spans="1:12">
       <c r="A76" s="170" t="s">
         <v>659</v>
       </c>
@@ -10494,7 +10514,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="36">
+    <row r="79" spans="1:12" ht="24">
       <c r="A79" s="170" t="s">
         <v>633</v>
       </c>
@@ -10552,7 +10572,7 @@
       <c r="K80" s="184"/>
       <c r="L80" s="184"/>
     </row>
-    <row r="81" spans="1:12" ht="60">
+    <row r="81" spans="1:12" ht="48">
       <c r="A81" s="170" t="s">
         <v>662</v>
       </c>
@@ -10756,7 +10776,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="36">
+    <row r="88" spans="1:12" ht="24">
       <c r="A88" s="170" t="s">
         <v>636</v>
       </c>
@@ -10814,7 +10834,7 @@
       <c r="K89" s="184"/>
       <c r="L89" s="184"/>
     </row>
-    <row r="90" spans="1:12" ht="24">
+    <row r="90" spans="1:12">
       <c r="A90" s="170" t="s">
         <v>665</v>
       </c>
@@ -10872,7 +10892,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="24">
+    <row r="92" spans="1:12">
       <c r="A92" s="170" t="s">
         <v>667</v>
       </c>
@@ -10930,7 +10950,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="24">
+    <row r="94" spans="1:12">
       <c r="A94" s="170" t="s">
         <v>669</v>
       </c>
@@ -10988,7 +11008,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="24">
+    <row r="96" spans="1:12">
       <c r="A96" s="170" t="s">
         <v>637</v>
       </c>
@@ -11216,7 +11236,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="24">
+    <row r="104" spans="1:12">
       <c r="A104" s="170" t="s">
         <v>645</v>
       </c>
@@ -11303,20 +11323,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="21"/>
-    <col min="5" max="6" width="17.28515625" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" style="51" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="51" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="51" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="1" max="1" width="20.7265625" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="21"/>
+    <col min="5" max="6" width="17.26953125" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="29.7265625" style="51" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="51" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" style="51" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -11357,7 +11377,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="72">
+    <row r="2" spans="1:12" ht="60">
       <c r="A2" s="39" t="s">
         <v>172</v>
       </c>
@@ -11397,23 +11417,23 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L11" sqref="L11"/>
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="7" width="23.5703125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="9"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" customWidth="1"/>
+    <col min="6" max="7" width="23.54296875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.1796875" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="9"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -11537,6 +11557,9 @@
       </c>
       <c r="G5" s="10" t="s">
         <v>536</v>
+      </c>
+      <c r="J5" s="78" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="57" customFormat="1" ht="24">
@@ -11730,21 +11753,21 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="51" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="51" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="51" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" style="51" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="51" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" style="51" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" style="51" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" style="51" customWidth="1"/>
     <col min="6" max="6" width="12" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.7109375" style="84" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="7" max="7" width="5.1796875" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7265625" style="84" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -11828,18 +11851,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.26953125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="21"/>
-    <col min="5" max="6" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.7109375" style="21" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="21"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="21"/>
+    <col min="4" max="4" width="9.1796875" style="21"/>
+    <col min="5" max="6" width="17.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.7265625" style="21" customWidth="1"/>
+    <col min="9" max="10" width="9.1796875" style="21"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -11986,25 +12009,25 @@
   <dimension ref="A1:L413"/>
   <sheetViews>
     <sheetView topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I118" sqref="I118"/>
+      <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="85" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="85" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" style="85" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" style="85" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" style="51" customWidth="1"/>
     <col min="7" max="7" width="40" style="51" customWidth="1"/>
-    <col min="8" max="8" width="41.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="8" max="8" width="41.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.1796875" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12167,7 +12190,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="24">
+    <row r="6" spans="1:12">
       <c r="A6" s="65" t="s">
         <v>341</v>
       </c>
@@ -12486,7 +12509,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="24">
+    <row r="17" spans="1:12">
       <c r="A17" s="70" t="s">
         <v>438</v>
       </c>
@@ -12704,7 +12727,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="24">
+    <row r="24" spans="1:12">
       <c r="A24" s="17" t="s">
         <v>335</v>
       </c>
@@ -12944,7 +12967,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12" ht="24">
+    <row r="32" spans="1:12">
       <c r="A32" s="17" t="s">
         <v>338</v>
       </c>
@@ -13122,7 +13145,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="24">
+    <row r="38" spans="1:12">
       <c r="A38" s="70" t="s">
         <v>440</v>
       </c>
@@ -13340,7 +13363,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="24">
+    <row r="45" spans="1:12">
       <c r="A45" s="17" t="s">
         <v>334</v>
       </c>
@@ -13578,7 +13601,7 @@
       <c r="K52" s="56"/>
       <c r="L52" s="151"/>
     </row>
-    <row r="53" spans="1:12" ht="24">
+    <row r="53" spans="1:12">
       <c r="A53" s="17" t="s">
         <v>337</v>
       </c>
@@ -13734,7 +13757,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="48">
+    <row r="58" spans="1:12" ht="36">
       <c r="A58" s="65" t="s">
         <v>714</v>
       </c>
@@ -13764,7 +13787,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="48">
+    <row r="59" spans="1:12" ht="36">
       <c r="A59" s="65" t="s">
         <v>715</v>
       </c>
@@ -13794,7 +13817,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="48">
+    <row r="60" spans="1:12" ht="36">
       <c r="A60" s="65" t="s">
         <v>716</v>
       </c>
@@ -13824,7 +13847,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="48">
+    <row r="61" spans="1:12" ht="36">
       <c r="A61" s="65" t="s">
         <v>717</v>
       </c>
@@ -13854,7 +13877,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="48">
+    <row r="62" spans="1:12" ht="36">
       <c r="A62" s="65" t="s">
         <v>718</v>
       </c>
@@ -13884,7 +13907,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="48">
+    <row r="63" spans="1:12" ht="36">
       <c r="A63" s="65" t="s">
         <v>719</v>
       </c>
@@ -13914,7 +13937,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="48">
+    <row r="64" spans="1:12" ht="36">
       <c r="A64" s="65" t="s">
         <v>703</v>
       </c>
@@ -13944,7 +13967,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="48">
+    <row r="65" spans="1:12" ht="36">
       <c r="A65" s="65" t="s">
         <v>704</v>
       </c>
@@ -14006,7 +14029,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="36">
+    <row r="67" spans="1:12" ht="24">
       <c r="A67" s="120" t="s">
         <v>720</v>
       </c>
@@ -14038,7 +14061,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="48">
+    <row r="68" spans="1:12" ht="36">
       <c r="A68" s="120" t="s">
         <v>721</v>
       </c>
@@ -14068,7 +14091,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="48">
+    <row r="69" spans="1:12" ht="36">
       <c r="A69" s="120" t="s">
         <v>722</v>
       </c>
@@ -14098,7 +14121,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="48">
+    <row r="70" spans="1:12" ht="36">
       <c r="A70" s="120" t="s">
         <v>723</v>
       </c>
@@ -14128,7 +14151,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="48">
+    <row r="71" spans="1:12" ht="36">
       <c r="A71" s="120" t="s">
         <v>724</v>
       </c>
@@ -14158,7 +14181,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="48">
+    <row r="72" spans="1:12" ht="36">
       <c r="A72" s="120" t="s">
         <v>725</v>
       </c>
@@ -14188,7 +14211,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="48">
+    <row r="73" spans="1:12" ht="36">
       <c r="A73" s="120" t="s">
         <v>726</v>
       </c>
@@ -14218,7 +14241,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="48">
+    <row r="74" spans="1:12" ht="36">
       <c r="A74" s="120" t="s">
         <v>706</v>
       </c>
@@ -14248,7 +14271,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="48">
+    <row r="75" spans="1:12" ht="36">
       <c r="A75" s="120" t="s">
         <v>707</v>
       </c>
@@ -15334,7 +15357,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="36">
+    <row r="109" spans="1:12" ht="24">
       <c r="A109" s="65" t="s">
         <v>917</v>
       </c>
@@ -15428,7 +15451,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="36">
+    <row r="112" spans="1:12" ht="24">
       <c r="A112" s="65" t="s">
         <v>920</v>
       </c>
@@ -16462,7 +16485,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="145" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="145" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A145" s="8" t="s">
         <v>463</v>
       </c>
@@ -16500,7 +16523,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="146" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="146" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A146" s="80" t="s">
         <v>465</v>
       </c>
@@ -16528,7 +16551,7 @@
       </c>
       <c r="L146" s="56"/>
     </row>
-    <row r="147" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="147" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A147" s="80" t="s">
         <v>466</v>
       </c>
@@ -16548,7 +16571,7 @@
       </c>
       <c r="L147" s="56"/>
     </row>
-    <row r="148" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="148" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A148" s="80" t="s">
         <v>372</v>
       </c>
@@ -16576,7 +16599,7 @@
       </c>
       <c r="L148" s="56"/>
     </row>
-    <row r="149" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="149" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A149" s="80" t="s">
         <v>467</v>
       </c>
@@ -16604,7 +16627,7 @@
       </c>
       <c r="L149" s="56"/>
     </row>
-    <row r="150" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="150" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A150" s="80" t="s">
         <v>471</v>
       </c>
@@ -16624,7 +16647,7 @@
       </c>
       <c r="L150" s="56"/>
     </row>
-    <row r="151" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="151" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A151" s="80" t="s">
         <v>468</v>
       </c>
@@ -16658,7 +16681,7 @@
       </c>
       <c r="L151" s="56"/>
     </row>
-    <row r="152" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="152" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A152" s="80" t="s">
         <v>469</v>
       </c>
@@ -16686,7 +16709,7 @@
       </c>
       <c r="L152" s="56"/>
     </row>
-    <row r="153" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="153" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A153" s="80" t="s">
         <v>472</v>
       </c>
@@ -16706,7 +16729,7 @@
       </c>
       <c r="L153" s="56"/>
     </row>
-    <row r="154" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="154" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A154" s="80" t="s">
         <v>470</v>
       </c>
@@ -16734,7 +16757,7 @@
       </c>
       <c r="L154" s="56"/>
     </row>
-    <row r="155" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="155" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A155" s="80" t="s">
         <v>473</v>
       </c>
@@ -16754,7 +16777,7 @@
       </c>
       <c r="L155" s="56"/>
     </row>
-    <row r="156" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="156" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A156" s="80" t="s">
         <v>474</v>
       </c>
@@ -16774,7 +16797,7 @@
       </c>
       <c r="L156" s="56"/>
     </row>
-    <row r="157" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="157" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A157" s="80" t="s">
         <v>475</v>
       </c>
@@ -19330,21 +19353,21 @@
       <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="28" customWidth="1"/>
+    <col min="1" max="1" width="44.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="28" customWidth="1"/>
     <col min="3" max="3" width="30" style="28" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="28" customWidth="1"/>
     <col min="5" max="5" width="20" style="176" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="176" customWidth="1"/>
+    <col min="6" max="6" width="27.26953125" style="176" customWidth="1"/>
     <col min="7" max="7" width="24" style="176" customWidth="1"/>
-    <col min="8" max="8" width="37.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="81" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="185" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="185" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="24.7265625" style="81" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="185" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -19385,7 +19408,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48">
+    <row r="2" spans="1:12" ht="36">
       <c r="A2" s="170" t="s">
         <v>911</v>
       </c>
@@ -20021,7 +20044,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="60">
+    <row r="25" spans="1:12" ht="48">
       <c r="A25" s="170" t="s">
         <v>1029</v>
       </c>
@@ -20243,7 +20266,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="120">
+    <row r="33" spans="1:12" ht="96">
       <c r="A33" s="170" t="s">
         <v>986</v>
       </c>
@@ -20839,7 +20862,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="24">
+    <row r="54" spans="1:12">
       <c r="A54" s="170" t="s">
         <v>1020</v>
       </c>
@@ -20871,7 +20894,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="24">
+    <row r="55" spans="1:12">
       <c r="A55" s="170" t="s">
         <v>1020</v>
       </c>
@@ -22317,7 +22340,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="100" spans="1:12" s="163" customFormat="1" ht="24.75">
+    <row r="100" spans="1:12" s="163" customFormat="1" ht="24.5">
       <c r="A100" s="80" t="s">
         <v>386</v>
       </c>
@@ -22599,7 +22622,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="109" spans="1:12" s="163" customFormat="1" ht="24.75">
+    <row r="109" spans="1:12" s="163" customFormat="1" ht="24.5">
       <c r="A109" s="80" t="s">
         <v>390</v>
       </c>
@@ -22663,7 +22686,7 @@
       </c>
       <c r="L110" s="184"/>
     </row>
-    <row r="111" spans="1:12" s="163" customFormat="1" ht="24.75">
+    <row r="111" spans="1:12" s="163" customFormat="1" ht="24.5">
       <c r="A111" s="80" t="s">
         <v>391</v>
       </c>
@@ -22771,20 +22794,20 @@
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="105"/>
-    <col min="4" max="4" width="14.85546875" style="105" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="106" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="105" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.42578125" style="135" customWidth="1"/>
-    <col min="9" max="9" width="52.42578125" style="105" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="105" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="105"/>
-    <col min="12" max="12" width="12.5703125" style="105" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="105"/>
+    <col min="1" max="1" width="31.1796875" style="105" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1796875" style="105"/>
+    <col min="4" max="4" width="14.81640625" style="105" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" style="106" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" style="105" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" style="105" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.453125" style="135" customWidth="1"/>
+    <col min="9" max="9" width="52.453125" style="105" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" style="105" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" style="105"/>
+    <col min="12" max="12" width="12.54296875" style="105" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="105"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="51" customFormat="1" ht="26.25" customHeight="1">
@@ -24169,7 +24192,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="24.75">
+    <row r="42" spans="1:12">
       <c r="A42" s="109" t="s">
         <v>821</v>
       </c>
@@ -24349,7 +24372,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="36.75">
+    <row r="48" spans="1:12" ht="36.5">
       <c r="A48" s="109" t="s">
         <v>828</v>
       </c>
@@ -24371,7 +24394,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="72.75">
+    <row r="49" spans="1:12" ht="60.5">
       <c r="A49" s="109" t="s">
         <v>829</v>
       </c>
@@ -24461,7 +24484,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="24.75">
+    <row r="52" spans="1:12" ht="24">
       <c r="A52" s="109" t="s">
         <v>832</v>
       </c>
@@ -24493,7 +24516,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="48.75">
+    <row r="53" spans="1:12" ht="36.5">
       <c r="A53" s="109" t="s">
         <v>833</v>
       </c>
@@ -24721,7 +24744,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="24.75">
+    <row r="61" spans="1:12">
       <c r="A61" s="109" t="s">
         <v>841</v>
       </c>
@@ -24895,7 +24918,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="36.75">
+    <row r="67" spans="1:12" ht="24.5">
       <c r="A67" s="109" t="s">
         <v>847</v>
       </c>
@@ -24921,7 +24944,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="72.75">
+    <row r="68" spans="1:12" ht="60.5">
       <c r="A68" s="109" t="s">
         <v>848</v>
       </c>
@@ -25011,7 +25034,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="24.75">
+    <row r="71" spans="1:12" ht="24">
       <c r="A71" s="109" t="s">
         <v>851</v>
       </c>
@@ -25043,7 +25066,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="48.75">
+    <row r="72" spans="1:12" ht="36.5">
       <c r="A72" s="109" t="s">
         <v>852</v>
       </c>

</xml_diff>

<commit_message>
Added RelativeTotalLungVolume to respiratory system data.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\respiratory-mechanics-source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24AE0C5-D465-4C32-A1B9-F63E20425075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C95253-E957-45A0-ACE8-5941CE30A7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="43200" windowHeight="23535" tabRatio="724" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3987" uniqueCount="1082">
   <si>
     <t>Output</t>
   </si>
@@ -3402,6 +3402,13 @@
   </si>
   <si>
     <t>8f</t>
+  </si>
+  <si>
+    <t>RelativeTotalLungVolume</t>
+  </si>
+  <si>
+    <t>Derived from Tidal Volume (TV) 
+~1/2 TV</t>
   </si>
 </sst>
 </file>
@@ -5091,25 +5098,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="40.1796875" style="51" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.81640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="52" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="51" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="52" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.26953125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="49.28515625" style="51" customWidth="1"/>
     <col min="9" max="9" width="36" style="51" customWidth="1"/>
-    <col min="10" max="11" width="28.81640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="52" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="51"/>
+    <col min="10" max="11" width="28.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="52" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
@@ -5734,7 +5741,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="42">
+    <row r="22" spans="1:12" ht="56.25">
       <c r="A22" s="109" t="s">
         <v>886</v>
       </c>
@@ -5764,7 +5771,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="21">
+    <row r="23" spans="1:12" ht="22.5">
       <c r="A23" s="15" t="s">
         <v>887</v>
       </c>
@@ -6812,7 +6819,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="14.5">
+    <row r="56" spans="1:12" ht="15">
       <c r="A56" s="80" t="s">
         <v>431</v>
       </c>
@@ -6906,7 +6913,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="12.5">
+    <row r="59" spans="1:12" ht="12.75">
       <c r="A59" s="80" t="s">
         <v>434</v>
       </c>
@@ -8227,21 +8234,21 @@
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="29" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="32.7265625" style="28" customWidth="1"/>
-    <col min="8" max="8" width="36.26953125" style="107" customWidth="1"/>
-    <col min="9" max="9" width="29.54296875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="27.54296875" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.81640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="52" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="5"/>
+    <col min="6" max="6" width="21.7109375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" style="28" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="107" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="52" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -8396,7 +8403,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48">
+    <row r="6" spans="1:12" ht="60">
       <c r="A6" s="172" t="s">
         <v>170</v>
       </c>
@@ -8726,7 +8733,7 @@
       <c r="K17" s="184"/>
       <c r="L17" s="184"/>
     </row>
-    <row r="18" spans="1:12" s="51" customFormat="1" ht="48">
+    <row r="18" spans="1:12" s="51" customFormat="1" ht="60">
       <c r="A18" s="170" t="s">
         <v>169</v>
       </c>
@@ -8758,7 +8765,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="51" customFormat="1">
+    <row r="19" spans="1:12" s="51" customFormat="1" ht="24">
       <c r="A19" s="170" t="s">
         <v>202</v>
       </c>
@@ -8972,7 +8979,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="51" customFormat="1">
+    <row r="27" spans="1:12" s="51" customFormat="1" ht="24">
       <c r="A27" s="170" t="s">
         <v>903</v>
       </c>
@@ -9034,7 +9041,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="51" customFormat="1" ht="36">
+    <row r="29" spans="1:12" s="51" customFormat="1" ht="48">
       <c r="A29" s="170" t="s">
         <v>177</v>
       </c>
@@ -9544,7 +9551,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="24">
+    <row r="46" spans="1:12" ht="36">
       <c r="A46" s="170" t="s">
         <v>623</v>
       </c>
@@ -9806,7 +9813,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="24">
+    <row r="55" spans="1:12" ht="36">
       <c r="A55" s="170" t="s">
         <v>626</v>
       </c>
@@ -9864,7 +9871,7 @@
       <c r="K56" s="184"/>
       <c r="L56" s="184"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" ht="24">
       <c r="A57" s="170" t="s">
         <v>647</v>
       </c>
@@ -9922,7 +9929,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" ht="24">
       <c r="A59" s="170" t="s">
         <v>649</v>
       </c>
@@ -9980,7 +9987,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" ht="24">
       <c r="A61" s="170" t="s">
         <v>651</v>
       </c>
@@ -10038,7 +10045,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" ht="24">
       <c r="A63" s="170" t="s">
         <v>627</v>
       </c>
@@ -10216,7 +10223,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" ht="24">
       <c r="A69" s="170" t="s">
         <v>653</v>
       </c>
@@ -10334,7 +10341,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" ht="24">
       <c r="A73" s="170" t="s">
         <v>656</v>
       </c>
@@ -10424,7 +10431,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" ht="24">
       <c r="A76" s="170" t="s">
         <v>659</v>
       </c>
@@ -10514,7 +10521,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="24">
+    <row r="79" spans="1:12" ht="36">
       <c r="A79" s="170" t="s">
         <v>633</v>
       </c>
@@ -10572,7 +10579,7 @@
       <c r="K80" s="184"/>
       <c r="L80" s="184"/>
     </row>
-    <row r="81" spans="1:12" ht="48">
+    <row r="81" spans="1:12" ht="60">
       <c r="A81" s="170" t="s">
         <v>662</v>
       </c>
@@ -10776,7 +10783,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="24">
+    <row r="88" spans="1:12" ht="36">
       <c r="A88" s="170" t="s">
         <v>636</v>
       </c>
@@ -10834,7 +10841,7 @@
       <c r="K89" s="184"/>
       <c r="L89" s="184"/>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" ht="24">
       <c r="A90" s="170" t="s">
         <v>665</v>
       </c>
@@ -10892,7 +10899,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" ht="24">
       <c r="A92" s="170" t="s">
         <v>667</v>
       </c>
@@ -10950,7 +10957,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" ht="24">
       <c r="A94" s="170" t="s">
         <v>669</v>
       </c>
@@ -11008,7 +11015,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" ht="24">
       <c r="A96" s="170" t="s">
         <v>637</v>
       </c>
@@ -11236,7 +11243,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" ht="24">
       <c r="A104" s="170" t="s">
         <v>645</v>
       </c>
@@ -11323,20 +11330,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="21"/>
-    <col min="5" max="6" width="17.26953125" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" style="51" customWidth="1"/>
-    <col min="8" max="8" width="29.7265625" style="51" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="51" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" style="51" customWidth="1"/>
-    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="51"/>
+    <col min="1" max="1" width="20.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="21"/>
+    <col min="5" max="6" width="17.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="51" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="51" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="51" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="51" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -11377,7 +11384,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60">
+    <row r="2" spans="1:12" ht="72">
       <c r="A2" s="39" t="s">
         <v>172</v>
       </c>
@@ -11421,22 +11428,22 @@
       <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" customWidth="1"/>
-    <col min="6" max="7" width="23.54296875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.1796875" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="9"/>
-    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="7" width="23.5703125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="9"/>
+    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="24">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -11753,21 +11760,21 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="26.453125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" style="51" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" style="51" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="51" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="51" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="51" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="51" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="51" customWidth="1"/>
     <col min="6" max="6" width="12" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.1796875" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.7265625" style="84" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="51" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="51"/>
+    <col min="7" max="7" width="5.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" style="84" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -11851,18 +11858,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="28.26953125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="21"/>
-    <col min="5" max="6" width="17.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.7265625" style="21" customWidth="1"/>
-    <col min="9" max="10" width="9.1796875" style="21"/>
-    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="21"/>
+    <col min="4" max="4" width="9.140625" style="21"/>
+    <col min="5" max="6" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.7109375" style="21" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="21"/>
+    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -12013,21 +12020,21 @@
       <selection pane="topRight" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.453125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="85" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="85" customWidth="1"/>
-    <col min="6" max="6" width="28.54296875" style="51" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="85" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="85" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="51" customWidth="1"/>
     <col min="7" max="7" width="40" style="51" customWidth="1"/>
-    <col min="8" max="8" width="41.81640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.1796875" style="51" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.453125" style="52" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="51"/>
+    <col min="8" max="8" width="41.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12190,7 +12197,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="24">
       <c r="A6" s="65" t="s">
         <v>341</v>
       </c>
@@ -12509,7 +12516,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="24">
       <c r="A17" s="70" t="s">
         <v>438</v>
       </c>
@@ -12727,7 +12734,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="24">
       <c r="A24" s="17" t="s">
         <v>335</v>
       </c>
@@ -12967,7 +12974,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="24">
       <c r="A32" s="17" t="s">
         <v>338</v>
       </c>
@@ -13145,7 +13152,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" ht="24">
       <c r="A38" s="70" t="s">
         <v>440</v>
       </c>
@@ -13363,7 +13370,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" ht="24">
       <c r="A45" s="17" t="s">
         <v>334</v>
       </c>
@@ -13601,7 +13608,7 @@
       <c r="K52" s="56"/>
       <c r="L52" s="151"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" ht="24">
       <c r="A53" s="17" t="s">
         <v>337</v>
       </c>
@@ -13757,7 +13764,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="36">
+    <row r="58" spans="1:12" ht="48">
       <c r="A58" s="65" t="s">
         <v>714</v>
       </c>
@@ -13787,7 +13794,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="36">
+    <row r="59" spans="1:12" ht="48">
       <c r="A59" s="65" t="s">
         <v>715</v>
       </c>
@@ -13817,7 +13824,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="36">
+    <row r="60" spans="1:12" ht="48">
       <c r="A60" s="65" t="s">
         <v>716</v>
       </c>
@@ -13847,7 +13854,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="36">
+    <row r="61" spans="1:12" ht="48">
       <c r="A61" s="65" t="s">
         <v>717</v>
       </c>
@@ -13877,7 +13884,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="36">
+    <row r="62" spans="1:12" ht="48">
       <c r="A62" s="65" t="s">
         <v>718</v>
       </c>
@@ -13907,7 +13914,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="36">
+    <row r="63" spans="1:12" ht="48">
       <c r="A63" s="65" t="s">
         <v>719</v>
       </c>
@@ -13937,7 +13944,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="36">
+    <row r="64" spans="1:12" ht="48">
       <c r="A64" s="65" t="s">
         <v>703</v>
       </c>
@@ -13967,7 +13974,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="36">
+    <row r="65" spans="1:12" ht="48">
       <c r="A65" s="65" t="s">
         <v>704</v>
       </c>
@@ -14029,7 +14036,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="24">
+    <row r="67" spans="1:12" ht="36">
       <c r="A67" s="120" t="s">
         <v>720</v>
       </c>
@@ -14061,7 +14068,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="36">
+    <row r="68" spans="1:12" ht="48">
       <c r="A68" s="120" t="s">
         <v>721</v>
       </c>
@@ -14091,7 +14098,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="36">
+    <row r="69" spans="1:12" ht="48">
       <c r="A69" s="120" t="s">
         <v>722</v>
       </c>
@@ -14121,7 +14128,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="36">
+    <row r="70" spans="1:12" ht="48">
       <c r="A70" s="120" t="s">
         <v>723</v>
       </c>
@@ -14151,7 +14158,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="36">
+    <row r="71" spans="1:12" ht="48">
       <c r="A71" s="120" t="s">
         <v>724</v>
       </c>
@@ -14181,7 +14188,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="36">
+    <row r="72" spans="1:12" ht="48">
       <c r="A72" s="120" t="s">
         <v>725</v>
       </c>
@@ -14211,7 +14218,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="36">
+    <row r="73" spans="1:12" ht="48">
       <c r="A73" s="120" t="s">
         <v>726</v>
       </c>
@@ -14241,7 +14248,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="36">
+    <row r="74" spans="1:12" ht="48">
       <c r="A74" s="120" t="s">
         <v>706</v>
       </c>
@@ -14271,7 +14278,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="36">
+    <row r="75" spans="1:12" ht="48">
       <c r="A75" s="120" t="s">
         <v>707</v>
       </c>
@@ -15357,7 +15364,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="24">
+    <row r="109" spans="1:12" ht="36">
       <c r="A109" s="65" t="s">
         <v>917</v>
       </c>
@@ -15451,7 +15458,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="24">
+    <row r="112" spans="1:12" ht="36">
       <c r="A112" s="65" t="s">
         <v>920</v>
       </c>
@@ -16485,7 +16492,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="145" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="145" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A145" s="8" t="s">
         <v>463</v>
       </c>
@@ -16523,7 +16530,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="146" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="146" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A146" s="80" t="s">
         <v>465</v>
       </c>
@@ -16551,7 +16558,7 @@
       </c>
       <c r="L146" s="56"/>
     </row>
-    <row r="147" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="147" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A147" s="80" t="s">
         <v>466</v>
       </c>
@@ -16571,7 +16578,7 @@
       </c>
       <c r="L147" s="56"/>
     </row>
-    <row r="148" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="148" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A148" s="80" t="s">
         <v>372</v>
       </c>
@@ -16599,7 +16606,7 @@
       </c>
       <c r="L148" s="56"/>
     </row>
-    <row r="149" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="149" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A149" s="80" t="s">
         <v>467</v>
       </c>
@@ -16627,7 +16634,7 @@
       </c>
       <c r="L149" s="56"/>
     </row>
-    <row r="150" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="150" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A150" s="80" t="s">
         <v>471</v>
       </c>
@@ -16647,7 +16654,7 @@
       </c>
       <c r="L150" s="56"/>
     </row>
-    <row r="151" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="151" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A151" s="80" t="s">
         <v>468</v>
       </c>
@@ -16681,7 +16688,7 @@
       </c>
       <c r="L151" s="56"/>
     </row>
-    <row r="152" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="152" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A152" s="80" t="s">
         <v>469</v>
       </c>
@@ -16709,7 +16716,7 @@
       </c>
       <c r="L152" s="56"/>
     </row>
-    <row r="153" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="153" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A153" s="80" t="s">
         <v>472</v>
       </c>
@@ -16729,7 +16736,7 @@
       </c>
       <c r="L153" s="56"/>
     </row>
-    <row r="154" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="154" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A154" s="80" t="s">
         <v>470</v>
       </c>
@@ -16757,7 +16764,7 @@
       </c>
       <c r="L154" s="56"/>
     </row>
-    <row r="155" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="155" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A155" s="80" t="s">
         <v>473</v>
       </c>
@@ -16777,7 +16784,7 @@
       </c>
       <c r="L155" s="56"/>
     </row>
-    <row r="156" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="156" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A156" s="80" t="s">
         <v>474</v>
       </c>
@@ -16797,7 +16804,7 @@
       </c>
       <c r="L156" s="56"/>
     </row>
-    <row r="157" spans="1:12" s="57" customFormat="1" ht="14.5">
+    <row r="157" spans="1:12" s="57" customFormat="1" ht="15">
       <c r="A157" s="80" t="s">
         <v>475</v>
       </c>
@@ -19344,30 +19351,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F8F0F7-B210-4329-9304-9AF1284E2465}">
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomRight" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="28" customWidth="1"/>
     <col min="3" max="3" width="30" style="28" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="28" customWidth="1"/>
     <col min="5" max="5" width="20" style="176" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" style="176" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="176" customWidth="1"/>
     <col min="7" max="7" width="24" style="176" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" style="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.7265625" style="81" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.81640625" style="185" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.453125" style="185" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="1"/>
+    <col min="10" max="10" width="24.7109375" style="81" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" style="185" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" style="185" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -19408,7 +19415,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="36">
+    <row r="2" spans="1:12" ht="48">
       <c r="A2" s="170" t="s">
         <v>911</v>
       </c>
@@ -20044,7 +20051,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="48">
+    <row r="25" spans="1:12" ht="60">
       <c r="A25" s="170" t="s">
         <v>1029</v>
       </c>
@@ -20266,7 +20273,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="96">
+    <row r="33" spans="1:12" ht="120">
       <c r="A33" s="170" t="s">
         <v>986</v>
       </c>
@@ -20360,20 +20367,30 @@
         <v>778</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="172" t="s">
-        <v>1014</v>
-      </c>
-      <c r="B36" s="180" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C36" s="167"/>
-      <c r="D36" s="167"/>
-      <c r="E36" s="180"/>
-      <c r="F36" s="180"/>
+    <row r="36" spans="1:12" s="163" customFormat="1" ht="24">
+      <c r="A36" s="170" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B36" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C36" s="167" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D36" s="180">
+        <v>3.5</v>
+      </c>
+      <c r="E36" s="180" t="s">
+        <v>241</v>
+      </c>
+      <c r="F36" s="165" t="s">
+        <v>246</v>
+      </c>
       <c r="G36" s="180"/>
-      <c r="H36" s="183"/>
-      <c r="I36" s="34"/>
+      <c r="H36" s="183" t="s">
+        <v>1081</v>
+      </c>
+      <c r="I36" s="32"/>
       <c r="J36" s="82" t="s">
         <v>383</v>
       </c>
@@ -20384,7 +20401,7 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="172" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B37" s="180" t="s">
         <v>1004</v>
@@ -20404,28 +20421,20 @@
         <v>778</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="36">
-      <c r="A38" s="170" t="s">
-        <v>232</v>
-      </c>
-      <c r="B38" s="62" t="s">
-        <v>199</v>
-      </c>
-      <c r="C38" s="167" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" s="62" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E38" s="196" t="s">
-        <v>1000</v>
-      </c>
-      <c r="F38" s="165" t="s">
-        <v>1001</v>
-      </c>
+    <row r="38" spans="1:12">
+      <c r="A38" s="172" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B38" s="180" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C38" s="167"/>
+      <c r="D38" s="167"/>
+      <c r="E38" s="180"/>
+      <c r="F38" s="180"/>
       <c r="G38" s="180"/>
       <c r="H38" s="183"/>
-      <c r="I38" s="33"/>
+      <c r="I38" s="34"/>
       <c r="J38" s="82" t="s">
         <v>383</v>
       </c>
@@ -20434,24 +20443,28 @@
         <v>778</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="172" t="s">
-        <v>1053</v>
-      </c>
-      <c r="B39" s="180"/>
+    <row r="39" spans="1:12" ht="36">
+      <c r="A39" s="170" t="s">
+        <v>232</v>
+      </c>
+      <c r="B39" s="62" t="s">
+        <v>199</v>
+      </c>
       <c r="C39" s="167" t="s">
         <v>167</v>
       </c>
-      <c r="D39" s="167">
-        <v>0</v>
-      </c>
-      <c r="E39" s="180" t="s">
-        <v>1034</v>
-      </c>
-      <c r="F39" s="180"/>
+      <c r="D39" s="62" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E39" s="196" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F39" s="165" t="s">
+        <v>1001</v>
+      </c>
       <c r="G39" s="180"/>
       <c r="H39" s="183"/>
-      <c r="I39" s="34"/>
+      <c r="I39" s="33"/>
       <c r="J39" s="82" t="s">
         <v>383</v>
       </c>
@@ -20460,18 +20473,24 @@
         <v>778</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="163" customFormat="1">
+    <row r="40" spans="1:12">
       <c r="A40" s="172" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B40" s="54"/>
-      <c r="C40" s="167"/>
-      <c r="D40" s="167"/>
-      <c r="E40" s="167"/>
-      <c r="F40" s="167"/>
-      <c r="G40" s="167"/>
-      <c r="H40" s="167"/>
-      <c r="I40" s="167"/>
+        <v>1053</v>
+      </c>
+      <c r="B40" s="180"/>
+      <c r="C40" s="167" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="167">
+        <v>0</v>
+      </c>
+      <c r="E40" s="180" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F40" s="180"/>
+      <c r="G40" s="180"/>
+      <c r="H40" s="183"/>
+      <c r="I40" s="34"/>
       <c r="J40" s="82" t="s">
         <v>383</v>
       </c>
@@ -20481,23 +20500,15 @@
       </c>
     </row>
     <row r="41" spans="1:12" s="163" customFormat="1">
-      <c r="A41" s="170" t="s">
-        <v>1067</v>
+      <c r="A41" s="172" t="s">
+        <v>1031</v>
       </c>
       <c r="B41" s="54"/>
-      <c r="C41" s="167" t="s">
-        <v>167</v>
-      </c>
-      <c r="D41" s="167">
-        <v>4.62</v>
-      </c>
-      <c r="E41" s="167" t="s">
-        <v>92</v>
-      </c>
+      <c r="C41" s="167"/>
+      <c r="D41" s="167"/>
+      <c r="E41" s="167"/>
       <c r="F41" s="167"/>
-      <c r="G41" s="167" t="s">
-        <v>1068</v>
-      </c>
+      <c r="G41" s="167"/>
       <c r="H41" s="167"/>
       <c r="I41" s="167"/>
       <c r="J41" s="82" t="s">
@@ -20508,28 +20519,26 @@
         <v>778</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="24">
+    <row r="42" spans="1:12" s="163" customFormat="1">
       <c r="A42" s="170" t="s">
-        <v>233</v>
-      </c>
-      <c r="B42" s="180"/>
+        <v>1067</v>
+      </c>
+      <c r="B42" s="54"/>
       <c r="C42" s="167" t="s">
         <v>167</v>
       </c>
-      <c r="D42" s="180">
-        <v>0.23</v>
-      </c>
-      <c r="E42" s="180" t="s">
-        <v>241</v>
-      </c>
-      <c r="F42" s="165" t="s">
-        <v>246</v>
-      </c>
-      <c r="G42" s="180"/>
-      <c r="H42" s="183" t="s">
-        <v>320</v>
-      </c>
-      <c r="I42" s="30"/>
+      <c r="D42" s="167">
+        <v>4.62</v>
+      </c>
+      <c r="E42" s="167" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="167"/>
+      <c r="G42" s="167" t="s">
+        <v>1068</v>
+      </c>
+      <c r="H42" s="167"/>
+      <c r="I42" s="167"/>
       <c r="J42" s="82" t="s">
         <v>383</v>
       </c>
@@ -20538,18 +20547,16 @@
         <v>778</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" ht="24">
       <c r="A43" s="170" t="s">
-        <v>234</v>
-      </c>
-      <c r="B43" s="180" t="s">
-        <v>7</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="B43" s="180"/>
       <c r="C43" s="167" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D43" s="167">
-        <v>7</v>
+        <v>167</v>
+      </c>
+      <c r="D43" s="180">
+        <v>0.23</v>
       </c>
       <c r="E43" s="180" t="s">
         <v>241</v>
@@ -20558,28 +20565,30 @@
         <v>246</v>
       </c>
       <c r="G43" s="180"/>
-      <c r="H43" s="183"/>
-      <c r="I43" s="34"/>
+      <c r="H43" s="183" t="s">
+        <v>320</v>
+      </c>
+      <c r="I43" s="30"/>
       <c r="J43" s="82" t="s">
         <v>383</v>
       </c>
       <c r="K43" s="184"/>
       <c r="L43" s="184" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="24">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="170" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B44" s="180" t="s">
-        <v>361</v>
+        <v>7</v>
       </c>
       <c r="C44" s="167" t="s">
         <v>1035</v>
       </c>
       <c r="D44" s="167">
-        <v>0.08</v>
+        <v>7</v>
       </c>
       <c r="E44" s="180" t="s">
         <v>241</v>
@@ -20588,21 +20597,19 @@
         <v>246</v>
       </c>
       <c r="G44" s="180"/>
-      <c r="H44" s="183" t="s">
-        <v>244</v>
-      </c>
+      <c r="H44" s="183"/>
       <c r="I44" s="34"/>
       <c r="J44" s="82" t="s">
         <v>383</v>
       </c>
       <c r="K44" s="184"/>
       <c r="L44" s="184" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="24">
       <c r="A45" s="170" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B45" s="180" t="s">
         <v>361</v>
@@ -20611,8 +20618,7 @@
         <v>1035</v>
       </c>
       <c r="D45" s="167">
-        <f>0.002*12</f>
-        <v>2.4E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E45" s="180" t="s">
         <v>241</v>
@@ -20622,9 +20628,9 @@
       </c>
       <c r="G45" s="180"/>
       <c r="H45" s="183" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="177"/>
+        <v>244</v>
+      </c>
+      <c r="I45" s="34"/>
       <c r="J45" s="82" t="s">
         <v>383</v>
       </c>
@@ -20633,18 +20639,19 @@
         <v>778</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="163" customFormat="1" ht="36">
+    <row r="46" spans="1:12" ht="24">
       <c r="A46" s="170" t="s">
-        <v>237</v>
-      </c>
-      <c r="B46" s="62" t="s">
-        <v>362</v>
+        <v>236</v>
+      </c>
+      <c r="B46" s="180" t="s">
+        <v>361</v>
       </c>
       <c r="C46" s="167" t="s">
         <v>1035</v>
       </c>
-      <c r="D46" s="180">
-        <v>3.3500000000000002E-2</v>
+      <c r="D46" s="167">
+        <f>0.002*12</f>
+        <v>2.4E-2</v>
       </c>
       <c r="E46" s="180" t="s">
         <v>241</v>
@@ -20654,9 +20661,9 @@
       </c>
       <c r="G46" s="180"/>
       <c r="H46" s="183" t="s">
-        <v>261</v>
-      </c>
-      <c r="I46" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="I46" s="177"/>
       <c r="J46" s="82" t="s">
         <v>383</v>
       </c>
@@ -20665,20 +20672,30 @@
         <v>778</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="172" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B47" s="180" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C47" s="167"/>
-      <c r="D47" s="167"/>
-      <c r="E47" s="180"/>
-      <c r="F47" s="180"/>
+    <row r="47" spans="1:12" s="163" customFormat="1" ht="36">
+      <c r="A47" s="170" t="s">
+        <v>237</v>
+      </c>
+      <c r="B47" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C47" s="167" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D47" s="180">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="E47" s="180" t="s">
+        <v>241</v>
+      </c>
+      <c r="F47" s="165" t="s">
+        <v>246</v>
+      </c>
       <c r="G47" s="180"/>
-      <c r="H47" s="183"/>
-      <c r="I47" s="34"/>
+      <c r="H47" s="183" t="s">
+        <v>261</v>
+      </c>
+      <c r="I47" s="32"/>
       <c r="J47" s="82" t="s">
         <v>383</v>
       </c>
@@ -20687,30 +20704,19 @@
         <v>778</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="45.75" customHeight="1">
-      <c r="A48" s="170" t="s">
-        <v>238</v>
+    <row r="48" spans="1:12">
+      <c r="A48" s="172" t="s">
+        <v>1010</v>
       </c>
       <c r="B48" s="180" t="s">
-        <v>361</v>
-      </c>
-      <c r="C48" s="167" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D48" s="167">
-        <f>0.007*12</f>
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="E48" s="180" t="s">
-        <v>241</v>
-      </c>
-      <c r="F48" s="165" t="s">
-        <v>246</v>
-      </c>
+        <v>1005</v>
+      </c>
+      <c r="C48" s="167"/>
+      <c r="D48" s="167"/>
+      <c r="E48" s="180"/>
+      <c r="F48" s="180"/>
       <c r="G48" s="180"/>
-      <c r="H48" s="183" t="s">
-        <v>260</v>
-      </c>
+      <c r="H48" s="183"/>
       <c r="I48" s="34"/>
       <c r="J48" s="82" t="s">
         <v>383</v>
@@ -20720,19 +20726,30 @@
         <v>778</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="172" t="s">
-        <v>1007</v>
+    <row r="49" spans="1:12" ht="45.75" customHeight="1">
+      <c r="A49" s="170" t="s">
+        <v>238</v>
       </c>
       <c r="B49" s="180" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C49" s="167"/>
-      <c r="D49" s="167"/>
-      <c r="E49" s="180"/>
-      <c r="F49" s="180"/>
+        <v>361</v>
+      </c>
+      <c r="C49" s="167" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D49" s="167">
+        <f>0.007*12</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E49" s="180" t="s">
+        <v>241</v>
+      </c>
+      <c r="F49" s="165" t="s">
+        <v>246</v>
+      </c>
       <c r="G49" s="180"/>
-      <c r="H49" s="183"/>
+      <c r="H49" s="183" t="s">
+        <v>260</v>
+      </c>
       <c r="I49" s="34"/>
       <c r="J49" s="82" t="s">
         <v>383</v>
@@ -20743,24 +20760,16 @@
       </c>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="170" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B50" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="182" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D50" s="167">
-        <v>-1</v>
-      </c>
-      <c r="E50" s="180" t="s">
-        <v>241</v>
-      </c>
-      <c r="F50" s="180" t="s">
-        <v>999</v>
-      </c>
+      <c r="A50" s="172" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B50" s="180" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C50" s="167"/>
+      <c r="D50" s="167"/>
+      <c r="E50" s="180"/>
+      <c r="F50" s="180"/>
       <c r="G50" s="180"/>
       <c r="H50" s="183"/>
       <c r="I50" s="34"/>
@@ -20780,10 +20789,10 @@
         <v>8</v>
       </c>
       <c r="C51" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D51" s="167">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E51" s="180" t="s">
         <v>241</v>
@@ -20804,22 +20813,22 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="170" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B52" s="180" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B52" s="62" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D52" s="167">
-        <v>5.2</v>
+        <v>1</v>
       </c>
       <c r="E52" s="180" t="s">
-        <v>92</v>
+        <v>241</v>
       </c>
       <c r="F52" s="180" t="s">
-        <v>240</v>
+        <v>999</v>
       </c>
       <c r="G52" s="180"/>
       <c r="H52" s="183"/>
@@ -20840,10 +20849,10 @@
         <v>8</v>
       </c>
       <c r="C53" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D53" s="167">
-        <v>7.2</v>
+        <v>5.2</v>
       </c>
       <c r="E53" s="180" t="s">
         <v>92</v>
@@ -20864,27 +20873,25 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="170" t="s">
-        <v>1020</v>
-      </c>
-      <c r="B54" s="62" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B54" s="180" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="182" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D54" s="162">
-        <v>-8</v>
+        <v>1045</v>
+      </c>
+      <c r="D54" s="167">
+        <v>7.2</v>
       </c>
       <c r="E54" s="180" t="s">
-        <v>241</v>
-      </c>
-      <c r="F54" s="165" t="s">
-        <v>988</v>
+        <v>92</v>
+      </c>
+      <c r="F54" s="180" t="s">
+        <v>240</v>
       </c>
       <c r="G54" s="180"/>
-      <c r="H54" s="183" t="s">
-        <v>995</v>
-      </c>
+      <c r="H54" s="183"/>
       <c r="I54" s="34"/>
       <c r="J54" s="82" t="s">
         <v>383</v>
@@ -20894,7 +20901,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" ht="24">
       <c r="A55" s="170" t="s">
         <v>1020</v>
       </c>
@@ -20902,10 +20909,10 @@
         <v>8</v>
       </c>
       <c r="C55" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D55" s="162">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="E55" s="180" t="s">
         <v>241</v>
@@ -20926,26 +20933,28 @@
         <v>778</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" ht="24">
       <c r="A56" s="170" t="s">
-        <v>1051</v>
+        <v>1020</v>
       </c>
       <c r="B56" s="62" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="182" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D56" s="193">
-        <v>-5.4</v>
+        <v>1045</v>
+      </c>
+      <c r="D56" s="162">
+        <v>-5</v>
       </c>
       <c r="E56" s="180" t="s">
-        <v>92</v>
-      </c>
-      <c r="F56" s="165"/>
+        <v>241</v>
+      </c>
+      <c r="F56" s="165" t="s">
+        <v>988</v>
+      </c>
       <c r="G56" s="180"/>
       <c r="H56" s="183" t="s">
-        <v>1052</v>
+        <v>995</v>
       </c>
       <c r="I56" s="34"/>
       <c r="J56" s="82" t="s">
@@ -20964,17 +20973,19 @@
         <v>8</v>
       </c>
       <c r="C57" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D57" s="193">
-        <v>0</v>
+        <v>-5.4</v>
       </c>
       <c r="E57" s="180" t="s">
         <v>92</v>
       </c>
       <c r="F57" s="165"/>
       <c r="G57" s="180"/>
-      <c r="H57" s="183"/>
+      <c r="H57" s="183" t="s">
+        <v>1052</v>
+      </c>
       <c r="I57" s="34"/>
       <c r="J57" s="82" t="s">
         <v>383</v>
@@ -20986,23 +20997,21 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="170" t="s">
-        <v>239</v>
-      </c>
-      <c r="B58" s="180" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B58" s="62" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="182" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D58" s="167">
-        <v>5</v>
+        <v>1045</v>
+      </c>
+      <c r="D58" s="193">
+        <v>0</v>
       </c>
       <c r="E58" s="180" t="s">
         <v>92</v>
       </c>
-      <c r="F58" s="180" t="s">
-        <v>240</v>
-      </c>
+      <c r="F58" s="165"/>
       <c r="G58" s="180"/>
       <c r="H58" s="183"/>
       <c r="I58" s="34"/>
@@ -21022,10 +21031,10 @@
         <v>8</v>
       </c>
       <c r="C59" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D59" s="167">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="E59" s="180" t="s">
         <v>92</v>
@@ -21044,28 +21053,26 @@
         <v>778</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="24">
+    <row r="60" spans="1:12">
       <c r="A60" s="170" t="s">
-        <v>1016</v>
-      </c>
-      <c r="B60" s="62" t="s">
+        <v>239</v>
+      </c>
+      <c r="B60" s="180" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D60" s="167">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="E60" s="180" t="s">
-        <v>1021</v>
+        <v>92</v>
       </c>
       <c r="F60" s="180" t="s">
-        <v>1022</v>
-      </c>
-      <c r="G60" s="180" t="s">
-        <v>1023</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="G60" s="180"/>
       <c r="H60" s="183"/>
       <c r="I60" s="34"/>
       <c r="J60" s="82" t="s">
@@ -21084,7 +21091,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D61" s="167">
         <v>0</v>
@@ -21108,26 +21115,28 @@
         <v>778</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" ht="24">
       <c r="A62" s="170" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B62" s="62" t="s">
         <v>8</v>
       </c>
       <c r="C62" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D62" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E62" s="180" t="s">
-        <v>241</v>
+        <v>1021</v>
       </c>
       <c r="F62" s="180" t="s">
-        <v>999</v>
-      </c>
-      <c r="G62" s="180"/>
+        <v>1022</v>
+      </c>
+      <c r="G62" s="180" t="s">
+        <v>1023</v>
+      </c>
       <c r="H62" s="183"/>
       <c r="I62" s="34"/>
       <c r="J62" s="82" t="s">
@@ -21146,10 +21155,10 @@
         <v>8</v>
       </c>
       <c r="C63" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D63" s="167">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E63" s="180" t="s">
         <v>241</v>
@@ -21168,79 +21177,75 @@
         <v>778</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="163" customFormat="1">
-      <c r="A64" s="164" t="s">
+    <row r="64" spans="1:12">
+      <c r="A64" s="170" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B64" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="182" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D64" s="167">
+        <v>1</v>
+      </c>
+      <c r="E64" s="180" t="s">
+        <v>241</v>
+      </c>
+      <c r="F64" s="180" t="s">
+        <v>999</v>
+      </c>
+      <c r="G64" s="180"/>
+      <c r="H64" s="183"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="82" t="s">
+        <v>383</v>
+      </c>
+      <c r="K64" s="184"/>
+      <c r="L64" s="184" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="163" customFormat="1">
+      <c r="A65" s="164" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="169" t="s">
+      <c r="B65" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="174" t="s">
+      <c r="C65" s="174" t="s">
         <v>221</v>
       </c>
-      <c r="D64" s="174" t="s">
+      <c r="D65" s="174" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="197" t="s">
+      <c r="E65" s="197" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="197" t="s">
+      <c r="F65" s="197" t="s">
         <v>65</v>
       </c>
-      <c r="G64" s="169" t="s">
+      <c r="G65" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="H64" s="169" t="s">
+      <c r="H65" s="169" t="s">
         <v>71</v>
       </c>
-      <c r="I64" s="197" t="s">
+      <c r="I65" s="197" t="s">
         <v>14</v>
       </c>
-      <c r="J64" s="174" t="s">
+      <c r="J65" s="174" t="s">
         <v>368</v>
       </c>
-      <c r="K64" s="174" t="s">
+      <c r="K65" s="174" t="s">
         <v>409</v>
       </c>
-      <c r="L64" s="174" t="s">
+      <c r="L65" s="174" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A65" s="170" t="s">
-        <v>676</v>
-      </c>
-      <c r="B65" s="180" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>414</v>
-      </c>
-      <c r="E65" s="180" t="s">
-        <v>92</v>
-      </c>
-      <c r="F65" s="180" t="s">
-        <v>262</v>
-      </c>
-      <c r="G65" s="180" t="s">
-        <v>496</v>
-      </c>
-      <c r="H65" s="183" t="s">
-        <v>263</v>
-      </c>
-      <c r="I65" s="34"/>
-      <c r="J65" s="82" t="s">
-        <v>384</v>
-      </c>
-      <c r="K65" s="184"/>
-      <c r="L65" s="184" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="24">
+    <row r="66" spans="1:12" ht="25.5" customHeight="1">
       <c r="A66" s="170" t="s">
         <v>676</v>
       </c>
@@ -21248,10 +21253,10 @@
         <v>8</v>
       </c>
       <c r="C66" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E66" s="180" t="s">
         <v>92</v>
@@ -21276,26 +21281,28 @@
     </row>
     <row r="67" spans="1:12" ht="24">
       <c r="A67" s="170" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B67" s="180" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C67" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D67" s="180" t="s">
-        <v>249</v>
-      </c>
-      <c r="E67" s="196" t="s">
-        <v>250</v>
+        <v>1044</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="E67" s="180" t="s">
+        <v>92</v>
       </c>
       <c r="F67" s="180" t="s">
-        <v>251</v>
-      </c>
-      <c r="G67" s="180"/>
+        <v>262</v>
+      </c>
+      <c r="G67" s="180" t="s">
+        <v>496</v>
+      </c>
       <c r="H67" s="183" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="I67" s="34"/>
       <c r="J67" s="82" t="s">
@@ -21303,10 +21310,10 @@
       </c>
       <c r="K67" s="184"/>
       <c r="L67" s="184" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="24">
       <c r="A68" s="170" t="s">
         <v>677</v>
       </c>
@@ -21314,20 +21321,22 @@
         <v>5</v>
       </c>
       <c r="C68" s="182" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D68" s="91">
-        <v>120</v>
-      </c>
-      <c r="E68" s="167" t="s">
-        <v>241</v>
+        <v>1045</v>
+      </c>
+      <c r="D68" s="180" t="s">
+        <v>249</v>
+      </c>
+      <c r="E68" s="196" t="s">
+        <v>250</v>
       </c>
       <c r="F68" s="180" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G68" s="180"/>
-      <c r="H68" s="184"/>
-      <c r="I68" s="177"/>
+      <c r="H68" s="183" t="s">
+        <v>247</v>
+      </c>
+      <c r="I68" s="34"/>
       <c r="J68" s="82" t="s">
         <v>384</v>
       </c>
@@ -21338,35 +21347,35 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="170" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B69" s="180" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D69" s="167" t="s">
-        <v>254</v>
+        <v>1044</v>
+      </c>
+      <c r="D69" s="91">
+        <v>120</v>
       </c>
       <c r="E69" s="167" t="s">
         <v>241</v>
       </c>
       <c r="F69" s="180" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G69" s="180"/>
-      <c r="H69" s="180"/>
-      <c r="I69" s="34"/>
+      <c r="H69" s="184"/>
+      <c r="I69" s="177"/>
       <c r="J69" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K69" s="184"/>
       <c r="L69" s="184" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="30" customHeight="1">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" s="170" t="s">
         <v>678</v>
       </c>
@@ -21374,21 +21383,19 @@
         <v>5</v>
       </c>
       <c r="C70" s="182" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D70" s="180" t="s">
-        <v>418</v>
-      </c>
-      <c r="E70" s="196" t="s">
-        <v>250</v>
+        <v>1045</v>
+      </c>
+      <c r="D70" s="167" t="s">
+        <v>254</v>
+      </c>
+      <c r="E70" s="167" t="s">
+        <v>241</v>
       </c>
       <c r="F70" s="180" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G70" s="180"/>
-      <c r="H70" s="183" t="s">
-        <v>248</v>
-      </c>
+      <c r="H70" s="180"/>
       <c r="I70" s="34"/>
       <c r="J70" s="82" t="s">
         <v>384</v>
@@ -21398,38 +21405,36 @@
         <v>778</v>
       </c>
     </row>
-    <row r="71" spans="1:12" s="163" customFormat="1" ht="24">
+    <row r="71" spans="1:12" ht="30" customHeight="1">
       <c r="A71" s="170" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B71" s="180" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C71" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D71" s="167">
-        <v>1028.2</v>
-      </c>
-      <c r="E71" s="180" t="s">
-        <v>92</v>
+        <v>1044</v>
+      </c>
+      <c r="D71" s="180" t="s">
+        <v>418</v>
+      </c>
+      <c r="E71" s="196" t="s">
+        <v>250</v>
       </c>
       <c r="F71" s="180" t="s">
-        <v>240</v>
-      </c>
-      <c r="G71" s="180" t="s">
-        <v>496</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="G71" s="180"/>
       <c r="H71" s="183" t="s">
-        <v>13</v>
-      </c>
-      <c r="I71" s="32"/>
+        <v>248</v>
+      </c>
+      <c r="I71" s="34"/>
       <c r="J71" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K71" s="184"/>
       <c r="L71" s="184" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="72" spans="1:12" s="163" customFormat="1" ht="24">
@@ -21440,10 +21445,10 @@
         <v>8</v>
       </c>
       <c r="C72" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D72" s="167">
-        <v>1025.7</v>
+        <v>1028.2</v>
       </c>
       <c r="E72" s="180" t="s">
         <v>92</v>
@@ -21468,16 +21473,16 @@
     </row>
     <row r="73" spans="1:12" s="163" customFormat="1" ht="24">
       <c r="A73" s="170" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B73" s="180" t="s">
         <v>8</v>
       </c>
       <c r="C73" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D73" s="167">
-        <v>1028.2</v>
+        <v>1025.7</v>
       </c>
       <c r="E73" s="180" t="s">
         <v>92</v>
@@ -21508,10 +21513,10 @@
         <v>8</v>
       </c>
       <c r="C74" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D74" s="167">
-        <v>1025.7</v>
+        <v>1028.2</v>
       </c>
       <c r="E74" s="180" t="s">
         <v>92</v>
@@ -21534,36 +21539,38 @@
         <v>779</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" s="163" customFormat="1" ht="24">
       <c r="A75" s="170" t="s">
-        <v>689</v>
-      </c>
-      <c r="B75" s="62" t="s">
-        <v>362</v>
-      </c>
-      <c r="C75" s="167" t="s">
-        <v>1036</v>
-      </c>
-      <c r="D75" s="198">
-        <v>0.03</v>
-      </c>
-      <c r="E75" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F75" s="165" t="s">
-        <v>246</v>
-      </c>
-      <c r="G75" s="180"/>
-      <c r="H75" s="168" t="s">
-        <v>323</v>
-      </c>
-      <c r="I75" s="199"/>
+        <v>680</v>
+      </c>
+      <c r="B75" s="180" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="182" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D75" s="167">
+        <v>1025.7</v>
+      </c>
+      <c r="E75" s="180" t="s">
+        <v>92</v>
+      </c>
+      <c r="F75" s="180" t="s">
+        <v>240</v>
+      </c>
+      <c r="G75" s="180" t="s">
+        <v>496</v>
+      </c>
+      <c r="H75" s="183" t="s">
+        <v>13</v>
+      </c>
+      <c r="I75" s="32"/>
       <c r="J75" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K75" s="184"/>
       <c r="L75" s="184" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -21574,10 +21581,10 @@
         <v>362</v>
       </c>
       <c r="C76" s="167" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D76" s="168">
-        <v>3.6999999999999998E-2</v>
+        <v>1036</v>
+      </c>
+      <c r="D76" s="198">
+        <v>0.03</v>
       </c>
       <c r="E76" s="167" t="s">
         <v>241</v>
@@ -21587,7 +21594,7 @@
       </c>
       <c r="G76" s="180"/>
       <c r="H76" s="168" t="s">
-        <v>259</v>
+        <v>323</v>
       </c>
       <c r="I76" s="199"/>
       <c r="J76" s="82" t="s">
@@ -21598,38 +21605,36 @@
         <v>777</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="24">
+    <row r="77" spans="1:12">
       <c r="A77" s="170" t="s">
-        <v>690</v>
-      </c>
-      <c r="B77" s="180" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D77" s="180" t="s">
-        <v>416</v>
-      </c>
-      <c r="E77" s="180" t="s">
-        <v>257</v>
-      </c>
-      <c r="F77" s="180" t="s">
-        <v>258</v>
-      </c>
-      <c r="G77" s="180" t="s">
-        <v>496</v>
-      </c>
-      <c r="H77" s="183" t="s">
-        <v>267</v>
-      </c>
-      <c r="I77" s="34"/>
+        <v>689</v>
+      </c>
+      <c r="B77" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C77" s="167" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D77" s="168">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E77" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="F77" s="165" t="s">
+        <v>246</v>
+      </c>
+      <c r="G77" s="180"/>
+      <c r="H77" s="168" t="s">
+        <v>259</v>
+      </c>
+      <c r="I77" s="199"/>
       <c r="J77" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K77" s="184"/>
       <c r="L77" s="184" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="24">
@@ -21640,10 +21645,10 @@
         <v>8</v>
       </c>
       <c r="C78" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D78" s="180" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E78" s="180" t="s">
         <v>257</v>
@@ -21668,16 +21673,16 @@
     </row>
     <row r="79" spans="1:12" ht="24">
       <c r="A79" s="170" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B79" s="180" t="s">
         <v>8</v>
       </c>
       <c r="C79" s="182" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D79" s="180" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E79" s="180" t="s">
         <v>257</v>
@@ -21689,7 +21694,7 @@
         <v>496</v>
       </c>
       <c r="H79" s="183" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I79" s="34"/>
       <c r="J79" s="82" t="s">
@@ -21708,10 +21713,10 @@
         <v>8</v>
       </c>
       <c r="C80" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D80" s="180" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E80" s="180" t="s">
         <v>257</v>
@@ -21736,26 +21741,28 @@
     </row>
     <row r="81" spans="1:12" ht="24">
       <c r="A81" s="170" t="s">
-        <v>681</v>
-      </c>
-      <c r="B81" s="62" t="s">
-        <v>362</v>
-      </c>
-      <c r="C81" s="167" t="s">
-        <v>1036</v>
-      </c>
-      <c r="D81" s="168">
-        <v>1.2599999999999998E-2</v>
-      </c>
-      <c r="E81" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F81" s="165" t="s">
-        <v>246</v>
-      </c>
-      <c r="G81" s="180"/>
-      <c r="H81" s="180" t="s">
-        <v>264</v>
+        <v>691</v>
+      </c>
+      <c r="B81" s="180" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="182" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D81" s="180" t="s">
+        <v>417</v>
+      </c>
+      <c r="E81" s="180" t="s">
+        <v>257</v>
+      </c>
+      <c r="F81" s="180" t="s">
+        <v>258</v>
+      </c>
+      <c r="G81" s="180" t="s">
+        <v>496</v>
+      </c>
+      <c r="H81" s="183" t="s">
+        <v>266</v>
       </c>
       <c r="I81" s="34"/>
       <c r="J81" s="82" t="s">
@@ -21763,7 +21770,7 @@
       </c>
       <c r="K81" s="184"/>
       <c r="L81" s="184" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="24">
@@ -21774,10 +21781,10 @@
         <v>362</v>
       </c>
       <c r="C82" s="167" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D82" s="168">
-        <v>1.5800000000000002E-2</v>
+        <v>1.2599999999999998E-2</v>
       </c>
       <c r="E82" s="167" t="s">
         <v>241</v>
@@ -21787,7 +21794,7 @@
       </c>
       <c r="G82" s="180"/>
       <c r="H82" s="180" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I82" s="34"/>
       <c r="J82" s="82" t="s">
@@ -21800,34 +21807,34 @@
     </row>
     <row r="83" spans="1:12" ht="24">
       <c r="A83" s="170" t="s">
-        <v>682</v>
-      </c>
-      <c r="B83" s="180" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D83" s="180" t="s">
-        <v>416</v>
-      </c>
-      <c r="E83" s="180" t="s">
-        <v>257</v>
-      </c>
-      <c r="F83" s="180" t="s">
-        <v>258</v>
-      </c>
-      <c r="G83" s="180" t="s">
-        <v>496</v>
-      </c>
-      <c r="H83" s="183"/>
+        <v>681</v>
+      </c>
+      <c r="B83" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C83" s="167" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D83" s="168">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="E83" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="F83" s="165" t="s">
+        <v>246</v>
+      </c>
+      <c r="G83" s="180"/>
+      <c r="H83" s="180" t="s">
+        <v>265</v>
+      </c>
       <c r="I83" s="34"/>
       <c r="J83" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K83" s="184"/>
       <c r="L83" s="184" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="24">
@@ -21838,10 +21845,10 @@
         <v>8</v>
       </c>
       <c r="C84" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D84" s="180" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E84" s="180" t="s">
         <v>257</v>
@@ -21862,26 +21869,28 @@
         <v>779</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="36">
+    <row r="85" spans="1:12" ht="24">
       <c r="A85" s="170" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B85" s="180" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="167" t="s">
-        <v>167</v>
-      </c>
-      <c r="D85" s="44" t="s">
-        <v>324</v>
-      </c>
-      <c r="E85" s="196" t="s">
-        <v>325</v>
+        <v>8</v>
+      </c>
+      <c r="C85" s="182" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D85" s="180" t="s">
+        <v>417</v>
+      </c>
+      <c r="E85" s="180" t="s">
+        <v>257</v>
       </c>
       <c r="F85" s="180" t="s">
-        <v>326</v>
-      </c>
-      <c r="G85" s="180"/>
+        <v>258</v>
+      </c>
+      <c r="G85" s="180" t="s">
+        <v>496</v>
+      </c>
       <c r="H85" s="183"/>
       <c r="I85" s="34"/>
       <c r="J85" s="82" t="s">
@@ -21889,12 +21898,12 @@
       </c>
       <c r="K85" s="184"/>
       <c r="L85" s="184" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="39" customHeight="1">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="36">
       <c r="A86" s="170" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B86" s="180" t="s">
         <v>5</v>
@@ -21902,49 +21911,47 @@
       <c r="C86" s="167" t="s">
         <v>167</v>
       </c>
-      <c r="D86" s="180" t="s">
-        <v>327</v>
+      <c r="D86" s="44" t="s">
+        <v>324</v>
       </c>
       <c r="E86" s="196" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F86" s="180" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G86" s="180"/>
-      <c r="H86" s="1"/>
+      <c r="H86" s="183"/>
       <c r="I86" s="34"/>
       <c r="J86" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K86" s="184"/>
       <c r="L86" s="184" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="24">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="39" customHeight="1">
       <c r="A87" s="170" t="s">
-        <v>685</v>
-      </c>
-      <c r="B87" s="62" t="s">
-        <v>362</v>
+        <v>684</v>
+      </c>
+      <c r="B87" s="180" t="s">
+        <v>5</v>
       </c>
       <c r="C87" s="167" t="s">
-        <v>1036</v>
-      </c>
-      <c r="D87" s="168">
-        <v>1.54E-2</v>
-      </c>
-      <c r="E87" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F87" s="165" t="s">
-        <v>246</v>
+        <v>167</v>
+      </c>
+      <c r="D87" s="180" t="s">
+        <v>327</v>
+      </c>
+      <c r="E87" s="196" t="s">
+        <v>328</v>
+      </c>
+      <c r="F87" s="180" t="s">
+        <v>329</v>
       </c>
       <c r="G87" s="180"/>
-      <c r="H87" s="180" t="s">
-        <v>264</v>
-      </c>
+      <c r="H87" s="1"/>
       <c r="I87" s="34"/>
       <c r="J87" s="82" t="s">
         <v>384</v>
@@ -21962,10 +21969,10 @@
         <v>362</v>
       </c>
       <c r="C88" s="167" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D88" s="168">
-        <v>1.9300000000000001E-2</v>
+        <v>1.54E-2</v>
       </c>
       <c r="E88" s="167" t="s">
         <v>241</v>
@@ -21975,7 +21982,7 @@
       </c>
       <c r="G88" s="180"/>
       <c r="H88" s="180" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I88" s="34"/>
       <c r="J88" s="82" t="s">
@@ -21988,34 +21995,34 @@
     </row>
     <row r="89" spans="1:12" ht="24">
       <c r="A89" s="170" t="s">
-        <v>686</v>
-      </c>
-      <c r="B89" s="180" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D89" s="180" t="s">
-        <v>416</v>
-      </c>
-      <c r="E89" s="180" t="s">
-        <v>257</v>
-      </c>
-      <c r="F89" s="180" t="s">
-        <v>258</v>
-      </c>
-      <c r="G89" s="180" t="s">
-        <v>496</v>
-      </c>
-      <c r="H89" s="183"/>
+        <v>685</v>
+      </c>
+      <c r="B89" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C89" s="167" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D89" s="168">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="E89" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="F89" s="165" t="s">
+        <v>246</v>
+      </c>
+      <c r="G89" s="180"/>
+      <c r="H89" s="180" t="s">
+        <v>265</v>
+      </c>
       <c r="I89" s="34"/>
       <c r="J89" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K89" s="184"/>
       <c r="L89" s="184" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="24">
@@ -22026,10 +22033,10 @@
         <v>8</v>
       </c>
       <c r="C90" s="182" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D90" s="180" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E90" s="180" t="s">
         <v>257</v>
@@ -22050,26 +22057,28 @@
         <v>779</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="36">
+    <row r="91" spans="1:12" ht="24">
       <c r="A91" s="170" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B91" s="180" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="167" t="s">
-        <v>167</v>
-      </c>
-      <c r="D91" s="44" t="s">
-        <v>324</v>
-      </c>
-      <c r="E91" s="196" t="s">
-        <v>325</v>
+        <v>8</v>
+      </c>
+      <c r="C91" s="182" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D91" s="180" t="s">
+        <v>417</v>
+      </c>
+      <c r="E91" s="180" t="s">
+        <v>257</v>
       </c>
       <c r="F91" s="180" t="s">
-        <v>326</v>
-      </c>
-      <c r="G91" s="180"/>
+        <v>258</v>
+      </c>
+      <c r="G91" s="180" t="s">
+        <v>496</v>
+      </c>
       <c r="H91" s="183"/>
       <c r="I91" s="34"/>
       <c r="J91" s="82" t="s">
@@ -22077,12 +22086,12 @@
       </c>
       <c r="K91" s="184"/>
       <c r="L91" s="184" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="36.75" customHeight="1">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="36">
       <c r="A92" s="170" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B92" s="180" t="s">
         <v>5</v>
@@ -22090,14 +22099,14 @@
       <c r="C92" s="167" t="s">
         <v>167</v>
       </c>
-      <c r="D92" s="180" t="s">
-        <v>327</v>
+      <c r="D92" s="44" t="s">
+        <v>324</v>
       </c>
       <c r="E92" s="196" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F92" s="180" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G92" s="180"/>
       <c r="H92" s="183"/>
@@ -22107,63 +22116,61 @@
       </c>
       <c r="K92" s="184"/>
       <c r="L92" s="184" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="36.75" customHeight="1">
       <c r="A93" s="170" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B93" s="62" t="s">
-        <v>362</v>
+        <v>688</v>
+      </c>
+      <c r="B93" s="180" t="s">
+        <v>5</v>
       </c>
       <c r="C93" s="167" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D93" s="92">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="E93" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F93" s="165" t="s">
-        <v>246</v>
+        <v>167</v>
+      </c>
+      <c r="D93" s="180" t="s">
+        <v>327</v>
+      </c>
+      <c r="E93" s="196" t="s">
+        <v>328</v>
+      </c>
+      <c r="F93" s="180" t="s">
+        <v>329</v>
       </c>
       <c r="G93" s="180"/>
-      <c r="H93" s="180" t="s">
-        <v>256</v>
-      </c>
+      <c r="H93" s="183"/>
       <c r="I93" s="34"/>
       <c r="J93" s="82" t="s">
         <v>384</v>
       </c>
       <c r="K93" s="184"/>
       <c r="L93" s="184" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="170" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B94" s="180" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="182" t="s">
-        <v>167</v>
-      </c>
-      <c r="D94" s="180" t="s">
-        <v>330</v>
-      </c>
-      <c r="E94" s="196" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B94" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C94" s="167" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D94" s="92">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E94" s="167" t="s">
         <v>241</v>
       </c>
-      <c r="F94" s="180" t="s">
-        <v>331</v>
+      <c r="F94" s="165" t="s">
+        <v>246</v>
       </c>
       <c r="G94" s="180"/>
-      <c r="H94" s="183" t="s">
-        <v>332</v>
+      <c r="H94" s="180" t="s">
+        <v>256</v>
       </c>
       <c r="I94" s="34"/>
       <c r="J94" s="82" t="s">
@@ -22171,12 +22178,12 @@
       </c>
       <c r="K94" s="184"/>
       <c r="L94" s="184" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="170" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B95" s="180" t="s">
         <v>5</v>
@@ -22184,10 +22191,10 @@
       <c r="C95" s="182" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="167" t="s">
-        <v>333</v>
-      </c>
-      <c r="E95" s="167" t="s">
+      <c r="D95" s="180" t="s">
+        <v>330</v>
+      </c>
+      <c r="E95" s="196" t="s">
         <v>241</v>
       </c>
       <c r="F95" s="180" t="s">
@@ -22203,31 +22210,31 @@
       </c>
       <c r="K95" s="184"/>
       <c r="L95" s="184" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="170" t="s">
-        <v>1041</v>
-      </c>
-      <c r="B96" s="62" t="s">
-        <v>362</v>
-      </c>
-      <c r="C96" s="167" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D96" s="3">
-        <v>1.1000000000000001E-3</v>
+        <v>1040</v>
+      </c>
+      <c r="B96" s="180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="182" t="s">
+        <v>167</v>
+      </c>
+      <c r="D96" s="167" t="s">
+        <v>333</v>
       </c>
       <c r="E96" s="167" t="s">
         <v>241</v>
       </c>
-      <c r="F96" s="165" t="s">
-        <v>246</v>
+      <c r="F96" s="180" t="s">
+        <v>331</v>
       </c>
       <c r="G96" s="180"/>
-      <c r="H96" s="180" t="s">
-        <v>255</v>
+      <c r="H96" s="183" t="s">
+        <v>332</v>
       </c>
       <c r="I96" s="34"/>
       <c r="J96" s="82" t="s">
@@ -22235,31 +22242,31 @@
       </c>
       <c r="K96" s="184"/>
       <c r="L96" s="184" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="170" t="s">
-        <v>1042</v>
-      </c>
-      <c r="B97" s="180" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="182" t="s">
-        <v>167</v>
-      </c>
-      <c r="D97" s="180" t="s">
-        <v>330</v>
-      </c>
-      <c r="E97" s="196" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B97" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="C97" s="167" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D97" s="3">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E97" s="167" t="s">
         <v>241</v>
       </c>
-      <c r="F97" s="180" t="s">
-        <v>331</v>
+      <c r="F97" s="165" t="s">
+        <v>246</v>
       </c>
       <c r="G97" s="180"/>
-      <c r="H97" s="183" t="s">
-        <v>332</v>
+      <c r="H97" s="180" t="s">
+        <v>255</v>
       </c>
       <c r="I97" s="34"/>
       <c r="J97" s="82" t="s">
@@ -22267,12 +22274,12 @@
       </c>
       <c r="K97" s="184"/>
       <c r="L97" s="184" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" ht="14.25" customHeight="1">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="170" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B98" s="180" t="s">
         <v>5</v>
@@ -22280,10 +22287,10 @@
       <c r="C98" s="182" t="s">
         <v>167</v>
       </c>
-      <c r="D98" s="167" t="s">
-        <v>333</v>
-      </c>
-      <c r="E98" s="167" t="s">
+      <c r="D98" s="180" t="s">
+        <v>330</v>
+      </c>
+      <c r="E98" s="196" t="s">
         <v>241</v>
       </c>
       <c r="F98" s="180" t="s">
@@ -22299,131 +22306,133 @@
       </c>
       <c r="K98" s="184"/>
       <c r="L98" s="184" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A99" s="170" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B99" s="180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" s="182" t="s">
+        <v>167</v>
+      </c>
+      <c r="D99" s="167" t="s">
+        <v>333</v>
+      </c>
+      <c r="E99" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="F99" s="180" t="s">
+        <v>331</v>
+      </c>
+      <c r="G99" s="180"/>
+      <c r="H99" s="183" t="s">
+        <v>332</v>
+      </c>
+      <c r="I99" s="34"/>
+      <c r="J99" s="82" t="s">
+        <v>384</v>
+      </c>
+      <c r="K99" s="184"/>
+      <c r="L99" s="184" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="99" spans="1:12" s="163" customFormat="1">
-      <c r="A99" s="8" t="s">
+    <row r="100" spans="1:12" s="163" customFormat="1">
+      <c r="A100" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="B99" s="174" t="s">
+      <c r="B100" s="174" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="174" t="s">
+      <c r="C100" s="174" t="s">
         <v>221</v>
       </c>
-      <c r="D99" s="174" t="s">
+      <c r="D100" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="E99" s="174" t="s">
+      <c r="E100" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="F99" s="174" t="s">
+      <c r="F100" s="174" t="s">
         <v>63</v>
       </c>
-      <c r="G99" s="174" t="s">
+      <c r="G100" s="174" t="s">
         <v>19</v>
       </c>
-      <c r="H99" s="174" t="s">
+      <c r="H100" s="174" t="s">
         <v>71</v>
       </c>
-      <c r="I99" s="174" t="s">
+      <c r="I100" s="174" t="s">
         <v>14</v>
       </c>
-      <c r="J99" s="174" t="s">
+      <c r="J100" s="174" t="s">
         <v>368</v>
       </c>
-      <c r="K99" s="174" t="s">
+      <c r="K100" s="174" t="s">
         <v>409</v>
       </c>
-      <c r="L99" s="174" t="s">
+      <c r="L100" s="174" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="100" spans="1:12" s="163" customFormat="1" ht="24.5">
-      <c r="A100" s="80" t="s">
+    <row r="101" spans="1:12" s="163" customFormat="1" ht="24.75">
+      <c r="A101" s="80" t="s">
         <v>386</v>
       </c>
-      <c r="B100" s="184" t="s">
+      <c r="B101" s="184" t="s">
         <v>362</v>
-      </c>
-      <c r="C100" s="167" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D100" s="184">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E100" s="167" t="s">
-        <v>427</v>
-      </c>
-      <c r="F100" s="64"/>
-      <c r="G100" s="64"/>
-      <c r="H100" s="101" t="s">
-        <v>446</v>
-      </c>
-      <c r="I100" s="7"/>
-      <c r="J100" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="K100" s="21" t="s">
-        <v>456</v>
-      </c>
-      <c r="L100" s="184" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" s="163" customFormat="1">
-      <c r="A101" s="24" t="s">
-        <v>457</v>
-      </c>
-      <c r="B101" s="184" t="s">
-        <v>7</v>
       </c>
       <c r="C101" s="167" t="s">
         <v>1035</v>
       </c>
-      <c r="D101" s="102">
-        <v>0.06</v>
+      <c r="D101" s="184">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E101" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F101" s="165" t="s">
-        <v>246</v>
-      </c>
-      <c r="G101" s="180"/>
-      <c r="H101" s="168" t="s">
-        <v>447</v>
+        <v>427</v>
+      </c>
+      <c r="F101" s="64"/>
+      <c r="G101" s="64"/>
+      <c r="H101" s="101" t="s">
+        <v>446</v>
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="K101" s="10" t="s">
+      <c r="K101" s="21" t="s">
         <v>456</v>
       </c>
-      <c r="L101" s="184"/>
+      <c r="L101" s="184" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="102" spans="1:12" s="163" customFormat="1">
       <c r="A102" s="24" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B102" s="184" t="s">
-        <v>362</v>
+        <v>7</v>
       </c>
       <c r="C102" s="167" t="s">
-        <v>167</v>
-      </c>
-      <c r="D102" s="10" t="s">
-        <v>455</v>
+        <v>1035</v>
+      </c>
+      <c r="D102" s="102">
+        <v>0.06</v>
       </c>
       <c r="E102" s="167" t="s">
-        <v>448</v>
-      </c>
-      <c r="F102" s="64"/>
-      <c r="G102" s="64"/>
-      <c r="H102" s="10" t="s">
-        <v>449</v>
+        <v>241</v>
+      </c>
+      <c r="F102" s="165" t="s">
+        <v>246</v>
+      </c>
+      <c r="G102" s="180"/>
+      <c r="H102" s="168" t="s">
+        <v>447</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="10" t="s">
@@ -22436,24 +22445,24 @@
     </row>
     <row r="103" spans="1:12" s="163" customFormat="1">
       <c r="A103" s="24" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B103" s="184" t="s">
-        <v>22</v>
+        <v>362</v>
       </c>
       <c r="C103" s="167" t="s">
         <v>167</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="E103" s="167" t="s">
         <v>448</v>
       </c>
       <c r="F103" s="64"/>
       <c r="G103" s="64"/>
-      <c r="H103" s="184" t="s">
-        <v>451</v>
+      <c r="H103" s="10" t="s">
+        <v>449</v>
       </c>
       <c r="I103" s="7"/>
       <c r="J103" s="10" t="s">
@@ -22465,59 +22474,57 @@
       <c r="L103" s="184"/>
     </row>
     <row r="104" spans="1:12" s="163" customFormat="1">
-      <c r="A104" s="80" t="s">
-        <v>387</v>
-      </c>
-      <c r="B104" s="183" t="s">
-        <v>362</v>
+      <c r="A104" s="24" t="s">
+        <v>459</v>
+      </c>
+      <c r="B104" s="184" t="s">
+        <v>22</v>
       </c>
       <c r="C104" s="167" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D104" s="102">
-        <v>0.03</v>
+        <v>167</v>
+      </c>
+      <c r="D104" s="10" t="s">
+        <v>450</v>
       </c>
       <c r="E104" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F104" s="165" t="s">
-        <v>246</v>
-      </c>
-      <c r="G104" s="180"/>
-      <c r="H104" s="168"/>
-      <c r="I104" s="199"/>
+        <v>448</v>
+      </c>
+      <c r="F104" s="64"/>
+      <c r="G104" s="64"/>
+      <c r="H104" s="184" t="s">
+        <v>451</v>
+      </c>
+      <c r="I104" s="7"/>
       <c r="J104" s="10" t="s">
         <v>401</v>
       </c>
       <c r="K104" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="L104" s="184" t="s">
-        <v>777</v>
-      </c>
+      <c r="L104" s="184"/>
     </row>
     <row r="105" spans="1:12" s="163" customFormat="1">
       <c r="A105" s="80" t="s">
-        <v>388</v>
-      </c>
-      <c r="B105" s="184" t="s">
+        <v>387</v>
+      </c>
+      <c r="B105" s="183" t="s">
         <v>362</v>
       </c>
       <c r="C105" s="167" t="s">
         <v>1035</v>
       </c>
       <c r="D105" s="102">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E105" s="167" t="s">
-        <v>427</v>
-      </c>
-      <c r="F105" s="64"/>
-      <c r="G105" s="64"/>
-      <c r="H105" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="I105" s="7"/>
+        <v>241</v>
+      </c>
+      <c r="F105" s="165" t="s">
+        <v>246</v>
+      </c>
+      <c r="G105" s="180"/>
+      <c r="H105" s="168"/>
+      <c r="I105" s="199"/>
       <c r="J105" s="10" t="s">
         <v>401</v>
       </c>
@@ -22530,7 +22537,7 @@
     </row>
     <row r="106" spans="1:12" s="163" customFormat="1">
       <c r="A106" s="80" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B106" s="184" t="s">
         <v>362</v>
@@ -22538,8 +22545,8 @@
       <c r="C106" s="167" t="s">
         <v>1035</v>
       </c>
-      <c r="D106" s="10">
-        <v>4.2999999999999997E-2</v>
+      <c r="D106" s="102">
+        <v>0.05</v>
       </c>
       <c r="E106" s="167" t="s">
         <v>427</v>
@@ -22561,17 +22568,17 @@
       </c>
     </row>
     <row r="107" spans="1:12" s="163" customFormat="1">
-      <c r="A107" s="24" t="s">
-        <v>460</v>
+      <c r="A107" s="80" t="s">
+        <v>389</v>
       </c>
       <c r="B107" s="184" t="s">
-        <v>22</v>
+        <v>362</v>
       </c>
       <c r="C107" s="167" t="s">
-        <v>167</v>
-      </c>
-      <c r="D107" s="10" t="s">
-        <v>452</v>
+        <v>1035</v>
+      </c>
+      <c r="D107" s="10">
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E107" s="167" t="s">
         <v>427</v>
@@ -22588,62 +22595,62 @@
       <c r="K107" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="L107" s="184"/>
+      <c r="L107" s="184" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="108" spans="1:12" s="163" customFormat="1">
       <c r="A108" s="24" t="s">
-        <v>461</v>
-      </c>
-      <c r="B108" s="62" t="s">
+        <v>460</v>
+      </c>
+      <c r="B108" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="C108" s="182" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D108" s="10">
-        <v>0.44</v>
-      </c>
-      <c r="E108" s="180" t="s">
-        <v>321</v>
-      </c>
-      <c r="F108" s="165" t="s">
-        <v>322</v>
-      </c>
-      <c r="G108" s="180"/>
-      <c r="H108" s="25"/>
-      <c r="I108" s="34"/>
+      <c r="C108" s="167" t="s">
+        <v>167</v>
+      </c>
+      <c r="D108" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="E108" s="167" t="s">
+        <v>427</v>
+      </c>
+      <c r="F108" s="64"/>
+      <c r="G108" s="64"/>
+      <c r="H108" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="I108" s="7"/>
       <c r="J108" s="10" t="s">
         <v>401</v>
       </c>
       <c r="K108" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="L108" s="184" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" s="163" customFormat="1" ht="24.5">
-      <c r="A109" s="80" t="s">
-        <v>390</v>
-      </c>
-      <c r="B109" s="184" t="s">
-        <v>362</v>
-      </c>
-      <c r="C109" s="167" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D109" s="184">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E109" s="167" t="s">
-        <v>427</v>
-      </c>
-      <c r="F109" s="64"/>
-      <c r="G109" s="64"/>
-      <c r="H109" s="101" t="s">
-        <v>446</v>
-      </c>
-      <c r="I109" s="7"/>
+      <c r="L108" s="184"/>
+    </row>
+    <row r="109" spans="1:12" s="163" customFormat="1">
+      <c r="A109" s="24" t="s">
+        <v>461</v>
+      </c>
+      <c r="B109" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C109" s="182" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D109" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="E109" s="180" t="s">
+        <v>321</v>
+      </c>
+      <c r="F109" s="165" t="s">
+        <v>322</v>
+      </c>
+      <c r="G109" s="180"/>
+      <c r="H109" s="25"/>
+      <c r="I109" s="34"/>
       <c r="J109" s="10" t="s">
         <v>401</v>
       </c>
@@ -22654,9 +22661,9 @@
         <v>777</v>
       </c>
     </row>
-    <row r="110" spans="1:12" s="163" customFormat="1">
-      <c r="A110" s="24" t="s">
-        <v>462</v>
+    <row r="110" spans="1:12" s="163" customFormat="1" ht="24.75">
+      <c r="A110" s="80" t="s">
+        <v>390</v>
       </c>
       <c r="B110" s="184" t="s">
         <v>362</v>
@@ -22664,18 +22671,16 @@
       <c r="C110" s="167" t="s">
         <v>1035</v>
       </c>
-      <c r="D110" s="103">
-        <v>0.06</v>
+      <c r="D110" s="184">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E110" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F110" s="165" t="s">
-        <v>246</v>
-      </c>
-      <c r="G110" s="180"/>
-      <c r="H110" s="168" t="s">
-        <v>453</v>
+        <v>427</v>
+      </c>
+      <c r="F110" s="64"/>
+      <c r="G110" s="64"/>
+      <c r="H110" s="101" t="s">
+        <v>446</v>
       </c>
       <c r="I110" s="7"/>
       <c r="J110" s="10" t="s">
@@ -22684,11 +22689,13 @@
       <c r="K110" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="L110" s="184"/>
-    </row>
-    <row r="111" spans="1:12" s="163" customFormat="1" ht="24.5">
-      <c r="A111" s="80" t="s">
-        <v>391</v>
+      <c r="L110" s="184" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" s="163" customFormat="1">
+      <c r="A111" s="24" t="s">
+        <v>462</v>
       </c>
       <c r="B111" s="184" t="s">
         <v>362</v>
@@ -22696,16 +22703,18 @@
       <c r="C111" s="167" t="s">
         <v>1035</v>
       </c>
-      <c r="D111" s="184">
-        <v>0.08</v>
+      <c r="D111" s="103">
+        <v>0.06</v>
       </c>
       <c r="E111" s="167" t="s">
-        <v>427</v>
-      </c>
-      <c r="F111" s="64"/>
-      <c r="G111" s="64"/>
-      <c r="H111" s="101" t="s">
-        <v>454</v>
+        <v>241</v>
+      </c>
+      <c r="F111" s="165" t="s">
+        <v>246</v>
+      </c>
+      <c r="G111" s="180"/>
+      <c r="H111" s="168" t="s">
+        <v>453</v>
       </c>
       <c r="I111" s="7"/>
       <c r="J111" s="10" t="s">
@@ -22714,32 +22723,30 @@
       <c r="K111" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="L111" s="184" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" s="163" customFormat="1">
+      <c r="L111" s="184"/>
+    </row>
+    <row r="112" spans="1:12" s="163" customFormat="1" ht="24.75">
       <c r="A112" s="80" t="s">
-        <v>392</v>
-      </c>
-      <c r="B112" s="183" t="s">
+        <v>391</v>
+      </c>
+      <c r="B112" s="184" t="s">
         <v>362</v>
       </c>
       <c r="C112" s="167" t="s">
         <v>1035</v>
       </c>
-      <c r="D112" s="103">
-        <v>0.06</v>
+      <c r="D112" s="184">
+        <v>0.08</v>
       </c>
       <c r="E112" s="167" t="s">
-        <v>241</v>
-      </c>
-      <c r="F112" s="165" t="s">
-        <v>246</v>
-      </c>
-      <c r="G112" s="180"/>
-      <c r="H112" s="168"/>
-      <c r="I112" s="199"/>
+        <v>427</v>
+      </c>
+      <c r="F112" s="64"/>
+      <c r="G112" s="64"/>
+      <c r="H112" s="101" t="s">
+        <v>454</v>
+      </c>
+      <c r="I112" s="7"/>
       <c r="J112" s="10" t="s">
         <v>401</v>
       </c>
@@ -22751,33 +22758,65 @@
       </c>
     </row>
     <row r="113" spans="1:12" s="163" customFormat="1">
-      <c r="A113" s="24" t="s">
-        <v>408</v>
-      </c>
-      <c r="B113" s="64"/>
-      <c r="C113" s="167"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="64"/>
-      <c r="F113" s="64"/>
-      <c r="G113" s="64"/>
-      <c r="H113" s="64"/>
-      <c r="I113" s="7"/>
+      <c r="A113" s="80" t="s">
+        <v>392</v>
+      </c>
+      <c r="B113" s="183" t="s">
+        <v>362</v>
+      </c>
+      <c r="C113" s="167" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D113" s="103">
+        <v>0.06</v>
+      </c>
+      <c r="E113" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="F113" s="165" t="s">
+        <v>246</v>
+      </c>
+      <c r="G113" s="180"/>
+      <c r="H113" s="168"/>
+      <c r="I113" s="199"/>
       <c r="J113" s="10" t="s">
         <v>401</v>
       </c>
       <c r="K113" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="L113" s="184"/>
-    </row>
-    <row r="117" spans="1:12">
-      <c r="E117" s="28"/>
+      <c r="L113" s="184" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" s="163" customFormat="1">
+      <c r="A114" s="24" t="s">
+        <v>408</v>
+      </c>
+      <c r="B114" s="64"/>
+      <c r="C114" s="167"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="64"/>
+      <c r="F114" s="64"/>
+      <c r="G114" s="64"/>
+      <c r="H114" s="64"/>
+      <c r="I114" s="7"/>
+      <c r="J114" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="K114" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="L114" s="184"/>
     </row>
     <row r="118" spans="1:12">
       <c r="E118" s="28"/>
     </row>
     <row r="119" spans="1:12">
       <c r="E119" s="28"/>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="E120" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22794,20 +22833,20 @@
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" style="105" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1796875" style="105"/>
-    <col min="4" max="4" width="14.81640625" style="105" customWidth="1"/>
-    <col min="5" max="5" width="26.453125" style="106" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" style="105" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" style="105" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.453125" style="135" customWidth="1"/>
-    <col min="9" max="9" width="52.453125" style="105" customWidth="1"/>
-    <col min="10" max="10" width="24.81640625" style="105" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" style="105"/>
-    <col min="12" max="12" width="12.54296875" style="105" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="105"/>
+    <col min="1" max="1" width="31.140625" style="105" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="105"/>
+    <col min="4" max="4" width="14.85546875" style="105" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="106" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="105" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="105" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.42578125" style="135" customWidth="1"/>
+    <col min="9" max="9" width="52.42578125" style="105" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="105" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="105"/>
+    <col min="12" max="12" width="12.5703125" style="105" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="105"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="51" customFormat="1" ht="26.25" customHeight="1">
@@ -24192,7 +24231,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" ht="24.75">
       <c r="A42" s="109" t="s">
         <v>821</v>
       </c>
@@ -24372,7 +24411,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="36.5">
+    <row r="48" spans="1:12" ht="36.75">
       <c r="A48" s="109" t="s">
         <v>828</v>
       </c>
@@ -24394,7 +24433,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="60.5">
+    <row r="49" spans="1:12" ht="72.75">
       <c r="A49" s="109" t="s">
         <v>829</v>
       </c>
@@ -24484,7 +24523,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="24">
+    <row r="52" spans="1:12" ht="24.75">
       <c r="A52" s="109" t="s">
         <v>832</v>
       </c>
@@ -24516,7 +24555,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="36.5">
+    <row r="53" spans="1:12" ht="48.75">
       <c r="A53" s="109" t="s">
         <v>833</v>
       </c>
@@ -24744,7 +24783,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" ht="24.75">
       <c r="A61" s="109" t="s">
         <v>841</v>
       </c>
@@ -24918,7 +24957,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="24.5">
+    <row r="67" spans="1:12" ht="36.75">
       <c r="A67" s="109" t="s">
         <v>847</v>
       </c>
@@ -24944,7 +24983,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="60.5">
+    <row r="68" spans="1:12" ht="72.75">
       <c r="A68" s="109" t="s">
         <v>848</v>
       </c>
@@ -25034,7 +25073,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="24">
+    <row r="71" spans="1:12" ht="24.75">
       <c r="A71" s="109" t="s">
         <v>851</v>
       </c>
@@ -25066,7 +25105,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="36.5">
+    <row r="72" spans="1:12" ht="48.75">
       <c r="A72" s="109" t="s">
         <v>852</v>
       </c>

</xml_diff>

<commit_message>
Add Validation Target support (extends data request and mgr) Add to genData Read in hemodynamics targets into our optimization study engine
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\4x-Source\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D39507-6670-447D-99AB-88A8C05783E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DD9594-EA56-47E9-B66C-DB4E67E76EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24165" yWindow="5340" windowWidth="28005" windowHeight="23970" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" tabRatio="724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4021" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4095" uniqueCount="1091">
   <si>
     <t>Output</t>
   </si>
@@ -3429,6 +3429,12 @@
   </si>
   <si>
     <t>[5.2E06,5.4E06]</t>
+  </si>
+  <si>
+    <t>OptimizerTargets</t>
+  </si>
+  <si>
+    <t>HemodynamicsTargets</t>
   </si>
 </sst>
 </file>
@@ -4179,7 +4185,7 @@
     <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4736,6 +4742,10 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -5118,25 +5128,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1796875" style="51" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" style="52" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.28515625" style="51" customWidth="1"/>
+    <col min="8" max="8" width="49.26953125" style="51" customWidth="1"/>
     <col min="9" max="9" width="36" style="51" customWidth="1"/>
-    <col min="10" max="11" width="28.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="52" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="10" max="11" width="28.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="52" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1">
@@ -5761,7 +5771,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="56.25">
+    <row r="22" spans="1:12" ht="42">
       <c r="A22" s="109" t="s">
         <v>884</v>
       </c>
@@ -5791,7 +5801,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="22.5">
+    <row r="23" spans="1:12" ht="21">
       <c r="A23" s="15" t="s">
         <v>885</v>
       </c>
@@ -6867,7 +6877,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15">
+    <row r="57" spans="1:12" ht="14.5">
       <c r="A57" s="80" t="s">
         <v>429</v>
       </c>
@@ -6961,7 +6971,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="12.75">
+    <row r="60" spans="1:12" ht="12.5">
       <c r="A60" s="80" t="s">
         <v>432</v>
       </c>
@@ -8274,31 +8284,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="29" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" style="28" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" style="107" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="52" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="5"/>
+    <col min="6" max="6" width="21.7265625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="32.7265625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="36.26953125" style="107" customWidth="1"/>
+    <col min="9" max="9" width="29.54296875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="27.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" style="52" customWidth="1"/>
+    <col min="13" max="13" width="25.1796875" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="169" t="s">
         <v>0</v>
       </c>
@@ -8335,8 +8346,11 @@
       <c r="L1" s="174" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="51" customFormat="1" ht="24">
+      <c r="M1" s="174" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="51" customFormat="1" ht="24">
       <c r="A2" s="172" t="s">
         <v>138</v>
       </c>
@@ -8355,8 +8369,9 @@
       </c>
       <c r="K2" s="184"/>
       <c r="L2" s="184"/>
-    </row>
-    <row r="3" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M2" s="64"/>
+    </row>
+    <row r="3" spans="1:13" ht="36.75" customHeight="1">
       <c r="A3" s="170" t="s">
         <v>136</v>
       </c>
@@ -8387,8 +8402,9 @@
       <c r="L3" s="184" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="36.75" customHeight="1">
+      <c r="M3" s="200"/>
+    </row>
+    <row r="4" spans="1:13" ht="36.75" customHeight="1">
       <c r="A4" s="170" t="s">
         <v>900</v>
       </c>
@@ -8419,8 +8435,9 @@
       <c r="L4" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="45.75" customHeight="1">
+      <c r="M4" s="200"/>
+    </row>
+    <row r="5" spans="1:13" ht="45.75" customHeight="1">
       <c r="A5" s="170" t="s">
         <v>137</v>
       </c>
@@ -8449,8 +8466,9 @@
       <c r="L5" s="184" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="60">
+      <c r="M5" s="200"/>
+    </row>
+    <row r="6" spans="1:13" ht="48">
       <c r="A6" s="172" t="s">
         <v>169</v>
       </c>
@@ -8481,8 +8499,9 @@
       </c>
       <c r="K6" s="184"/>
       <c r="L6" s="184"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="200"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="170" t="s">
         <v>878</v>
       </c>
@@ -8509,8 +8528,9 @@
       <c r="L7" s="184" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="200"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="170" t="s">
         <v>879</v>
       </c>
@@ -8537,8 +8557,9 @@
       <c r="L8" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="45.75" customHeight="1">
+      <c r="M8" s="200"/>
+    </row>
+    <row r="9" spans="1:13" ht="45.75" customHeight="1">
       <c r="A9" s="170" t="s">
         <v>140</v>
       </c>
@@ -8569,8 +8590,9 @@
       <c r="L9" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="27.75" customHeight="1">
+      <c r="M9" s="200"/>
+    </row>
+    <row r="10" spans="1:13" ht="27.75" customHeight="1">
       <c r="A10" s="170" t="s">
         <v>141</v>
       </c>
@@ -8597,8 +8619,9 @@
       <c r="L10" s="184" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="74.25" customHeight="1">
+      <c r="M10" s="200"/>
+    </row>
+    <row r="11" spans="1:13" ht="74.25" customHeight="1">
       <c r="A11" s="170" t="s">
         <v>142</v>
       </c>
@@ -8627,8 +8650,9 @@
       <c r="L11" s="184" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="51" customFormat="1">
+      <c r="M11" s="200"/>
+    </row>
+    <row r="12" spans="1:13" s="51" customFormat="1">
       <c r="A12" s="172" t="s">
         <v>139</v>
       </c>
@@ -8647,8 +8671,9 @@
       </c>
       <c r="K12" s="184"/>
       <c r="L12" s="184"/>
-    </row>
-    <row r="13" spans="1:12" ht="65.25" customHeight="1">
+      <c r="M12" s="64"/>
+    </row>
+    <row r="13" spans="1:13" ht="65.25" customHeight="1">
       <c r="A13" s="170" t="s">
         <v>143</v>
       </c>
@@ -8677,8 +8702,9 @@
       <c r="L13" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="200"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="170" t="s">
         <v>880</v>
       </c>
@@ -8707,8 +8733,9 @@
       <c r="L14" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="40.5" customHeight="1">
+      <c r="M14" s="200"/>
+    </row>
+    <row r="15" spans="1:13" ht="40.5" customHeight="1">
       <c r="A15" s="170" t="s">
         <v>144</v>
       </c>
@@ -8739,8 +8766,9 @@
       <c r="L15" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="51" customFormat="1">
+      <c r="M15" s="200"/>
+    </row>
+    <row r="16" spans="1:13" s="51" customFormat="1">
       <c r="A16" s="172" t="s">
         <v>152</v>
       </c>
@@ -8759,8 +8787,9 @@
       </c>
       <c r="K16" s="184"/>
       <c r="L16" s="184"/>
-    </row>
-    <row r="17" spans="1:12" s="51" customFormat="1">
+      <c r="M16" s="64"/>
+    </row>
+    <row r="17" spans="1:13" s="51" customFormat="1">
       <c r="A17" s="172" t="s">
         <v>153</v>
       </c>
@@ -8779,8 +8808,9 @@
       </c>
       <c r="K17" s="184"/>
       <c r="L17" s="184"/>
-    </row>
-    <row r="18" spans="1:12" s="51" customFormat="1" ht="60">
+      <c r="M17" s="64"/>
+    </row>
+    <row r="18" spans="1:13" s="51" customFormat="1" ht="48">
       <c r="A18" s="170" t="s">
         <v>168</v>
       </c>
@@ -8811,8 +8841,9 @@
       <c r="L18" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="51" customFormat="1" ht="24">
+      <c r="M18" s="64"/>
+    </row>
+    <row r="19" spans="1:13" s="51" customFormat="1">
       <c r="A19" s="170" t="s">
         <v>201</v>
       </c>
@@ -8841,8 +8872,9 @@
       <c r="L19" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" s="51" customFormat="1" ht="24">
+      <c r="M19" s="64"/>
+    </row>
+    <row r="20" spans="1:13" s="51" customFormat="1" ht="24">
       <c r="A20" s="172" t="s">
         <v>154</v>
       </c>
@@ -8861,8 +8893,9 @@
       </c>
       <c r="K20" s="184"/>
       <c r="L20" s="184"/>
-    </row>
-    <row r="21" spans="1:12" ht="41.25" customHeight="1">
+      <c r="M20" s="64"/>
+    </row>
+    <row r="21" spans="1:13" ht="41.25" customHeight="1">
       <c r="A21" s="170" t="s">
         <v>145</v>
       </c>
@@ -8893,8 +8926,9 @@
       <c r="L21" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" s="51" customFormat="1" ht="24">
+      <c r="M21" s="200"/>
+    </row>
+    <row r="22" spans="1:13" s="51" customFormat="1" ht="24">
       <c r="A22" s="170" t="s">
         <v>179</v>
       </c>
@@ -8925,8 +8959,9 @@
       <c r="L22" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" s="51" customFormat="1">
+      <c r="M22" s="64"/>
+    </row>
+    <row r="23" spans="1:13" s="51" customFormat="1">
       <c r="A23" s="170" t="s">
         <v>178</v>
       </c>
@@ -8953,8 +8988,9 @@
       <c r="L23" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" s="51" customFormat="1">
+      <c r="M23" s="64"/>
+    </row>
+    <row r="24" spans="1:13" s="51" customFormat="1">
       <c r="A24" s="172" t="s">
         <v>755</v>
       </c>
@@ -8973,8 +9009,9 @@
       </c>
       <c r="K24" s="184"/>
       <c r="L24" s="184"/>
-    </row>
-    <row r="25" spans="1:12" s="51" customFormat="1">
+      <c r="M24" s="64"/>
+    </row>
+    <row r="25" spans="1:13" s="51" customFormat="1">
       <c r="A25" s="172" t="s">
         <v>756</v>
       </c>
@@ -8993,8 +9030,9 @@
       </c>
       <c r="K25" s="184"/>
       <c r="L25" s="184"/>
-    </row>
-    <row r="26" spans="1:12" s="51" customFormat="1">
+      <c r="M25" s="64"/>
+    </row>
+    <row r="26" spans="1:13" s="51" customFormat="1">
       <c r="A26" s="170" t="s">
         <v>177</v>
       </c>
@@ -9025,8 +9063,9 @@
       <c r="L26" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" s="51" customFormat="1" ht="24">
+      <c r="M26" s="64"/>
+    </row>
+    <row r="27" spans="1:13" s="51" customFormat="1">
       <c r="A27" s="170" t="s">
         <v>901</v>
       </c>
@@ -9055,8 +9094,9 @@
       <c r="L27" s="184" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" s="51" customFormat="1" ht="36">
+      <c r="M27" s="64"/>
+    </row>
+    <row r="28" spans="1:13" s="51" customFormat="1" ht="36">
       <c r="A28" s="170" t="s">
         <v>902</v>
       </c>
@@ -9087,8 +9127,9 @@
       <c r="L28" s="184" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" s="51" customFormat="1" ht="48">
+      <c r="M28" s="64"/>
+    </row>
+    <row r="29" spans="1:13" s="51" customFormat="1" ht="36">
       <c r="A29" s="170" t="s">
         <v>176</v>
       </c>
@@ -9121,8 +9162,9 @@
       <c r="L29" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" s="51" customFormat="1" ht="24" customHeight="1">
+      <c r="M29" s="64"/>
+    </row>
+    <row r="30" spans="1:13" s="51" customFormat="1" ht="24" customHeight="1">
       <c r="A30" s="170" t="s">
         <v>175</v>
       </c>
@@ -9153,8 +9195,9 @@
       <c r="L30" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="44.25" customHeight="1">
+      <c r="M30" s="64"/>
+    </row>
+    <row r="31" spans="1:13" ht="44.25" customHeight="1">
       <c r="A31" s="170" t="s">
         <v>146</v>
       </c>
@@ -9185,8 +9228,9 @@
       <c r="L31" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" s="51" customFormat="1">
+      <c r="M31" s="200"/>
+    </row>
+    <row r="32" spans="1:13" s="51" customFormat="1">
       <c r="A32" s="164" t="s">
         <v>66</v>
       </c>
@@ -9223,8 +9267,11 @@
       <c r="L32" s="174" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="24">
+      <c r="M32" s="174" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="24">
       <c r="A33" s="170" t="s">
         <v>611</v>
       </c>
@@ -9253,8 +9300,11 @@
       <c r="L33" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="36">
+      <c r="M33" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="36">
       <c r="A34" s="170" t="s">
         <v>612</v>
       </c>
@@ -9283,8 +9333,11 @@
       <c r="L34" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="170" t="s">
         <v>613</v>
       </c>
@@ -9311,8 +9364,11 @@
       <c r="L35" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="170" t="s">
         <v>614</v>
       </c>
@@ -9339,8 +9395,11 @@
       <c r="L36" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="170" t="s">
         <v>953</v>
       </c>
@@ -9369,8 +9428,9 @@
       <c r="L37" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" s="200"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="170" t="s">
         <v>615</v>
       </c>
@@ -9399,8 +9459,11 @@
       <c r="L38" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="170" t="s">
         <v>616</v>
       </c>
@@ -9427,8 +9490,11 @@
       <c r="L39" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="170" t="s">
         <v>617</v>
       </c>
@@ -9455,8 +9521,11 @@
       <c r="L40" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="170" t="s">
         <v>618</v>
       </c>
@@ -9483,8 +9552,11 @@
       <c r="L41" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="170" t="s">
         <v>669</v>
       </c>
@@ -9511,8 +9583,11 @@
       <c r="L42" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="170" t="s">
         <v>670</v>
       </c>
@@ -9539,8 +9614,11 @@
       <c r="L43" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="24">
+      <c r="M43" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="24">
       <c r="A44" s="170" t="s">
         <v>619</v>
       </c>
@@ -9569,8 +9647,11 @@
       <c r="L44" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="170" t="s">
         <v>620</v>
       </c>
@@ -9597,8 +9678,11 @@
       <c r="L45" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="36">
+      <c r="M45" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="24">
       <c r="A46" s="170" t="s">
         <v>621</v>
       </c>
@@ -9627,8 +9711,11 @@
       <c r="L46" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="170" t="s">
         <v>965</v>
       </c>
@@ -9655,8 +9742,11 @@
       </c>
       <c r="K47" s="184"/>
       <c r="L47" s="184"/>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="170" t="s">
         <v>672</v>
       </c>
@@ -9683,8 +9773,11 @@
       <c r="L48" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="170" t="s">
         <v>672</v>
       </c>
@@ -9711,8 +9804,11 @@
       <c r="L49" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="170" t="s">
         <v>671</v>
       </c>
@@ -9739,8 +9835,11 @@
       <c r="L50" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="48">
+      <c r="M50" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="48">
       <c r="A51" s="170" t="s">
         <v>671</v>
       </c>
@@ -9771,8 +9870,11 @@
       <c r="L51" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="170" t="s">
         <v>673</v>
       </c>
@@ -9799,8 +9901,11 @@
       <c r="L52" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="24">
+      <c r="M52" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="24">
       <c r="A53" s="170" t="s">
         <v>622</v>
       </c>
@@ -9829,8 +9934,11 @@
       <c r="L53" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="24">
+      <c r="M53" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="24">
       <c r="A54" s="170" t="s">
         <v>623</v>
       </c>
@@ -9859,8 +9967,11 @@
       <c r="L54" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="36">
+      <c r="M54" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="24">
       <c r="A55" s="170" t="s">
         <v>624</v>
       </c>
@@ -9889,8 +10000,11 @@
       <c r="L55" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="170" t="s">
         <v>968</v>
       </c>
@@ -9917,8 +10031,11 @@
       </c>
       <c r="K56" s="184"/>
       <c r="L56" s="184"/>
-    </row>
-    <row r="57" spans="1:12" ht="24">
+      <c r="M56" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="170" t="s">
         <v>645</v>
       </c>
@@ -9947,8 +10064,11 @@
       <c r="L57" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="170" t="s">
         <v>646</v>
       </c>
@@ -9975,8 +10095,11 @@
       <c r="L58" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="24">
+      <c r="M58" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="170" t="s">
         <v>647</v>
       </c>
@@ -10005,8 +10128,11 @@
       <c r="L59" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="170" t="s">
         <v>648</v>
       </c>
@@ -10033,8 +10159,11 @@
       <c r="L60" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" ht="24">
+      <c r="M60" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="170" t="s">
         <v>649</v>
       </c>
@@ -10063,8 +10192,11 @@
       <c r="L61" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="170" t="s">
         <v>650</v>
       </c>
@@ -10091,8 +10223,11 @@
       <c r="L62" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="24">
+      <c r="M62" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="170" t="s">
         <v>625</v>
       </c>
@@ -10121,8 +10256,11 @@
       <c r="L63" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="M63" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="170" t="s">
         <v>626</v>
       </c>
@@ -10153,8 +10291,11 @@
       <c r="L64" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="M64" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" s="170" t="s">
         <v>627</v>
       </c>
@@ -10183,8 +10324,11 @@
       <c r="L65" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="M65" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" s="170" t="s">
         <v>628</v>
       </c>
@@ -10211,8 +10355,11 @@
       <c r="L66" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="M66" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" s="170" t="s">
         <v>629</v>
       </c>
@@ -10241,8 +10388,11 @@
       <c r="L67" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="M67" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="170" t="s">
         <v>630</v>
       </c>
@@ -10269,8 +10419,11 @@
       <c r="L68" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" ht="24">
+      <c r="M68" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="170" t="s">
         <v>651</v>
       </c>
@@ -10299,8 +10452,11 @@
       <c r="L69" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="170" t="s">
         <v>652</v>
       </c>
@@ -10327,8 +10483,11 @@
       <c r="L70" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" s="170" t="s">
         <v>653</v>
       </c>
@@ -10357,8 +10516,11 @@
       <c r="L71" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="M71" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="170" t="s">
         <v>653</v>
       </c>
@@ -10387,8 +10549,11 @@
       <c r="L72" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" ht="24">
+      <c r="M72" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="A73" s="170" t="s">
         <v>654</v>
       </c>
@@ -10417,8 +10582,11 @@
       <c r="L73" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="M73" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
       <c r="A74" s="170" t="s">
         <v>655</v>
       </c>
@@ -10445,8 +10613,11 @@
       <c r="L74" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="M74" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
       <c r="A75" s="170" t="s">
         <v>656</v>
       </c>
@@ -10477,8 +10648,11 @@
       <c r="L75" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" ht="24">
+      <c r="M75" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
       <c r="A76" s="170" t="s">
         <v>657</v>
       </c>
@@ -10507,8 +10681,11 @@
       <c r="L76" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="M76" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
       <c r="A77" s="170" t="s">
         <v>658</v>
       </c>
@@ -10535,8 +10712,11 @@
       <c r="L77" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" ht="36">
+      <c r="M77" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="36">
       <c r="A78" s="170" t="s">
         <v>659</v>
       </c>
@@ -10567,8 +10747,11 @@
       <c r="L78" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" ht="36">
+      <c r="M78" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="24">
       <c r="A79" s="170" t="s">
         <v>631</v>
       </c>
@@ -10597,8 +10780,11 @@
       <c r="L79" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="M79" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" s="170" t="s">
         <v>972</v>
       </c>
@@ -10625,8 +10811,11 @@
       </c>
       <c r="K80" s="184"/>
       <c r="L80" s="184"/>
-    </row>
-    <row r="81" spans="1:12" ht="60">
+      <c r="M80" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="48">
       <c r="A81" s="170" t="s">
         <v>660</v>
       </c>
@@ -10655,8 +10844,11 @@
       <c r="L81" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" ht="24">
+      <c r="M81" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="24">
       <c r="A82" s="170" t="s">
         <v>660</v>
       </c>
@@ -10683,8 +10875,11 @@
       <c r="L82" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" ht="36">
+      <c r="M82" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="36">
       <c r="A83" s="170" t="s">
         <v>661</v>
       </c>
@@ -10713,8 +10908,11 @@
       <c r="L83" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="M83" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" s="170" t="s">
         <v>661</v>
       </c>
@@ -10741,8 +10939,11 @@
       <c r="L84" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="M84" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" s="170" t="s">
         <v>662</v>
       </c>
@@ -10769,8 +10970,11 @@
       <c r="L85" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" ht="24">
+      <c r="M85" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="24">
       <c r="A86" s="170" t="s">
         <v>632</v>
       </c>
@@ -10799,8 +11003,11 @@
       <c r="L86" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" ht="24">
+      <c r="M86" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="24">
       <c r="A87" s="170" t="s">
         <v>633</v>
       </c>
@@ -10829,8 +11036,11 @@
       <c r="L87" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" ht="36">
+      <c r="M87" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="24">
       <c r="A88" s="170" t="s">
         <v>634</v>
       </c>
@@ -10859,8 +11069,11 @@
       <c r="L88" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="M88" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" s="170" t="s">
         <v>969</v>
       </c>
@@ -10887,8 +11100,11 @@
       </c>
       <c r="K89" s="184"/>
       <c r="L89" s="184"/>
-    </row>
-    <row r="90" spans="1:12" ht="24">
+      <c r="M89" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" s="170" t="s">
         <v>663</v>
       </c>
@@ -10917,8 +11133,11 @@
       <c r="L90" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="M90" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" s="170" t="s">
         <v>664</v>
       </c>
@@ -10945,8 +11164,11 @@
       <c r="L91" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" ht="24">
+      <c r="M91" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" s="170" t="s">
         <v>665</v>
       </c>
@@ -10975,8 +11197,11 @@
       <c r="L92" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="93" spans="1:12">
+      <c r="M92" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" s="170" t="s">
         <v>666</v>
       </c>
@@ -11003,8 +11228,11 @@
       <c r="L93" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" ht="24">
+      <c r="M93" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" s="170" t="s">
         <v>667</v>
       </c>
@@ -11033,8 +11261,11 @@
       <c r="L94" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="M94" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" s="170" t="s">
         <v>668</v>
       </c>
@@ -11061,8 +11292,11 @@
       <c r="L95" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" ht="24">
+      <c r="M95" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" s="170" t="s">
         <v>635</v>
       </c>
@@ -11091,8 +11325,11 @@
       <c r="L96" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="97" spans="1:12">
+      <c r="M96" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
       <c r="A97" s="170" t="s">
         <v>636</v>
       </c>
@@ -11119,8 +11356,11 @@
       <c r="L97" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="98" spans="1:12">
+      <c r="M97" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" s="170" t="s">
         <v>637</v>
       </c>
@@ -11147,8 +11387,11 @@
       <c r="L98" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="99" spans="1:12">
+      <c r="M98" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" s="170" t="s">
         <v>638</v>
       </c>
@@ -11175,8 +11418,11 @@
       <c r="L99" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="100" spans="1:12">
+      <c r="M99" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" s="170" t="s">
         <v>639</v>
       </c>
@@ -11203,8 +11449,11 @@
       <c r="L100" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="101" spans="1:12">
+      <c r="M100" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
       <c r="A101" s="170" t="s">
         <v>640</v>
       </c>
@@ -11233,8 +11482,11 @@
       <c r="L101" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="102" spans="1:12">
+      <c r="M101" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
       <c r="A102" s="170" t="s">
         <v>641</v>
       </c>
@@ -11261,8 +11513,11 @@
       <c r="L102" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="103" spans="1:12">
+      <c r="M102" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
       <c r="A103" s="170" t="s">
         <v>642</v>
       </c>
@@ -11289,8 +11544,11 @@
       <c r="L103" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" ht="24">
+      <c r="M103" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
       <c r="A104" s="170" t="s">
         <v>643</v>
       </c>
@@ -11319,8 +11577,11 @@
       <c r="L104" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="105" spans="1:12">
+      <c r="M104" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
       <c r="A105" s="170" t="s">
         <v>644</v>
       </c>
@@ -11347,17 +11608,20 @@
       <c r="L105" s="184" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="106" spans="1:12">
+      <c r="M105" s="201" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
       <c r="F106" s="28"/>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:13">
       <c r="F107" s="28"/>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:13">
       <c r="E108" s="28"/>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:13">
       <c r="E109" s="28"/>
     </row>
   </sheetData>
@@ -11377,20 +11641,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="21"/>
-    <col min="5" max="6" width="17.28515625" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" style="51" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="51" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="51" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="1" max="1" width="20.7265625" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="21"/>
+    <col min="5" max="6" width="17.26953125" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="29.7265625" style="51" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="51" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" style="51" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -11431,7 +11695,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="72">
+    <row r="2" spans="1:12" ht="60">
       <c r="A2" s="39" t="s">
         <v>171</v>
       </c>
@@ -11475,19 +11739,19 @@
       <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="7" width="23.5703125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="9"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" customWidth="1"/>
+    <col min="6" max="7" width="23.54296875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.1796875" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="9"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -11807,21 +12071,21 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="51" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="51" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="51" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" style="51" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="51" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" style="51" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" style="51" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" style="51" customWidth="1"/>
     <col min="6" max="6" width="12" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.7109375" style="84" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="7" max="7" width="5.1796875" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7265625" style="84" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -11905,18 +12169,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.26953125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="21"/>
-    <col min="5" max="6" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.7109375" style="21" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="21"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="21"/>
+    <col min="4" max="4" width="9.1796875" style="21"/>
+    <col min="5" max="6" width="17.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.7265625" style="21" customWidth="1"/>
+    <col min="9" max="10" width="9.1796875" style="21"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24">
@@ -12067,21 +12331,21 @@
       <selection pane="topRight" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="85" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="85" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" style="85" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" style="85" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" style="51" customWidth="1"/>
     <col min="7" max="7" width="40" style="51" customWidth="1"/>
-    <col min="8" max="8" width="41.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="51" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="51"/>
+    <col min="8" max="8" width="41.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.1796875" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="51" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12244,7 +12508,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="24">
+    <row r="6" spans="1:12">
       <c r="A6" s="65" t="s">
         <v>340</v>
       </c>
@@ -12563,7 +12827,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="24">
+    <row r="17" spans="1:12">
       <c r="A17" s="70" t="s">
         <v>436</v>
       </c>
@@ -12781,7 +13045,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="24">
+    <row r="24" spans="1:12">
       <c r="A24" s="17" t="s">
         <v>334</v>
       </c>
@@ -13021,7 +13285,7 @@
       <c r="K31" s="56"/>
       <c r="L31" s="56"/>
     </row>
-    <row r="32" spans="1:12" ht="24">
+    <row r="32" spans="1:12">
       <c r="A32" s="17" t="s">
         <v>337</v>
       </c>
@@ -13199,7 +13463,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="24">
+    <row r="38" spans="1:12">
       <c r="A38" s="70" t="s">
         <v>438</v>
       </c>
@@ -13417,7 +13681,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="24">
+    <row r="45" spans="1:12">
       <c r="A45" s="17" t="s">
         <v>333</v>
       </c>
@@ -13655,7 +13919,7 @@
       <c r="K52" s="56"/>
       <c r="L52" s="151"/>
     </row>
-    <row r="53" spans="1:12" ht="24">
+    <row r="53" spans="1:12">
       <c r="A53" s="17" t="s">
         <v>336</v>
       </c>
@@ -13811,7 +14075,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="48">
+    <row r="58" spans="1:12" ht="36">
       <c r="A58" s="65" t="s">
         <v>712</v>
       </c>
@@ -13841,7 +14105,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="48">
+    <row r="59" spans="1:12" ht="36">
       <c r="A59" s="65" t="s">
         <v>713</v>
       </c>
@@ -13871,7 +14135,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="48">
+    <row r="60" spans="1:12" ht="36">
       <c r="A60" s="65" t="s">
         <v>714</v>
       </c>
@@ -13901,7 +14165,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="48">
+    <row r="61" spans="1:12" ht="36">
       <c r="A61" s="65" t="s">
         <v>715</v>
       </c>
@@ -13931,7 +14195,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="48">
+    <row r="62" spans="1:12" ht="36">
       <c r="A62" s="65" t="s">
         <v>716</v>
       </c>
@@ -13961,7 +14225,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="48">
+    <row r="63" spans="1:12" ht="36">
       <c r="A63" s="65" t="s">
         <v>717</v>
       </c>
@@ -13991,7 +14255,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="48">
+    <row r="64" spans="1:12" ht="36">
       <c r="A64" s="65" t="s">
         <v>701</v>
       </c>
@@ -14021,7 +14285,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="48">
+    <row r="65" spans="1:12" ht="36">
       <c r="A65" s="65" t="s">
         <v>702</v>
       </c>
@@ -14083,7 +14347,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="36">
+    <row r="67" spans="1:12" ht="24">
       <c r="A67" s="120" t="s">
         <v>718</v>
       </c>
@@ -14115,7 +14379,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="48">
+    <row r="68" spans="1:12" ht="36">
       <c r="A68" s="120" t="s">
         <v>719</v>
       </c>
@@ -14145,7 +14409,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="48">
+    <row r="69" spans="1:12" ht="36">
       <c r="A69" s="120" t="s">
         <v>720</v>
       </c>
@@ -14175,7 +14439,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="48">
+    <row r="70" spans="1:12" ht="36">
       <c r="A70" s="120" t="s">
         <v>721</v>
       </c>
@@ -14205,7 +14469,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="48">
+    <row r="71" spans="1:12" ht="36">
       <c r="A71" s="120" t="s">
         <v>722</v>
       </c>
@@ -14235,7 +14499,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="48">
+    <row r="72" spans="1:12" ht="36">
       <c r="A72" s="120" t="s">
         <v>723</v>
       </c>
@@ -14265,7 +14529,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="48">
+    <row r="73" spans="1:12" ht="36">
       <c r="A73" s="120" t="s">
         <v>724</v>
       </c>
@@ -14295,7 +14559,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="48">
+    <row r="74" spans="1:12" ht="36">
       <c r="A74" s="120" t="s">
         <v>704</v>
       </c>
@@ -14325,7 +14589,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="48">
+    <row r="75" spans="1:12" ht="36">
       <c r="A75" s="120" t="s">
         <v>705</v>
       </c>
@@ -15411,7 +15675,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="36">
+    <row r="109" spans="1:12" ht="24">
       <c r="A109" s="65" t="s">
         <v>914</v>
       </c>
@@ -15505,7 +15769,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="36">
+    <row r="112" spans="1:12" ht="24">
       <c r="A112" s="65" t="s">
         <v>917</v>
       </c>
@@ -16539,7 +16803,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="145" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="145" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A145" s="8" t="s">
         <v>461</v>
       </c>
@@ -16577,7 +16841,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="146" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="146" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A146" s="80" t="s">
         <v>463</v>
       </c>
@@ -16605,7 +16869,7 @@
       </c>
       <c r="L146" s="56"/>
     </row>
-    <row r="147" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="147" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A147" s="80" t="s">
         <v>464</v>
       </c>
@@ -16625,7 +16889,7 @@
       </c>
       <c r="L147" s="56"/>
     </row>
-    <row r="148" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="148" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A148" s="80" t="s">
         <v>371</v>
       </c>
@@ -16653,7 +16917,7 @@
       </c>
       <c r="L148" s="56"/>
     </row>
-    <row r="149" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="149" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A149" s="80" t="s">
         <v>465</v>
       </c>
@@ -16681,7 +16945,7 @@
       </c>
       <c r="L149" s="56"/>
     </row>
-    <row r="150" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="150" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A150" s="80" t="s">
         <v>469</v>
       </c>
@@ -16701,7 +16965,7 @@
       </c>
       <c r="L150" s="56"/>
     </row>
-    <row r="151" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="151" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A151" s="80" t="s">
         <v>466</v>
       </c>
@@ -16735,7 +16999,7 @@
       </c>
       <c r="L151" s="56"/>
     </row>
-    <row r="152" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="152" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A152" s="80" t="s">
         <v>467</v>
       </c>
@@ -16763,7 +17027,7 @@
       </c>
       <c r="L152" s="56"/>
     </row>
-    <row r="153" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="153" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A153" s="80" t="s">
         <v>470</v>
       </c>
@@ -16783,7 +17047,7 @@
       </c>
       <c r="L153" s="56"/>
     </row>
-    <row r="154" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="154" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A154" s="80" t="s">
         <v>468</v>
       </c>
@@ -16811,7 +17075,7 @@
       </c>
       <c r="L154" s="56"/>
     </row>
-    <row r="155" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="155" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A155" s="80" t="s">
         <v>471</v>
       </c>
@@ -16831,7 +17095,7 @@
       </c>
       <c r="L155" s="56"/>
     </row>
-    <row r="156" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="156" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A156" s="80" t="s">
         <v>472</v>
       </c>
@@ -16851,7 +17115,7 @@
       </c>
       <c r="L156" s="56"/>
     </row>
-    <row r="157" spans="1:12" s="57" customFormat="1" ht="15">
+    <row r="157" spans="1:12" s="57" customFormat="1" ht="14.5">
       <c r="A157" s="80" t="s">
         <v>473</v>
       </c>
@@ -19407,21 +19671,21 @@
       <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="28" customWidth="1"/>
+    <col min="1" max="1" width="44.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="28" customWidth="1"/>
     <col min="3" max="3" width="30" style="28" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="28" customWidth="1"/>
     <col min="5" max="5" width="20" style="176" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="176" customWidth="1"/>
+    <col min="6" max="6" width="27.26953125" style="176" customWidth="1"/>
     <col min="7" max="7" width="24" style="176" customWidth="1"/>
-    <col min="8" max="8" width="37.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="81" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" style="185" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="185" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="24.7265625" style="81" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" style="185" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -19492,7 +19756,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="48">
+    <row r="3" spans="1:12" ht="36">
       <c r="A3" s="170" t="s">
         <v>908</v>
       </c>
@@ -20216,7 +20480,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="60">
+    <row r="29" spans="1:12" ht="48">
       <c r="A29" s="170" t="s">
         <v>1026</v>
       </c>
@@ -20438,7 +20702,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="120">
+    <row r="37" spans="1:12" ht="96">
       <c r="A37" s="170" t="s">
         <v>983</v>
       </c>
@@ -21066,7 +21330,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="24">
+    <row r="59" spans="1:12">
       <c r="A59" s="170" t="s">
         <v>1017</v>
       </c>
@@ -21098,7 +21362,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="24">
+    <row r="60" spans="1:12">
       <c r="A60" s="170" t="s">
         <v>1017</v>
       </c>
@@ -22544,7 +22808,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="105" spans="1:12" s="163" customFormat="1" ht="24.75">
+    <row r="105" spans="1:12" s="163" customFormat="1" ht="24.5">
       <c r="A105" s="80" t="s">
         <v>385</v>
       </c>
@@ -22826,7 +23090,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="114" spans="1:12" s="163" customFormat="1" ht="24.75">
+    <row r="114" spans="1:12" s="163" customFormat="1" ht="24.5">
       <c r="A114" s="80" t="s">
         <v>389</v>
       </c>
@@ -22890,7 +23154,7 @@
       </c>
       <c r="L115" s="184"/>
     </row>
-    <row r="116" spans="1:12" s="163" customFormat="1" ht="24.75">
+    <row r="116" spans="1:12" s="163" customFormat="1" ht="24.5">
       <c r="A116" s="80" t="s">
         <v>390</v>
       </c>
@@ -22998,20 +23262,20 @@
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="105"/>
-    <col min="4" max="4" width="14.85546875" style="105" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="106" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="105" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.42578125" style="135" customWidth="1"/>
-    <col min="9" max="9" width="52.42578125" style="105" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="105" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="105"/>
-    <col min="12" max="12" width="12.5703125" style="105" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="105"/>
+    <col min="1" max="1" width="31.1796875" style="105" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1796875" style="105"/>
+    <col min="4" max="4" width="14.81640625" style="105" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" style="106" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" style="105" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" style="105" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.453125" style="135" customWidth="1"/>
+    <col min="9" max="9" width="52.453125" style="105" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" style="105" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" style="105"/>
+    <col min="12" max="12" width="12.54296875" style="105" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="105"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="51" customFormat="1" ht="26.25" customHeight="1">
@@ -24396,7 +24660,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="24.75">
+    <row r="42" spans="1:12">
       <c r="A42" s="109" t="s">
         <v>819</v>
       </c>
@@ -24576,7 +24840,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="36.75">
+    <row r="48" spans="1:12" ht="36.5">
       <c r="A48" s="109" t="s">
         <v>826</v>
       </c>
@@ -24598,7 +24862,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="72.75">
+    <row r="49" spans="1:12" ht="60.5">
       <c r="A49" s="109" t="s">
         <v>827</v>
       </c>
@@ -24688,7 +24952,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="24.75">
+    <row r="52" spans="1:12" ht="24">
       <c r="A52" s="109" t="s">
         <v>830</v>
       </c>
@@ -24720,7 +24984,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="48.75">
+    <row r="53" spans="1:12" ht="36.5">
       <c r="A53" s="109" t="s">
         <v>831</v>
       </c>
@@ -24948,7 +25212,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="24.75">
+    <row r="61" spans="1:12">
       <c r="A61" s="109" t="s">
         <v>839</v>
       </c>
@@ -25122,7 +25386,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="36.75">
+    <row r="67" spans="1:12" ht="24.5">
       <c r="A67" s="109" t="s">
         <v>845</v>
       </c>
@@ -25148,7 +25412,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="72.75">
+    <row r="68" spans="1:12" ht="60.5">
       <c r="A68" s="109" t="s">
         <v>846</v>
       </c>
@@ -25238,7 +25502,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="24.75">
+    <row r="71" spans="1:12" ht="24">
       <c r="A71" s="109" t="s">
         <v>849</v>
       </c>
@@ -25270,7 +25534,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="48.75">
+    <row r="72" spans="1:12" ht="36.5">
       <c r="A72" s="109" t="s">
         <v>850</v>
       </c>

</xml_diff>

<commit_message>
All cells in the Data.xslx optimizer column need at least an empty cell
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron.bray\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C559A11B-F4BE-4DC8-8349-03C4065E10AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F800B9A3-90DE-46F0-B93C-1046C2BBD25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="32400" windowHeight="10590" tabRatio="724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" tabRatio="724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood Chemistry" sheetId="4" r:id="rId1"/>
@@ -8298,9 +8298,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12"/>
@@ -8381,7 +8381,7 @@
       </c>
       <c r="K2" s="184"/>
       <c r="L2" s="184"/>
-      <c r="M2" s="64"/>
+      <c r="M2" s="200"/>
     </row>
     <row r="3" spans="1:13" ht="36.75" customHeight="1">
       <c r="A3" s="170" t="s">
@@ -8631,6 +8631,7 @@
       <c r="L10" s="184" t="s">
         <v>963</v>
       </c>
+      <c r="M10" s="200"/>
     </row>
     <row r="11" spans="1:13" ht="45.75" customHeight="1">
       <c r="A11" s="170" t="s">
@@ -8661,6 +8662,7 @@
       <c r="L11" s="184" t="s">
         <v>963</v>
       </c>
+      <c r="M11" s="200"/>
     </row>
     <row r="12" spans="1:13" ht="27.75" customHeight="1">
       <c r="A12" s="170" t="s">
@@ -8741,7 +8743,7 @@
       </c>
       <c r="K14" s="184"/>
       <c r="L14" s="184"/>
-      <c r="M14" s="64"/>
+      <c r="M14" s="200"/>
     </row>
     <row r="15" spans="1:13" ht="65.25" customHeight="1">
       <c r="A15" s="170" t="s">
@@ -8857,7 +8859,7 @@
       </c>
       <c r="K18" s="184"/>
       <c r="L18" s="184"/>
-      <c r="M18" s="64"/>
+      <c r="M18" s="200"/>
     </row>
     <row r="19" spans="1:13" s="51" customFormat="1">
       <c r="A19" s="172" t="s">
@@ -8878,7 +8880,7 @@
       </c>
       <c r="K19" s="184"/>
       <c r="L19" s="184"/>
-      <c r="M19" s="64"/>
+      <c r="M19" s="200"/>
     </row>
     <row r="20" spans="1:13" s="51" customFormat="1" ht="48">
       <c r="A20" s="170" t="s">
@@ -8911,7 +8913,7 @@
       <c r="L20" s="184" t="s">
         <v>963</v>
       </c>
-      <c r="M20" s="64"/>
+      <c r="M20" s="200"/>
     </row>
     <row r="21" spans="1:13" s="51" customFormat="1">
       <c r="A21" s="170" t="s">
@@ -8942,7 +8944,7 @@
       <c r="L21" s="184" t="s">
         <v>963</v>
       </c>
-      <c r="M21" s="64"/>
+      <c r="M21" s="200"/>
     </row>
     <row r="22" spans="1:13" s="51" customFormat="1" ht="24">
       <c r="A22" s="172" t="s">
@@ -8963,7 +8965,7 @@
       </c>
       <c r="K22" s="184"/>
       <c r="L22" s="184"/>
-      <c r="M22" s="64"/>
+      <c r="M22" s="200"/>
     </row>
     <row r="23" spans="1:13" ht="41.25" customHeight="1">
       <c r="A23" s="170" t="s">
@@ -9029,7 +9031,7 @@
       <c r="L24" s="184" t="s">
         <v>963</v>
       </c>
-      <c r="M24" s="64"/>
+      <c r="M24" s="200"/>
     </row>
     <row r="25" spans="1:13" s="51" customFormat="1">
       <c r="A25" s="170" t="s">
@@ -9058,7 +9060,7 @@
       <c r="L25" s="184" t="s">
         <v>963</v>
       </c>
-      <c r="M25" s="64"/>
+      <c r="M25" s="200"/>
     </row>
     <row r="26" spans="1:13" s="51" customFormat="1">
       <c r="A26" s="172" t="s">
@@ -9079,7 +9081,7 @@
       </c>
       <c r="K26" s="184"/>
       <c r="L26" s="184"/>
-      <c r="M26" s="64"/>
+      <c r="M26" s="200"/>
     </row>
     <row r="27" spans="1:13" s="51" customFormat="1">
       <c r="A27" s="172" t="s">
@@ -9100,7 +9102,7 @@
       </c>
       <c r="K27" s="184"/>
       <c r="L27" s="184"/>
-      <c r="M27" s="64"/>
+      <c r="M27" s="200"/>
     </row>
     <row r="28" spans="1:13" s="51" customFormat="1">
       <c r="A28" s="170" t="s">
@@ -9133,7 +9135,7 @@
       <c r="L28" s="184" t="s">
         <v>963</v>
       </c>
-      <c r="M28" s="64"/>
+      <c r="M28" s="200"/>
     </row>
     <row r="29" spans="1:13" s="51" customFormat="1">
       <c r="A29" s="170" t="s">
@@ -9164,7 +9166,7 @@
       <c r="L29" s="184" t="s">
         <v>961</v>
       </c>
-      <c r="M29" s="64"/>
+      <c r="M29" s="200"/>
     </row>
     <row r="30" spans="1:13" s="51" customFormat="1" ht="36">
       <c r="A30" s="170" t="s">
@@ -9197,7 +9199,7 @@
       <c r="L30" s="184" t="s">
         <v>961</v>
       </c>
-      <c r="M30" s="64"/>
+      <c r="M30" s="200"/>
     </row>
     <row r="31" spans="1:13" s="51" customFormat="1" ht="36">
       <c r="A31" s="170" t="s">
@@ -9232,7 +9234,7 @@
       <c r="L31" s="184" t="s">
         <v>963</v>
       </c>
-      <c r="M31" s="64"/>
+      <c r="M31" s="200"/>
     </row>
     <row r="32" spans="1:13" s="51" customFormat="1" ht="24" customHeight="1">
       <c r="A32" s="170" t="s">
@@ -9265,7 +9267,7 @@
       <c r="L32" s="184" t="s">
         <v>963</v>
       </c>
-      <c r="M32" s="64"/>
+      <c r="M32" s="200"/>
     </row>
     <row r="33" spans="1:13" ht="44.25" customHeight="1">
       <c r="A33" s="170" t="s">
@@ -9331,6 +9333,7 @@
       <c r="L34" s="184" t="s">
         <v>963</v>
       </c>
+      <c r="M34" s="200"/>
     </row>
     <row r="35" spans="1:13" ht="44.25" customHeight="1">
       <c r="A35" s="170" t="s">
@@ -9359,6 +9362,7 @@
       <c r="L35" s="184" t="s">
         <v>963</v>
       </c>
+      <c r="M35" s="200"/>
     </row>
     <row r="36" spans="1:13" s="51" customFormat="1">
       <c r="A36" s="164" t="s">

</xml_diff>

<commit_message>
Corrected Pulmonary flows and volumes to the spreadsheet.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D52FBD6-B79B-4010-8E9B-65D4A5AC7BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F0E173-D360-48F2-BA1C-7F181E1C33FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29235" yWindow="13110" windowWidth="19440" windowHeight="11190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20490" yWindow="7320" windowWidth="38445" windowHeight="21540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -4492,8 +4492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9925,10 +9925,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK109"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A81" sqref="A81"/>
-      <selection pane="topRight" activeCell="F47" sqref="F47"/>
+      <selection pane="topRight" activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12022,10 +12022,15 @@
       <c r="C61" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="D61" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="E61" s="8">
+        <v>0.03</v>
+      </c>
       <c r="F61" s="8">
-        <v>96.5</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C2="Male",D61,E61)</f>
+        <v>51.262450249986841</v>
       </c>
       <c r="G61" s="18" t="s">
         <v>259</v>
@@ -12057,10 +12062,15 @@
       <c r="C62" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
+      <c r="D62" s="8">
+        <v>1</v>
+      </c>
+      <c r="E62" s="8">
+        <v>1</v>
+      </c>
       <c r="F62" s="8">
-        <v>45</v>
+        <f>Patient!C10*Patient!C6*IF(Patient!C3="Male",D62,E62)/60</f>
+        <v>32.666666666666664</v>
       </c>
       <c r="G62" s="18" t="s">
         <v>259</v>
@@ -12090,10 +12100,15 @@
       <c r="C63" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="D63" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="E63" s="8">
+        <v>0.02</v>
+      </c>
       <c r="F63" s="8">
-        <v>65.3</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C4="Male",D63,E63)</f>
+        <v>34.174966833324561</v>
       </c>
       <c r="G63" s="18" t="s">
         <v>259</v>
@@ -12125,10 +12140,15 @@
       <c r="C64" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
+      <c r="D64" s="8">
+        <v>1</v>
+      </c>
+      <c r="E64" s="8">
+        <v>1</v>
+      </c>
       <c r="F64" s="8">
-        <v>45</v>
+        <f>Patient!C10*Patient!C6*IF(Patient!C5="Male",D64,E64)/60</f>
+        <v>32.666666666666664</v>
       </c>
       <c r="G64" s="18" t="s">
         <v>259</v>
@@ -12158,10 +12178,15 @@
       <c r="C65" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
+      <c r="D65" s="8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E65" s="8">
+        <v>5.5E-2</v>
+      </c>
       <c r="F65" s="8">
-        <v>192.9</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C6="Male",D65,E65)</f>
+        <v>93.981158791642542</v>
       </c>
       <c r="G65" s="18" t="s">
         <v>259</v>
@@ -12193,10 +12218,15 @@
       <c r="C66" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+      <c r="D66" s="8">
+        <v>1</v>
+      </c>
+      <c r="E66" s="8">
+        <v>1</v>
+      </c>
       <c r="F66" s="8">
-        <v>45</v>
+        <f>Patient!C10*Patient!C6*IF(Patient!C7="Male",D66,E66)/60</f>
+        <v>32.666666666666664</v>
       </c>
       <c r="G66" s="18" t="s">
         <v>259</v>
@@ -12464,10 +12494,15 @@
       <c r="C73" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
+      <c r="D73" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="E73" s="8">
+        <v>0.03</v>
+      </c>
       <c r="F73" s="8">
-        <v>192.9</v>
+        <f>Patient!C7*IF(Patient!C14="Male",D73,E73)</f>
+        <v>128.15612562496707</v>
       </c>
       <c r="G73" s="18" t="s">
         <v>259</v>
@@ -12499,10 +12534,15 @@
       <c r="C74" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
+      <c r="D74" s="8">
+        <v>1</v>
+      </c>
+      <c r="E74" s="8">
+        <v>1</v>
+      </c>
       <c r="F74" s="8">
-        <v>94.7</v>
+        <f>Patient!C6*IF(Patient!C15="Male",D74,E74)/60</f>
+        <v>81.666666666666671</v>
       </c>
       <c r="G74" s="18" t="s">
         <v>259</v>
@@ -12532,8 +12572,8 @@
       <c r="C75" s="21" t="s">
         <v>354</v>
       </c>
-      <c r="D75" s="21"/>
-      <c r="E75" s="21"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
       <c r="F75" s="8" t="s">
         <v>267</v>
       </c>
@@ -12567,8 +12607,8 @@
       <c r="C76" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="D76" s="21"/>
-      <c r="E76" s="21"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
       <c r="F76" s="8" t="s">
         <v>308</v>
       </c>
@@ -12602,10 +12642,15 @@
       <c r="C77" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+      <c r="D77" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="E77" s="8">
+        <v>0.02</v>
+      </c>
       <c r="F77" s="8">
-        <v>130.5</v>
+        <f>Patient!C7*IF(Patient!C18="Male",D77,E77)</f>
+        <v>85.437417083311388</v>
       </c>
       <c r="G77" s="18" t="s">
         <v>259</v>
@@ -12637,10 +12682,15 @@
       <c r="C78" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
+      <c r="D78" s="8">
+        <v>1</v>
+      </c>
+      <c r="E78" s="8">
+        <v>1</v>
+      </c>
       <c r="F78" s="8">
-        <v>94.7</v>
+        <f>Patient!C6*IF(Patient!C19="Male",D78,E78)/60</f>
+        <v>81.666666666666671</v>
       </c>
       <c r="G78" s="18" t="s">
         <v>259</v>
@@ -12670,8 +12720,8 @@
       <c r="C79" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
       <c r="F79" s="8" t="s">
         <v>267</v>
       </c>
@@ -12707,10 +12757,15 @@
       <c r="C80" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
+      <c r="D80" s="8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E80" s="8">
+        <v>5.5E-2</v>
+      </c>
       <c r="F80" s="8">
-        <v>385.8</v>
+        <f>Patient!C7*IF(Patient!C21="Male",D80,E80)</f>
+        <v>234.95289697910633</v>
       </c>
       <c r="G80" s="18" t="s">
         <v>259</v>
@@ -12742,10 +12797,15 @@
       <c r="C81" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
+      <c r="D81" s="8">
+        <v>1</v>
+      </c>
+      <c r="E81" s="8">
+        <v>1</v>
+      </c>
       <c r="F81" s="8">
-        <v>94.7</v>
+        <f>Patient!C6*IF(Patient!C22="Male",D81,E81)/60</f>
+        <v>81.666666666666671</v>
       </c>
       <c r="G81" s="18" t="s">
         <v>259</v>
@@ -13209,10 +13269,15 @@
       <c r="C94" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
+      <c r="D94" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="E94" s="8">
+        <v>0.03</v>
+      </c>
       <c r="F94" s="8">
-        <v>96.5</v>
+        <f>Patient!C9*Patient!C7*IF(Patient!C35="Male",D94,E94)</f>
+        <v>76.893675374980248</v>
       </c>
       <c r="G94" s="18" t="s">
         <v>259</v>
@@ -13244,10 +13309,15 @@
       <c r="C95" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
+      <c r="D95" s="8">
+        <v>1</v>
+      </c>
+      <c r="E95" s="8">
+        <v>1</v>
+      </c>
       <c r="F95" s="8">
-        <v>49.7</v>
+        <f>Patient!C9*Patient!C6*IF(Patient!C36="Male",D95,E95)/60</f>
+        <v>49</v>
       </c>
       <c r="G95" s="18" t="s">
         <v>259</v>
@@ -13277,10 +13347,15 @@
       <c r="C96" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
+      <c r="D96" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="E96" s="8">
+        <v>0.02</v>
+      </c>
       <c r="F96" s="8">
-        <v>65.3</v>
+        <f>Patient!C9*Patient!C7*IF(Patient!C37="Male",D96,E96)</f>
+        <v>51.262450249986834</v>
       </c>
       <c r="G96" s="18" t="s">
         <v>259</v>
@@ -13312,10 +13387,15 @@
       <c r="C97" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
+      <c r="D97" s="8">
+        <v>1</v>
+      </c>
+      <c r="E97" s="8">
+        <v>1</v>
+      </c>
       <c r="F97" s="8">
-        <v>49.7</v>
+        <f>Patient!C9*Patient!C6*IF(Patient!C38="Male",D97,E97)/60</f>
+        <v>49</v>
       </c>
       <c r="G97" s="18" t="s">
         <v>259</v>
@@ -13345,10 +13425,15 @@
       <c r="C98" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
+      <c r="D98" s="8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E98" s="8">
+        <v>5.5E-2</v>
+      </c>
       <c r="F98" s="8">
-        <v>192.9</v>
+        <f>Patient!C9*Patient!C7*IF(Patient!C39="Male",D98,E98)</f>
+        <v>140.97173818746379</v>
       </c>
       <c r="G98" s="18" t="s">
         <v>259</v>
@@ -13380,10 +13465,15 @@
       <c r="C99" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
+      <c r="D99" s="8">
+        <v>1</v>
+      </c>
+      <c r="E99" s="8">
+        <v>1</v>
+      </c>
       <c r="F99" s="8">
-        <v>49.7</v>
+        <f>Patient!C9*Patient!C6*IF(Patient!C40="Male",D99,E99)/60</f>
+        <v>49</v>
       </c>
       <c r="G99" s="18" t="s">
         <v>259</v>

</xml_diff>

<commit_message>
Updated the validation spreadsheet to correct errors and updated the cardiovascular circuit setup and the renal circuit to reflect the validation data.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F0E173-D360-48F2-BA1C-7F181E1C33FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E666E75-DC5E-426C-A972-E5C4704061AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20490" yWindow="7320" windowWidth="38445" windowHeight="21540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10575" yWindow="675" windowWidth="15525" windowHeight="11190" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -3497,9 +3497,6 @@
     <t>[25,100]</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>1790 roza1984metabolic for 77 kg man</t>
   </si>
   <si>
@@ -3510,6 +3507,9 @@
   </si>
   <si>
     <t>Norgan2003energy</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -4493,7 +4493,7 @@
   <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>1107</v>
+        <v>1111</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="C6" s="5">
         <f>IF(C2="Male",5600,4900)</f>
-        <v>4900</v>
+        <v>5600</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>14</v>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="C8" s="6">
         <f>0.001*C6/C5</f>
-        <v>2.9819853955979925</v>
+        <v>3.4079833092548486</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>14</v>
@@ -4642,7 +4642,7 @@
       </c>
       <c r="C11" s="10">
         <f>IF(C2="Male",15,14)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" s="10"/>
     </row>
@@ -7353,9 +7353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK77"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F9" sqref="F9"/>
+      <selection pane="topRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7644,7 +7644,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="23">
         <f>Patient!C6*Patient!C11/100</f>
-        <v>686</v>
+        <v>840</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>68</v>
@@ -7805,7 +7805,7 @@
       <c r="E14" s="25"/>
       <c r="F14" s="23">
         <f>(F9/0.000000000029)/(Patient!C7*1000)</f>
-        <v>5537426.8608159265</v>
+        <v>6780522.6867133798</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>14</v>
@@ -9385,7 +9385,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="7">
         <f>F14</f>
-        <v>5537426.8608159265</v>
+        <v>6780522.6867133798</v>
       </c>
       <c r="G61" s="7" t="str">
         <f>G14</f>
@@ -9925,10 +9925,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A81" sqref="A81"/>
-      <selection pane="topRight" activeCell="F91" sqref="F91"/>
+      <selection pane="topRight" activeCell="D92" sqref="D92:E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10069,7 +10069,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="49">
         <f>Patient!C8</f>
-        <v>2.9819853955979925</v>
+        <v>3.4079833092548486</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>14</v>
@@ -10105,7 +10105,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="24">
         <f>Patient!C6</f>
-        <v>4900</v>
+        <v>5600</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>14</v>
@@ -10170,17 +10170,11 @@
       <c r="C7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="8">
-        <f>VLOOKUP(A40,A2:J128,MATCH(D1,A1:J1,0),0)</f>
-        <v>0.12</v>
-      </c>
-      <c r="E7" s="8">
-        <f>VLOOKUP(A40,A2:J128,MATCH(E1,A1:J1,0),0)</f>
-        <v>0.12</v>
-      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="21">
         <f>F40*60</f>
-        <v>588</v>
+        <v>672</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>259</v>
@@ -10605,9 +10599,9 @@
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="8">
-        <f>60*F101</f>
-        <v>244.99999999999997</v>
+      <c r="F21" s="52">
+        <f>F101</f>
+        <v>4.666666666666667</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>259</v>
@@ -10945,7 +10939,7 @@
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="8">
+      <c r="F32" s="52">
         <v>1</v>
       </c>
       <c r="G32" s="8" t="s">
@@ -11172,7 +11166,7 @@
       </c>
       <c r="F38" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D38,E38)/60</f>
-        <v>81.666666666666671</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="G38" s="18" t="s">
         <v>259</v>
@@ -11250,7 +11244,7 @@
       </c>
       <c r="F40" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D40,E40)/60</f>
-        <v>9.8000000000000007</v>
+        <v>11.2</v>
       </c>
       <c r="G40" s="18" t="s">
         <v>259</v>
@@ -11319,7 +11313,7 @@
       <c r="E42" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F42" s="21">
+      <c r="F42" s="49">
         <f>Patient!C7*IF(Patient!C2="Male",D42,E42)</f>
         <v>299.03095979158991</v>
       </c>
@@ -11361,7 +11355,7 @@
       </c>
       <c r="F43" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D43,E43)/60</f>
-        <v>4.083333333333333</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="G43" s="18" t="s">
         <v>259</v>
@@ -11397,9 +11391,9 @@
       <c r="E44" s="8">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F44" s="21">
+      <c r="F44" s="49">
         <f>Patient!C7*IF(Patient!C2="Male",D44,E44)</f>
-        <v>363.10902260407346</v>
+        <v>213.59354270827851</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>259</v>
@@ -11437,7 +11431,7 @@
       </c>
       <c r="F45" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D45,E45)/60</f>
-        <v>6.9416666666666673</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="G45" s="18" t="s">
         <v>259</v>
@@ -11473,7 +11467,7 @@
       <c r="E46" s="8">
         <v>0.02</v>
       </c>
-      <c r="F46" s="21">
+      <c r="F46" s="49">
         <f>Patient!C7*IF(Patient!C2="Male",D46,E46)</f>
         <v>85.437417083311388</v>
       </c>
@@ -11513,7 +11507,7 @@
       </c>
       <c r="F47" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D47,E47)/60</f>
-        <v>13.883333333333335</v>
+        <v>17.733333333333334</v>
       </c>
       <c r="G47" s="18" t="s">
         <v>259</v>
@@ -11549,7 +11543,7 @@
       <c r="E48" s="8">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="F48" s="21">
+      <c r="F48" s="49">
         <f>Patient!C7*IF(Patient!C2="Male",D48,E48)</f>
         <v>93.981158791642528</v>
       </c>
@@ -11591,7 +11585,7 @@
       </c>
       <c r="F49" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D49,E49)/60</f>
-        <v>4.083333333333333</v>
+        <v>3.7333333333333334</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>259</v>
@@ -11622,14 +11616,14 @@
         <v>37</v>
       </c>
       <c r="D50" s="8">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E50" s="8">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F50" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="F50" s="52">
         <f>Patient!C7*IF(Patient!C2="Male",D50,E50)</f>
-        <v>106.79677135413925</v>
+        <v>85.437417083311388</v>
       </c>
       <c r="G50" s="18" t="s">
         <v>259</v>
@@ -11662,14 +11656,14 @@
         <v>37</v>
       </c>
       <c r="D51" s="8">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E51" s="8">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F51" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D51,E51)/60</f>
-        <v>1.6333333333333333</v>
+        <v>1.4</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>259</v>
@@ -11874,9 +11868,9 @@
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
-      <c r="F57" s="4">
-        <f>F46*0.55</f>
-        <v>46.990579395821264</v>
+      <c r="F57" s="6">
+        <f>F46*0.5</f>
+        <v>42.718708541655694</v>
       </c>
       <c r="G57" s="27" t="s">
         <v>362</v>
@@ -11911,8 +11905,8 @@
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="49">
-        <f>F47*0.55</f>
-        <v>7.635833333333335</v>
+        <f>F47*0.5</f>
+        <v>8.8666666666666671</v>
       </c>
       <c r="G58" s="18" t="s">
         <v>259</v>
@@ -11945,14 +11939,14 @@
         <v>37</v>
       </c>
       <c r="D59" s="8">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E59" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="F59" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="F59" s="52">
         <f>Patient!C7*IF(Patient!C2="Male",D59,E59)</f>
-        <v>213.59354270827851</v>
+        <v>170.87483416662278</v>
       </c>
       <c r="G59" s="18" t="s">
         <v>259</v>
@@ -11985,14 +11979,14 @@
         <v>37</v>
       </c>
       <c r="D60" s="8">
-        <v>6.25E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E60" s="8">
-        <v>6.25E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F60" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D60,E60)/60</f>
-        <v>5.104166666666667</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G60" s="18" t="s">
         <v>368</v>
@@ -12028,7 +12022,7 @@
       <c r="E61" s="8">
         <v>0.03</v>
       </c>
-      <c r="F61" s="8">
+      <c r="F61" s="52">
         <f>Patient!C10*Patient!C7*IF(Patient!C2="Male",D61,E61)</f>
         <v>51.262450249986841</v>
       </c>
@@ -12068,9 +12062,9 @@
       <c r="E62" s="8">
         <v>1</v>
       </c>
-      <c r="F62" s="8">
+      <c r="F62" s="52">
         <f>Patient!C10*Patient!C6*IF(Patient!C3="Male",D62,E62)/60</f>
-        <v>32.666666666666664</v>
+        <v>37.333333333333336</v>
       </c>
       <c r="G62" s="18" t="s">
         <v>259</v>
@@ -12106,7 +12100,7 @@
       <c r="E63" s="8">
         <v>0.02</v>
       </c>
-      <c r="F63" s="8">
+      <c r="F63" s="52">
         <f>Patient!C10*Patient!C7*IF(Patient!C4="Male",D63,E63)</f>
         <v>34.174966833324561</v>
       </c>
@@ -12146,9 +12140,9 @@
       <c r="E64" s="8">
         <v>1</v>
       </c>
-      <c r="F64" s="8">
+      <c r="F64" s="52">
         <f>Patient!C10*Patient!C6*IF(Patient!C5="Male",D64,E64)/60</f>
-        <v>32.666666666666664</v>
+        <v>37.333333333333336</v>
       </c>
       <c r="G64" s="18" t="s">
         <v>259</v>
@@ -12184,7 +12178,7 @@
       <c r="E65" s="8">
         <v>5.5E-2</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F65" s="52">
         <f>Patient!C10*Patient!C7*IF(Patient!C6="Male",D65,E65)</f>
         <v>93.981158791642542</v>
       </c>
@@ -12224,9 +12218,9 @@
       <c r="E66" s="8">
         <v>1</v>
       </c>
-      <c r="F66" s="8">
+      <c r="F66" s="52">
         <f>Patient!C10*Patient!C6*IF(Patient!C7="Male",D66,E66)/60</f>
-        <v>32.666666666666664</v>
+        <v>37.333333333333336</v>
       </c>
       <c r="G66" s="18" t="s">
         <v>259</v>
@@ -12262,7 +12256,7 @@
       <c r="E67" s="8">
         <v>0.1</v>
       </c>
-      <c r="F67" s="21">
+      <c r="F67" s="49">
         <f>Patient!C7*IF(Patient!C2="Male",D67,E67)</f>
         <v>427.18708541655701</v>
       </c>
@@ -12304,7 +12298,7 @@
       </c>
       <c r="F68" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D68,E68)/60</f>
-        <v>22.05</v>
+        <v>23.8</v>
       </c>
       <c r="G68" s="18" t="s">
         <v>14</v>
@@ -12342,11 +12336,11 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E69" s="8">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="F69" s="8">
+        <v>0.105</v>
+      </c>
+      <c r="F69" s="52">
         <f>Patient!C7*IF(Patient!C2="Male",D69,E69)</f>
-        <v>44.854643968738486</v>
+        <v>598.06191958317982</v>
       </c>
       <c r="G69" s="18" t="s">
         <v>259</v>
@@ -12386,7 +12380,7 @@
       </c>
       <c r="F70" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D70,E70)/60</f>
-        <v>9.8000000000000007</v>
+        <v>15.866666666666669</v>
       </c>
       <c r="G70" s="18" t="s">
         <v>259</v>
@@ -12422,7 +12416,7 @@
       <c r="E71" s="8">
         <v>0.01</v>
       </c>
-      <c r="F71" s="8">
+      <c r="F71" s="52">
         <f>Patient!C7*IF(Patient!C2="Male",D71,E71)</f>
         <v>42.718708541655694</v>
       </c>
@@ -12464,7 +12458,7 @@
       </c>
       <c r="F72" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D72,E72)/60</f>
-        <v>4.083333333333333</v>
+        <v>3.7333333333333334</v>
       </c>
       <c r="G72" s="18" t="s">
         <v>259</v>
@@ -12500,7 +12494,7 @@
       <c r="E73" s="8">
         <v>0.03</v>
       </c>
-      <c r="F73" s="8">
+      <c r="F73" s="52">
         <f>Patient!C7*IF(Patient!C14="Male",D73,E73)</f>
         <v>128.15612562496707</v>
       </c>
@@ -12540,9 +12534,9 @@
       <c r="E74" s="8">
         <v>1</v>
       </c>
-      <c r="F74" s="8">
+      <c r="F74" s="52">
         <f>Patient!C6*IF(Patient!C15="Male",D74,E74)/60</f>
-        <v>81.666666666666671</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="G74" s="18" t="s">
         <v>259</v>
@@ -12648,7 +12642,7 @@
       <c r="E77" s="8">
         <v>0.02</v>
       </c>
-      <c r="F77" s="8">
+      <c r="F77" s="52">
         <f>Patient!C7*IF(Patient!C18="Male",D77,E77)</f>
         <v>85.437417083311388</v>
       </c>
@@ -12688,9 +12682,9 @@
       <c r="E78" s="8">
         <v>1</v>
       </c>
-      <c r="F78" s="8">
+      <c r="F78" s="52">
         <f>Patient!C6*IF(Patient!C19="Male",D78,E78)/60</f>
-        <v>81.666666666666671</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="G78" s="18" t="s">
         <v>259</v>
@@ -12763,7 +12757,7 @@
       <c r="E80" s="8">
         <v>5.5E-2</v>
       </c>
-      <c r="F80" s="8">
+      <c r="F80" s="52">
         <f>Patient!C7*IF(Patient!C21="Male",D80,E80)</f>
         <v>234.95289697910633</v>
       </c>
@@ -12803,9 +12797,9 @@
       <c r="E81" s="8">
         <v>1</v>
       </c>
-      <c r="F81" s="8">
+      <c r="F81" s="52">
         <f>Patient!C6*IF(Patient!C22="Male",D81,E81)/60</f>
-        <v>81.666666666666671</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="G81" s="18" t="s">
         <v>259</v>
@@ -12873,14 +12867,14 @@
         <v>37</v>
       </c>
       <c r="D83" s="8">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E83" s="8">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F83" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="F83" s="52">
         <f>Patient!C7*IF(Patient!C2="Male",D83,E83)</f>
-        <v>106.79677135413925</v>
+        <v>85.437417083311388</v>
       </c>
       <c r="G83" s="18" t="s">
         <v>259</v>
@@ -12913,14 +12907,14 @@
         <v>37</v>
       </c>
       <c r="D84" s="8">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E84" s="8">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F84" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D84,E84)/60</f>
-        <v>1.6333333333333333</v>
+        <v>1.4</v>
       </c>
       <c r="G84" s="18" t="s">
         <v>401</v>
@@ -13121,9 +13115,9 @@
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
-      <c r="F90" s="4">
-        <f>F46*0.45</f>
-        <v>38.446837687490124</v>
+      <c r="F90" s="6">
+        <f>F46*0.5</f>
+        <v>42.718708541655694</v>
       </c>
       <c r="G90" s="27" t="s">
         <v>362</v>
@@ -13158,8 +13152,8 @@
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
       <c r="F91" s="49">
-        <f>F47*0.55</f>
-        <v>7.635833333333335</v>
+        <f>F47*0.5</f>
+        <v>8.8666666666666671</v>
       </c>
       <c r="G91" s="18" t="s">
         <v>259</v>
@@ -13192,14 +13186,14 @@
         <v>37</v>
       </c>
       <c r="D92" s="8">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E92" s="8">
-        <v>0</v>
-      </c>
-      <c r="F92" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="F92" s="52">
         <f>Patient!C7*IF(Patient!C2="Male",D92,E92)</f>
-        <v>0</v>
+        <v>170.87483416662278</v>
       </c>
       <c r="G92" s="18" t="s">
         <v>259</v>
@@ -13232,14 +13226,14 @@
         <v>37</v>
       </c>
       <c r="D93" s="8">
-        <v>6.25E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E93" s="8">
-        <v>6.25E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F93" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D93,E93)/60</f>
-        <v>5.104166666666667</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G93" s="18" t="s">
         <v>368</v>
@@ -13275,7 +13269,7 @@
       <c r="E94" s="8">
         <v>0.03</v>
       </c>
-      <c r="F94" s="8">
+      <c r="F94" s="52">
         <f>Patient!C9*Patient!C7*IF(Patient!C35="Male",D94,E94)</f>
         <v>76.893675374980248</v>
       </c>
@@ -13317,7 +13311,7 @@
       </c>
       <c r="F95" s="8">
         <f>Patient!C9*Patient!C6*IF(Patient!C36="Male",D95,E95)/60</f>
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G95" s="18" t="s">
         <v>259</v>
@@ -13353,7 +13347,7 @@
       <c r="E96" s="8">
         <v>0.02</v>
       </c>
-      <c r="F96" s="8">
+      <c r="F96" s="52">
         <f>Patient!C9*Patient!C7*IF(Patient!C37="Male",D96,E96)</f>
         <v>51.262450249986834</v>
       </c>
@@ -13395,7 +13389,7 @@
       </c>
       <c r="F97" s="8">
         <f>Patient!C9*Patient!C6*IF(Patient!C38="Male",D97,E97)/60</f>
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G97" s="18" t="s">
         <v>259</v>
@@ -13431,7 +13425,7 @@
       <c r="E98" s="8">
         <v>5.5E-2</v>
       </c>
-      <c r="F98" s="8">
+      <c r="F98" s="52">
         <f>Patient!C9*Patient!C7*IF(Patient!C39="Male",D98,E98)</f>
         <v>140.97173818746379</v>
       </c>
@@ -13473,7 +13467,7 @@
       </c>
       <c r="F99" s="8">
         <f>Patient!C9*Patient!C6*IF(Patient!C40="Male",D99,E99)/60</f>
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G99" s="18" t="s">
         <v>259</v>
@@ -13509,7 +13503,7 @@
       <c r="E100" s="8">
         <v>0.03</v>
       </c>
-      <c r="F100" s="8">
+      <c r="F100" s="52">
         <f>Patient!C7*IF(Patient!C2="Male",D100,E100)</f>
         <v>128.15612562496707</v>
       </c>
@@ -13551,7 +13545,7 @@
       </c>
       <c r="F101" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D101,E101)/60</f>
-        <v>4.083333333333333</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="G101" s="18" t="s">
         <v>259</v>
@@ -13587,7 +13581,7 @@
       <c r="E102" s="8">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="F102" s="21">
+      <c r="F102" s="49">
         <f>Patient!C7*IF(Patient!C2="Male",D102,E102)</f>
         <v>162.33109245829164</v>
       </c>
@@ -13627,7 +13621,7 @@
       </c>
       <c r="F103" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D103,E103)/60</f>
-        <v>8.9833333333333325</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="G103" s="18" t="s">
         <v>259</v>
@@ -13658,14 +13652,14 @@
         <v>37</v>
       </c>
       <c r="D104" s="8">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
       <c r="E104" s="8">
-        <v>0.11</v>
-      </c>
-      <c r="F104" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="F104" s="49">
         <f>Patient!C7*IF(Patient!C2="Male",D104,E104)</f>
-        <v>469.90579395821266</v>
+        <v>42.718708541655694</v>
       </c>
       <c r="G104" s="18" t="s">
         <v>259</v>
@@ -13696,14 +13690,14 @@
         <v>37</v>
       </c>
       <c r="D105" s="8">
-        <v>2.5000000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E105" s="8">
-        <v>2.5000000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F105" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D105,E105)/60</f>
-        <v>2.0416666666666665</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="G105" s="18" t="s">
         <v>259</v>
@@ -13741,8 +13735,9 @@
       <c r="E106" s="8">
         <v>1.4E-2</v>
       </c>
-      <c r="F106" s="21">
-        <v>79.400000000000006</v>
+      <c r="F106" s="49">
+        <f>Patient!C7*IF(Patient!C2="Male",D106,E106)</f>
+        <v>59.806191958317974</v>
       </c>
       <c r="G106" s="18" t="s">
         <v>259</v>
@@ -13780,7 +13775,7 @@
       </c>
       <c r="F107" s="49">
         <f>Patient!C6*IF(Patient!C2="Male",D107,E107)/60</f>
-        <v>2.4500000000000002</v>
+        <v>2.8</v>
       </c>
       <c r="G107" s="18" t="s">
         <v>259</v>
@@ -13811,13 +13806,14 @@
         <v>37</v>
       </c>
       <c r="D108" s="8">
-        <v>0.18</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="E108" s="8">
-        <v>0.18</v>
-      </c>
-      <c r="F108" s="8">
-        <v>1032.7</v>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="F108" s="52">
+        <f>Patient!C7*IF(Patient!C2="Male",D108,E108)</f>
+        <v>747.5773994789746</v>
       </c>
       <c r="G108" s="18" t="s">
         <v>259</v>
@@ -13857,7 +13853,7 @@
       </c>
       <c r="F109" s="52">
         <f>Patient!C6*IF(Patient!C2="Male",D109,E109)/60</f>
-        <v>81.666666666666671</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="G109" s="18" t="s">
         <v>259</v>
@@ -14303,17 +14299,17 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="7" t="s">
+        <v>1109</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>1110</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>1111</v>
       </c>
       <c r="H11" s="61"/>
       <c r="I11" s="7" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>1108</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>1109</v>
       </c>
       <c r="K11" s="61"/>
       <c r="L11" s="62" t="s">
@@ -14794,7 +14790,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="52">
         <f>Cardiovascular!F47*60</f>
-        <v>833.00000000000011</v>
+        <v>1064</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>259</v>
@@ -14827,7 +14823,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8">
         <f>F4*0.6</f>
-        <v>499.80000000000007</v>
+        <v>638.4</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Updated the spreadhseet to correct errors in calculating total extracellular and intracellular tissue and adding coronary perfusion pressure.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\patient_variability\source\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87817C4B-7F47-464E-8B0D-132E97E188D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7C5CB0-3C1B-4B6D-BE60-9837AB0037C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="3990" windowWidth="32640" windowHeight="21840" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="0" windowWidth="23640" windowHeight="12900" tabRatio="500" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4709" uniqueCount="1103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4715" uniqueCount="1107">
   <si>
     <t>Patient Inputs</t>
   </si>
@@ -3481,6 +3481,18 @@
   </si>
   <si>
     <t>General range for men and women</t>
+  </si>
+  <si>
+    <t>CoronaryPerfusionPressure</t>
+  </si>
+  <si>
+    <t>[60,80]</t>
+  </si>
+  <si>
+    <t>AhmedCoronary2014</t>
+  </si>
+  <si>
+    <t>Excluding intravascular fluid, sum of compartments</t>
   </si>
 </sst>
 </file>
@@ -4681,10 +4693,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="I91" sqref="I91"/>
+      <selection pane="topRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4799,19 +4811,19 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="8">
-        <f>SUM(F13,F17,F20,F23,F26,F29,F32,F35,F38,F41,F46,F49,F52)</f>
-        <v>6647.9417176647639</v>
+      <c r="F3" s="49">
+        <f>SUM(F14,F17,F20,F23,F26,F29,F32,F35,F38,F41,F46,F49,F52)</f>
+        <v>8751.6116205773851</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>266</v>
+        <v>985</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="7" t="s">
         <v>1100</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>959</v>
+        <v>1106</v>
       </c>
       <c r="K3" s="33" t="s">
         <v>960</v>
@@ -4841,10 +4853,10 @@
       <c r="E4" s="7"/>
       <c r="F4" s="8">
         <f>SUM(F13:F42,F46:F53)</f>
-        <v>34081.065120622952</v>
+        <v>34084.065120622952</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>266</v>
+        <v>985</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7" t="s">
@@ -4914,11 +4926,12 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="8">
-        <v>25320</v>
+      <c r="F6" s="49">
+        <f>SUM(F15+F18+F21+F24+F27+F30+F33+F36+F39+F42+F47+F50+F53)</f>
+        <v>25271.303751033935</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>266</v>
+        <v>985</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="7" t="s">
@@ -6146,8 +6159,8 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="6">
-        <f>F34*0.44*1000</f>
-        <v>132</v>
+        <f>F34*0.446*1000</f>
+        <v>133.80000000000001</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>985</v>
@@ -6272,8 +6285,8 @@
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="6">
-        <f>F37*0.44*1000</f>
-        <v>88.000000000000014</v>
+        <f>F37*0.446*1000</f>
+        <v>89.2</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>985</v>
@@ -11028,12 +11041,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AML109"/>
+  <dimension ref="A1:AML110"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A77" sqref="A77"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="topRight" activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11142,7 +11155,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="22">
-        <f>Patient!C7</f>
+        <f>Patient!$C$7</f>
         <v>5509.6546665792184</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -11181,7 +11194,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="47">
-        <f>Patient!C8</f>
+        <f>Patient!$C$8</f>
         <v>2.9991033145287878</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -11220,7 +11233,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="22">
-        <f>Patient!C6</f>
+        <f>Patient!$C$6</f>
         <v>5600</v>
       </c>
       <c r="G5" s="8" t="s">
@@ -11293,7 +11306,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="19">
-        <f>F40*60</f>
+        <f>F41*60</f>
         <v>672</v>
       </c>
       <c r="G7" s="16" t="s">
@@ -11349,11 +11362,11 @@
       </c>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="45.75" customHeight="1">
+    <row r="9" spans="1:16">
       <c r="A9" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="B9" s="8" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>191</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -11362,34 +11375,26 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="19" t="s">
-        <v>271</v>
+        <v>1104</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>263</v>
-      </c>
+        <v>1105</v>
+      </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8" t="s">
-        <v>272</v>
-      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="46"/>
-      <c r="M9" s="4" t="s">
-        <v>255</v>
-      </c>
+      <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O9" s="4"/>
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" ht="45.75" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>191</v>
@@ -11399,18 +11404,22 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
-        <v>274</v>
+      <c r="F10" s="19" t="s">
+        <v>271</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="H10" s="8"/>
+        <v>83</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>263</v>
+      </c>
       <c r="I10" s="8" t="s">
         <v>1100</v>
       </c>
       <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="K10" s="8" t="s">
+        <v>272</v>
+      </c>
       <c r="L10" s="46"/>
       <c r="M10" s="4" t="s">
         <v>255</v>
@@ -11423,7 +11432,7 @@
     </row>
     <row r="11" spans="1:16" ht="45.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>191</v>
@@ -11434,19 +11443,17 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J11" s="48"/>
-      <c r="K11" s="24" t="s">
-        <v>278</v>
-      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="46"/>
       <c r="M11" s="4" t="s">
         <v>255</v>
@@ -11457,29 +11464,31 @@
       </c>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="27.75" customHeight="1">
+    <row r="12" spans="1:16" ht="45.75" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="B12" s="8"/>
+        <v>276</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>191</v>
+      </c>
       <c r="C12" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="19">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="25"/>
+      <c r="F12" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="H12" s="16"/>
       <c r="I12" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8" t="s">
-        <v>280</v>
+      <c r="J12" s="48"/>
+      <c r="K12" s="24" t="s">
+        <v>278</v>
       </c>
       <c r="L12" s="46"/>
       <c r="M12" s="4" t="s">
@@ -11487,57 +11496,65 @@
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:16" ht="74.25" customHeight="1">
+    <row r="13" spans="1:16" ht="27.75" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>282</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="19" t="s">
-        <v>283</v>
+      <c r="F13" s="19">
+        <v>0.55000000000000004</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="H13" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="H13" s="25"/>
       <c r="I13" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="K13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8" t="s">
+        <v>280</v>
+      </c>
       <c r="L13" s="46"/>
       <c r="M13" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+    <row r="14" spans="1:16" ht="74.25" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>284</v>
+      </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8" t="s">
-        <v>286</v>
+      <c r="I14" s="8" t="s">
+        <v>1100</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="46"/>
@@ -11545,71 +11562,61 @@
         <v>255</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="O14" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:16" ht="65.25" customHeight="1">
-      <c r="A15" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>44</v>
-      </c>
+    <row r="15" spans="1:16">
+      <c r="A15" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="G15" s="43" t="s">
-        <v>289</v>
-      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="8" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8" t="s">
-        <v>290</v>
-      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="K15" s="8"/>
       <c r="L15" s="46"/>
       <c r="M15" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O15" s="4"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" ht="65.25" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>191</v>
+        <v>287</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="19" t="s">
-        <v>292</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>293</v>
+      <c r="F16" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>289</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J16" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="K16" s="16"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8" t="s">
+        <v>290</v>
+      </c>
       <c r="L16" s="46"/>
       <c r="M16" s="4" t="s">
         <v>255</v>
@@ -11620,11 +11627,11 @@
       </c>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16" ht="40.5" customHeight="1">
+    <row r="17" spans="1:16">
       <c r="A17" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="B17" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>191</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -11632,22 +11639,20 @@
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="8" t="s">
-        <v>296</v>
+      <c r="F17" s="19" t="s">
+        <v>292</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>263</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8" t="s">
-        <v>272</v>
-      </c>
+      <c r="J17" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="K17" s="16"/>
       <c r="L17" s="46"/>
       <c r="M17" s="4" t="s">
         <v>255</v>
@@ -11658,33 +11663,47 @@
       </c>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="45" t="s">
-        <v>297</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+    <row r="18" spans="1:16" ht="40.5" customHeight="1">
+      <c r="A18" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="K18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>1100</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8" t="s">
+        <v>272</v>
+      </c>
       <c r="L18" s="46"/>
       <c r="M18" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
+      <c r="O18" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="45" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -11706,69 +11725,57 @@
       <c r="O19" s="4"/>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16" ht="60">
-      <c r="A20" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>44</v>
-      </c>
+    <row r="20" spans="1:16">
+      <c r="A20" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J20" s="8"/>
-      <c r="K20" s="16" t="s">
-        <v>264</v>
-      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="K20" s="8"/>
       <c r="L20" s="46"/>
       <c r="M20" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N20" s="4"/>
-      <c r="O20" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O20" s="4"/>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" ht="24">
+    <row r="21" spans="1:16" ht="60">
       <c r="A21" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>191</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="49">
-        <f>F101</f>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="H21" s="8"/>
+      <c r="F21" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>263</v>
+      </c>
       <c r="I21" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="K21" s="8" t="s">
-        <v>303</v>
+      <c r="J21" s="8"/>
+      <c r="K21" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="L21" s="46"/>
       <c r="M21" s="4" t="s">
@@ -11780,73 +11787,71 @@
       </c>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16" ht="24">
-      <c r="A22" s="45" t="s">
-        <v>304</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="24">
+      <c r="A22" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="F22" s="49">
+        <f>F102</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>266</v>
+      </c>
       <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="K22" s="8"/>
+      <c r="I22" s="8" t="s">
+        <v>1100</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>303</v>
+      </c>
       <c r="L22" s="46"/>
       <c r="M22" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
+      <c r="O22" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" ht="41.25" customHeight="1">
-      <c r="A23" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>44</v>
-      </c>
+    <row r="23" spans="1:16" ht="24">
+      <c r="A23" s="45" t="s">
+        <v>304</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16" t="s">
-        <v>306</v>
-      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="K23" s="8"/>
       <c r="L23" s="46"/>
       <c r="M23" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N23" s="4"/>
-      <c r="O23" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O23" s="4"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16" ht="24">
+    <row r="24" spans="1:16" ht="41.25" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="B24" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>191</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -11854,21 +11859,21 @@
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="8" t="s">
-        <v>308</v>
+      <c r="F24" s="16" t="s">
+        <v>274</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>310</v>
+        <v>83</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8" t="s">
-        <v>272</v>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16" t="s">
+        <v>306</v>
       </c>
       <c r="L24" s="46"/>
       <c r="M24" s="4" t="s">
@@ -11880,9 +11885,9 @@
       </c>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" ht="24">
       <c r="A25" s="11" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>191</v>
@@ -11893,17 +11898,21 @@
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="H25" s="8"/>
+        <v>308</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>310</v>
+      </c>
       <c r="I25" s="8" t="s">
         <v>1100</v>
       </c>
       <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="K25" s="8" t="s">
+        <v>272</v>
+      </c>
       <c r="L25" s="46"/>
       <c r="M25" s="4" t="s">
         <v>255</v>
@@ -11915,38 +11924,48 @@
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="45" t="s">
-        <v>313</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="F26" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>275</v>
+      </c>
       <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="I26" s="8" t="s">
+        <v>1100</v>
+      </c>
       <c r="J26" s="8"/>
-      <c r="K26" s="8" t="s">
-        <v>314</v>
-      </c>
+      <c r="K26" s="8"/>
       <c r="L26" s="46"/>
       <c r="M26" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
+      <c r="O26" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="50"/>
+      <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -11963,85 +11982,73 @@
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="A28" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>1100</v>
-      </c>
+      <c r="F28" s="50"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="L28" s="46"/>
       <c r="M28" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N28" s="4"/>
-      <c r="O28" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O28" s="4"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16" ht="24">
+    <row r="29" spans="1:16">
       <c r="A29" s="11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>319</v>
+        <v>191</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="8">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>15</v>
+      <c r="F29" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>320</v>
+        <v>263</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>1100</v>
       </c>
       <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="K29" s="8" t="s">
+        <v>272</v>
+      </c>
       <c r="L29" s="46"/>
       <c r="M29" s="4" t="s">
         <v>255</v>
       </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="s">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16" s="1" customFormat="1" ht="36">
+    <row r="30" spans="1:16" ht="24">
       <c r="A30" s="11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>44</v>
@@ -12049,20 +12056,19 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8">
-        <v>0.24</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J30" s="8" t="s">
-        <v>324</v>
-      </c>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
       <c r="L30" s="46"/>
       <c r="M30" s="4" t="s">
         <v>255</v>
@@ -12073,33 +12079,32 @@
       </c>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16" ht="24">
+    <row r="31" spans="1:16" s="1" customFormat="1" ht="36">
       <c r="A31" s="11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>191</v>
+        <v>322</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="8" t="s">
-        <v>326</v>
+      <c r="F31" s="8">
+        <v>0.24</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="H31" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>323</v>
+      </c>
       <c r="I31" s="8" t="s">
         <v>1100</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="L31" s="46"/>
       <c r="M31" s="4" t="s">
@@ -12107,37 +12112,37 @@
       </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" ht="24" customHeight="1">
+    <row r="32" spans="1:16" ht="24">
       <c r="A32" s="11" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>319</v>
+        <v>191</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="49">
-        <v>1</v>
+      <c r="F32" s="8" t="s">
+        <v>326</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>331</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="H32" s="8"/>
       <c r="I32" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J32" s="8"/>
+      <c r="J32" s="8" t="s">
+        <v>328</v>
+      </c>
       <c r="K32" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="L32" s="46"/>
       <c r="M32" s="4" t="s">
@@ -12149,33 +12154,33 @@
       </c>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="1:16" ht="44.25" customHeight="1">
+    <row r="33" spans="1:16" ht="24" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>191</v>
+        <v>319</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="19" t="s">
-        <v>334</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>83</v>
+      <c r="F33" s="49">
+        <v>1</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>263</v>
+        <v>331</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>1100</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8" t="s">
-        <v>272</v>
+        <v>332</v>
       </c>
       <c r="L33" s="46"/>
       <c r="M33" s="4" t="s">
@@ -12189,7 +12194,7 @@
     </row>
     <row r="34" spans="1:16" ht="44.25" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>191</v>
@@ -12199,21 +12204,21 @@
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="19" t="s">
         <v>334</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>337</v>
+        <v>83</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>263</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J34" s="48"/>
-      <c r="K34" s="24" t="s">
-        <v>338</v>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="L34" s="46"/>
       <c r="M34" s="4" t="s">
@@ -12227,7 +12232,7 @@
     </row>
     <row r="35" spans="1:16" ht="44.25" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>191</v>
@@ -12238,17 +12243,21 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="H35" s="8"/>
+        <v>336</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>337</v>
+      </c>
       <c r="I35" s="8" t="s">
         <v>1100</v>
       </c>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="24" t="s">
+        <v>338</v>
+      </c>
       <c r="L35" s="46"/>
       <c r="M35" s="4" t="s">
         <v>255</v>
@@ -12259,118 +12268,109 @@
       </c>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16">
-      <c r="A36" s="27" t="s">
+    <row r="36" spans="1:16" ht="44.25" customHeight="1">
+      <c r="A36" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8" t="s">
+        <v>1100</v>
+      </c>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G36" s="28" t="s">
+      <c r="G37" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H37" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="I36" s="10" t="s">
+      <c r="I37" s="10" t="s">
         <v>1099</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L36" s="28" t="s">
+      <c r="L37" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M36" s="10" t="s">
+      <c r="M37" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="N36" s="10" t="s">
+      <c r="N37" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O36" s="10" t="s">
+      <c r="O37" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="P36" s="10" t="s">
+      <c r="P37" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="24.75">
-      <c r="A37" s="11" t="s">
+    <row r="38" spans="1:16" ht="24.75">
+      <c r="A38" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B38" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="8">
+      <c r="C38" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="8">
         <v>0.05</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E38" s="8">
         <v>0.05</v>
       </c>
-      <c r="F37" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D37,E37)</f>
+      <c r="F38" s="49">
+        <f>Patient!C7*IF(Patient!C2="Male",D38,E38)</f>
         <v>275.48273332896093</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J37" s="48"/>
-      <c r="K37" s="44" t="s">
-        <v>342</v>
-      </c>
-      <c r="L37" s="46"/>
-      <c r="M37" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P37" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="36.75">
-      <c r="A38" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="8">
-        <v>1</v>
-      </c>
-      <c r="E38" s="8">
-        <v>1</v>
-      </c>
-      <c r="F38" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D38,E38)/60</f>
-        <v>93.333333333333329</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>266</v>
@@ -12380,8 +12380,8 @@
         <v>1100</v>
       </c>
       <c r="J38" s="48"/>
-      <c r="K38" s="24" t="s">
-        <v>346</v>
+      <c r="K38" s="44" t="s">
+        <v>342</v>
       </c>
       <c r="L38" s="46"/>
       <c r="M38" s="4" t="s">
@@ -12395,25 +12395,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" ht="36.75">
       <c r="A39" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D39" s="8">
-        <v>1.2E-2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="8">
-        <v>1.2E-2</v>
+        <v>1</v>
       </c>
       <c r="F39" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D39,E39)</f>
-        <v>66.115855998950622</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D39,E39)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>266</v>
@@ -12422,8 +12422,10 @@
       <c r="I39" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J39" s="16"/>
-      <c r="K39" s="24"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="24" t="s">
+        <v>346</v>
+      </c>
       <c r="L39" s="46"/>
       <c r="M39" s="4" t="s">
         <v>343</v>
@@ -12438,23 +12440,23 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="8">
-        <v>0.12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E40" s="8">
-        <v>0.12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F40" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D40,E40)/60</f>
-        <v>11.2</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D40,E40)</f>
+        <v>66.115855998950622</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>266</v>
@@ -12479,30 +12481,33 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>191</v>
+        <v>302</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="19">
-        <v>40</v>
+      <c r="D41" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="E41" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="F41" s="49">
+        <f>Patient!C6*IF(Patient!C2="Male",D41,E41)/60</f>
+        <v>11.2</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="H41" s="16">
-        <v>409</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H41" s="16"/>
       <c r="I41" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J41" s="16"/>
-      <c r="K41" s="51"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="46"/>
       <c r="M41" s="4" t="s">
         <v>343</v>
@@ -12511,39 +12516,36 @@
       <c r="O41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P41" s="3"/>
+      <c r="P41" s="7" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>17</v>
+        <v>191</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E42" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F42" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D42,E42)</f>
-        <v>385.67582666054534</v>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="19">
+        <v>40</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H42" s="16"/>
+        <v>350</v>
+      </c>
+      <c r="H42" s="16">
+        <v>409</v>
+      </c>
       <c r="I42" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J42" s="16"/>
-      <c r="K42" s="44" t="s">
-        <v>352</v>
-      </c>
+      <c r="K42" s="51"/>
       <c r="L42" s="46"/>
       <c r="M42" s="4" t="s">
         <v>343</v>
@@ -12552,29 +12554,27 @@
       <c r="O42" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P42" s="7" t="s">
-        <v>344</v>
-      </c>
+      <c r="P42" s="3"/>
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D43" s="8">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E43" s="8">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F43" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D43,E43)/60</f>
-        <v>4.666666666666667</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D43,E43)</f>
+        <v>385.67582666054534</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>266</v>
@@ -12584,7 +12584,9 @@
         <v>1100</v>
       </c>
       <c r="J43" s="16"/>
-      <c r="K43" s="24"/>
+      <c r="K43" s="44" t="s">
+        <v>352</v>
+      </c>
       <c r="L43" s="46"/>
       <c r="M43" s="4" t="s">
         <v>343</v>
@@ -12599,10 +12601,10 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>44</v>
@@ -12611,20 +12613,20 @@
         <v>0.05</v>
       </c>
       <c r="E44" s="8">
-        <v>8.5000000000000006E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F44" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D44,E44)</f>
-        <v>275.48273332896093</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D44,E44)/60</f>
+        <v>4.666666666666667</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="H44" s="8"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J44" s="8"/>
+      <c r="J44" s="16"/>
       <c r="K44" s="24"/>
       <c r="L44" s="46"/>
       <c r="M44" s="4" t="s">
@@ -12640,10 +12642,10 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>44</v>
@@ -12655,17 +12657,17 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F45" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D45,E45)/60</f>
-        <v>4.666666666666667</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D45,E45)</f>
+        <v>275.48273332896093</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="H45" s="16"/>
+      <c r="H45" s="8"/>
       <c r="I45" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J45" s="16"/>
+      <c r="J45" s="8"/>
       <c r="K45" s="24"/>
       <c r="L45" s="46"/>
       <c r="M45" s="4" t="s">
@@ -12681,32 +12683,32 @@
     </row>
     <row r="46" spans="1:16">
       <c r="A46" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D46" s="8">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E46" s="8">
-        <v>0.02</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F46" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D46,E46)</f>
-        <v>110.19309333158436</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D46,E46)/60</f>
+        <v>4.666666666666667</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="H46" s="52"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J46" s="52"/>
+      <c r="J46" s="16"/>
       <c r="K46" s="24"/>
       <c r="L46" s="46"/>
       <c r="M46" s="4" t="s">
@@ -12722,32 +12724,32 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D47" s="8">
-        <v>0.19</v>
+        <v>0.02</v>
       </c>
       <c r="E47" s="8">
-        <v>0.17</v>
+        <v>0.02</v>
       </c>
       <c r="F47" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D47,E47)/60</f>
-        <v>17.733333333333334</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D47,E47)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="H47" s="16"/>
+      <c r="H47" s="52"/>
       <c r="I47" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J47" s="16"/>
+      <c r="J47" s="52"/>
       <c r="K47" s="24"/>
       <c r="L47" s="46"/>
       <c r="M47" s="4" t="s">
@@ -12761,25 +12763,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="24.75">
+    <row r="48" spans="1:16">
       <c r="A48" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D48" s="8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.19</v>
       </c>
       <c r="E48" s="8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.17</v>
       </c>
       <c r="F48" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D48,E48)</f>
-        <v>121.2124026647428</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D48,E48)/60</f>
+        <v>17.733333333333334</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>266</v>
@@ -12789,9 +12791,7 @@
         <v>1100</v>
       </c>
       <c r="J48" s="16"/>
-      <c r="K48" s="44" t="s">
-        <v>359</v>
-      </c>
+      <c r="K48" s="24"/>
       <c r="L48" s="46"/>
       <c r="M48" s="4" t="s">
         <v>343</v>
@@ -12804,25 +12804,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" ht="24.75">
       <c r="A49" s="11" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D49" s="8">
-        <v>0.04</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E49" s="8">
-        <v>0.05</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F49" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D49,E49)/60</f>
-        <v>3.7333333333333334</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D49,E49)</f>
+        <v>121.2124026647428</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>266</v>
@@ -12832,7 +12832,9 @@
         <v>1100</v>
       </c>
       <c r="J49" s="16"/>
-      <c r="K49" s="24"/>
+      <c r="K49" s="44" t="s">
+        <v>359</v>
+      </c>
       <c r="L49" s="46"/>
       <c r="M49" s="4" t="s">
         <v>343</v>
@@ -12845,25 +12847,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="36.75">
+    <row r="50" spans="1:16">
       <c r="A50" s="11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D50" s="8">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E50" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F50" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D50,E50)</f>
-        <v>110.19309333158436</v>
+        <v>0.05</v>
+      </c>
+      <c r="F50" s="47">
+        <f>Patient!C6*IF(Patient!C2="Male",D50,E50)/60</f>
+        <v>3.7333333333333334</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>266</v>
@@ -12872,10 +12874,8 @@
       <c r="I50" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J50" s="48"/>
-      <c r="K50" s="44" t="s">
-        <v>362</v>
-      </c>
+      <c r="J50" s="16"/>
+      <c r="K50" s="24"/>
       <c r="L50" s="46"/>
       <c r="M50" s="4" t="s">
         <v>343</v>
@@ -12888,25 +12888,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" ht="36.75">
       <c r="A51" s="11" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D51" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E51" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F51" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D51,E51)/60</f>
-        <v>1.4</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D51,E51)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>266</v>
@@ -12917,50 +12917,57 @@
       </c>
       <c r="J51" s="48"/>
       <c r="K51" s="44" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L51" s="46"/>
       <c r="M51" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
+      <c r="O51" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="P51" s="7" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>366</v>
-      </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="8" t="s">
-        <v>367</v>
+        <v>302</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E52" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F52" s="49">
+        <f>Patient!C6*IF(Patient!C2="Male",D52,E52)/60</f>
+        <v>1.4</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>368</v>
+        <v>266</v>
       </c>
       <c r="H52" s="16"/>
       <c r="I52" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J52" s="48"/>
-      <c r="K52" s="24"/>
+      <c r="K52" s="44" t="s">
+        <v>364</v>
+      </c>
       <c r="L52" s="46"/>
       <c r="M52" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N52" s="4"/>
-      <c r="O52" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O52" s="4"/>
       <c r="P52" s="7" t="s">
         <v>344</v>
       </c>
@@ -12973,12 +12980,12 @@
         <v>17</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="19"/>
       <c r="F53" s="8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>368</v>
@@ -13003,21 +13010,21 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="11" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>191</v>
+        <v>17</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="19"/>
       <c r="F54" s="8" t="s">
-        <v>274</v>
+        <v>370</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>275</v>
+        <v>368</v>
       </c>
       <c r="H54" s="16"/>
       <c r="I54" s="16" t="s">
@@ -13037,7 +13044,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="48.75">
+    <row r="55" spans="1:16">
       <c r="A55" s="11" t="s">
         <v>371</v>
       </c>
@@ -13045,26 +13052,22 @@
         <v>191</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D55" s="19"/>
       <c r="E55" s="19"/>
       <c r="F55" s="8" t="s">
-        <v>334</v>
+        <v>274</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>337</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="H55" s="16"/>
       <c r="I55" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J55" s="48"/>
-      <c r="K55" s="24" t="s">
-        <v>338</v>
-      </c>
+      <c r="K55" s="24"/>
       <c r="L55" s="46"/>
       <c r="M55" s="4" t="s">
         <v>343</v>
@@ -13077,34 +13080,34 @@
         <v>344</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" ht="48.75">
       <c r="A56" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D56" s="8">
-        <v>1</v>
-      </c>
-      <c r="E56" s="8">
-        <v>1</v>
-      </c>
-      <c r="F56" s="8">
-        <v>94.7</v>
+        <v>191</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H56" s="16"/>
+        <v>336</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>337</v>
+      </c>
       <c r="I56" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J56" s="48"/>
-      <c r="K56" s="24"/>
+      <c r="K56" s="24" t="s">
+        <v>338</v>
+      </c>
       <c r="L56" s="46"/>
       <c r="M56" s="4" t="s">
         <v>343</v>
@@ -13117,33 +13120,34 @@
         <v>344</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="24.75">
+    <row r="57" spans="1:16">
       <c r="A57" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="6">
-        <f>F46*0.5</f>
-        <v>55.096546665792182</v>
-      </c>
-      <c r="G57" s="25" t="s">
-        <v>374</v>
+      <c r="D57" s="8">
+        <v>1</v>
+      </c>
+      <c r="E57" s="8">
+        <v>1</v>
+      </c>
+      <c r="F57" s="8">
+        <v>94.7</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="H57" s="16"/>
       <c r="I57" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J57" s="48"/>
-      <c r="K57" s="44" t="s">
-        <v>375</v>
-      </c>
+      <c r="K57" s="24"/>
       <c r="L57" s="46"/>
       <c r="M57" s="4" t="s">
         <v>343</v>
@@ -13158,30 +13162,30 @@
     </row>
     <row r="58" spans="1:16" ht="24.75">
       <c r="A58" s="11" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
-      <c r="F58" s="47">
+      <c r="F58" s="6">
         <f>F47*0.5</f>
-        <v>8.8666666666666671</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>266</v>
+        <v>55.096546665792182</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>374</v>
       </c>
       <c r="H58" s="16"/>
       <c r="I58" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J58" s="48"/>
-      <c r="K58" s="24" t="s">
-        <v>377</v>
+      <c r="K58" s="44" t="s">
+        <v>375</v>
       </c>
       <c r="L58" s="46"/>
       <c r="M58" s="4" t="s">
@@ -13195,25 +13199,21 @@
         <v>344</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="36.75">
+    <row r="59" spans="1:16" ht="24.75">
       <c r="A59" s="11" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D59" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="E59" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="F59" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D59,E59)</f>
-        <v>220.38618666316873</v>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="47">
+        <f>F48*0.5</f>
+        <v>8.8666666666666671</v>
       </c>
       <c r="G59" s="16" t="s">
         <v>266</v>
@@ -13223,8 +13223,8 @@
         <v>1100</v>
       </c>
       <c r="J59" s="48"/>
-      <c r="K59" s="44" t="s">
-        <v>362</v>
+      <c r="K59" s="24" t="s">
+        <v>377</v>
       </c>
       <c r="L59" s="46"/>
       <c r="M59" s="4" t="s">
@@ -13238,28 +13238,28 @@
         <v>344</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" ht="36.75">
       <c r="A60" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D60" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E60" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F60" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D60,E60)/60</f>
-        <v>4.9000000000000004</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D60,E60)</f>
+        <v>220.38618666316873</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>380</v>
+        <v>266</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="16" t="s">
@@ -13267,40 +13267,42 @@
       </c>
       <c r="J60" s="48"/>
       <c r="K60" s="44" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="L60" s="46"/>
       <c r="M60" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
+      <c r="O60" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="P60" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="24.75">
+    <row r="61" spans="1:16">
       <c r="A61" s="11" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D61" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E61" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F61" s="49">
-        <f>Patient!C10*Patient!C7*IF(Patient!C2="Male",D61,E61)</f>
-        <v>66.115855998950622</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D61,E61)/60</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>266</v>
+        <v>380</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16" t="s">
@@ -13308,39 +13310,37 @@
       </c>
       <c r="J61" s="48"/>
       <c r="K61" s="44" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L61" s="46"/>
       <c r="M61" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N61" s="4"/>
-      <c r="O61" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O61" s="4"/>
       <c r="P61" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" ht="24.75">
       <c r="A62" s="11" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D62" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E62" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="F62" s="49">
-        <f>Patient!C10*Patient!C6*IF(Patient!C3="Male",D62,E62)/60</f>
-        <v>37.333333333333336</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C2="Male",D62,E62)</f>
+        <v>66.115855998950622</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>266</v>
@@ -13350,7 +13350,9 @@
         <v>1100</v>
       </c>
       <c r="J62" s="48"/>
-      <c r="K62" s="24"/>
+      <c r="K62" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L62" s="46"/>
       <c r="M62" s="4" t="s">
         <v>343</v>
@@ -13363,25 +13365,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="24.75">
+    <row r="63" spans="1:16">
       <c r="A63" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D63" s="8">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="E63" s="8">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="F63" s="49">
-        <f>Patient!C10*Patient!C7*IF(Patient!C4="Male",D63,E63)</f>
-        <v>44.07723733263375</v>
+        <f>Patient!C10*Patient!C6*IF(Patient!C3="Male",D63,E63)/60</f>
+        <v>37.333333333333336</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>266</v>
@@ -13391,9 +13393,7 @@
         <v>1100</v>
       </c>
       <c r="J63" s="48"/>
-      <c r="K63" s="44" t="s">
-        <v>383</v>
-      </c>
+      <c r="K63" s="24"/>
       <c r="L63" s="46"/>
       <c r="M63" s="4" t="s">
         <v>343</v>
@@ -13406,25 +13406,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" ht="24.75">
       <c r="A64" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D64" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="E64" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="F64" s="49">
-        <f>Patient!C10*Patient!C6*IF(Patient!C5="Male",D64,E64)/60</f>
-        <v>37.333333333333336</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C4="Male",D64,E64)</f>
+        <v>44.07723733263375</v>
       </c>
       <c r="G64" s="16" t="s">
         <v>266</v>
@@ -13434,7 +13434,9 @@
         <v>1100</v>
       </c>
       <c r="J64" s="48"/>
-      <c r="K64" s="24"/>
+      <c r="K64" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L64" s="46"/>
       <c r="M64" s="4" t="s">
         <v>343</v>
@@ -13447,25 +13449,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="24.75">
+    <row r="65" spans="1:16">
       <c r="A65" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D65" s="8">
-        <v>5.5E-2</v>
+        <v>1</v>
       </c>
       <c r="E65" s="8">
-        <v>5.5E-2</v>
+        <v>1</v>
       </c>
       <c r="F65" s="49">
-        <f>Patient!C10*Patient!C7*IF(Patient!C6="Male",D65,E65)</f>
-        <v>121.21240266474281</v>
+        <f>Patient!C10*Patient!C6*IF(Patient!C5="Male",D65,E65)/60</f>
+        <v>37.333333333333336</v>
       </c>
       <c r="G65" s="16" t="s">
         <v>266</v>
@@ -13475,9 +13477,7 @@
         <v>1100</v>
       </c>
       <c r="J65" s="48"/>
-      <c r="K65" s="44" t="s">
-        <v>383</v>
-      </c>
+      <c r="K65" s="24"/>
       <c r="L65" s="46"/>
       <c r="M65" s="4" t="s">
         <v>343</v>
@@ -13490,25 +13490,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" ht="24.75">
       <c r="A66" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D66" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E66" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F66" s="49">
-        <f>Patient!C10*Patient!C6*IF(Patient!C7="Male",D66,E66)/60</f>
-        <v>37.333333333333336</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C6="Male",D66,E66)</f>
+        <v>121.21240266474281</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>266</v>
@@ -13518,7 +13518,9 @@
         <v>1100</v>
       </c>
       <c r="J66" s="48"/>
-      <c r="K66" s="24"/>
+      <c r="K66" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L66" s="46"/>
       <c r="M66" s="4" t="s">
         <v>343</v>
@@ -13531,25 +13533,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="24.75">
+    <row r="67" spans="1:16">
       <c r="A67" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D67" s="8">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E67" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F67" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D67,E67)</f>
-        <v>550.96546665792187</v>
+        <v>1</v>
+      </c>
+      <c r="F67" s="49">
+        <f>Patient!C10*Patient!C6*IF(Patient!C7="Male",D67,E67)/60</f>
+        <v>37.333333333333336</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>266</v>
@@ -13558,10 +13560,8 @@
       <c r="I67" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J67" s="16"/>
-      <c r="K67" s="44" t="s">
-        <v>390</v>
-      </c>
+      <c r="J67" s="48"/>
+      <c r="K67" s="24"/>
       <c r="L67" s="46"/>
       <c r="M67" s="4" t="s">
         <v>343</v>
@@ -13574,38 +13574,36 @@
         <v>344</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" ht="24.75">
       <c r="A68" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D68" s="8">
-        <v>0.255</v>
+        <v>0.1</v>
       </c>
       <c r="E68" s="8">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="F68" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D68,E68)/60</f>
-        <v>23.8</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D68,E68)</f>
+        <v>550.96546665792187</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>392</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H68" s="16"/>
       <c r="I68" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J68" s="16"/>
-      <c r="K68" s="24" t="s">
-        <v>393</v>
+      <c r="K68" s="44" t="s">
+        <v>390</v>
       </c>
       <c r="L68" s="46"/>
       <c r="M68" s="4" t="s">
@@ -13621,34 +13619,36 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="11" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D69" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.255</v>
       </c>
       <c r="E69" s="8">
-        <v>0.105</v>
-      </c>
-      <c r="F69" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D69,E69)</f>
-        <v>771.35165332109068</v>
+        <v>0.27</v>
+      </c>
+      <c r="F69" s="47">
+        <f>Patient!C6*IF(Patient!C2="Male",D69,E69)/60</f>
+        <v>23.8</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H69" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="H69" s="16" t="s">
+        <v>392</v>
+      </c>
       <c r="I69" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J69" s="16"/>
-      <c r="K69" s="44" t="s">
-        <v>395</v>
+      <c r="K69" s="24" t="s">
+        <v>393</v>
       </c>
       <c r="L69" s="46"/>
       <c r="M69" s="4" t="s">
@@ -13664,23 +13664,23 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" s="11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D70" s="8">
-        <v>0.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E70" s="8">
-        <v>0.12</v>
+        <v>0.105</v>
       </c>
       <c r="F70" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D70,E70)/60</f>
-        <v>15.866666666666669</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D70,E70)</f>
+        <v>771.35165332109068</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>266</v>
@@ -13690,7 +13690,9 @@
         <v>1100</v>
       </c>
       <c r="J70" s="16"/>
-      <c r="K70" s="24"/>
+      <c r="K70" s="44" t="s">
+        <v>395</v>
+      </c>
       <c r="L70" s="46"/>
       <c r="M70" s="4" t="s">
         <v>343</v>
@@ -13705,23 +13707,23 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D71" s="8">
-        <v>0.01</v>
+        <v>0.17</v>
       </c>
       <c r="E71" s="8">
-        <v>0.01</v>
+        <v>0.12</v>
       </c>
       <c r="F71" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D71,E71)</f>
-        <v>55.096546665792182</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D71,E71)/60</f>
+        <v>15.866666666666669</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>266</v>
@@ -13730,10 +13732,8 @@
       <c r="I71" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J71" s="48"/>
-      <c r="K71" s="44" t="s">
-        <v>398</v>
-      </c>
+      <c r="J71" s="16"/>
+      <c r="K71" s="24"/>
       <c r="L71" s="46"/>
       <c r="M71" s="4" t="s">
         <v>343</v>
@@ -13748,23 +13748,23 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D72" s="8">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="E72" s="8">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F72" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D72,E72)/60</f>
-        <v>3.7333333333333334</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D72,E72)</f>
+        <v>55.096546665792182</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>266</v>
@@ -13774,7 +13774,9 @@
         <v>1100</v>
       </c>
       <c r="J72" s="48"/>
-      <c r="K72" s="24"/>
+      <c r="K72" s="44" t="s">
+        <v>398</v>
+      </c>
       <c r="L72" s="46"/>
       <c r="M72" s="4" t="s">
         <v>343</v>
@@ -13787,25 +13789,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="24.75">
+    <row r="73" spans="1:16">
       <c r="A73" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D73" s="8">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E73" s="8">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F73" s="49">
-        <f>Patient!C7*IF(Patient!C19="Male",D73,E73)</f>
-        <v>165.28963999737655</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D73,E73)/60</f>
+        <v>3.7333333333333334</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>266</v>
@@ -13815,9 +13817,7 @@
         <v>1100</v>
       </c>
       <c r="J73" s="48"/>
-      <c r="K73" s="44" t="s">
-        <v>383</v>
-      </c>
+      <c r="K73" s="24"/>
       <c r="L73" s="46"/>
       <c r="M73" s="4" t="s">
         <v>343</v>
@@ -13830,25 +13830,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" ht="24.75">
       <c r="A74" s="11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D74" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E74" s="8">
-        <v>1</v>
-      </c>
-      <c r="F74" s="49" t="e">
-        <f>Patient!C6*IF(Patient!#REF!="Male",D74,E74)/60</f>
-        <v>#REF!</v>
+        <v>0.03</v>
+      </c>
+      <c r="F74" s="49">
+        <f>Patient!C7*IF(Patient!C19="Male",D74,E74)</f>
+        <v>165.28963999737655</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>266</v>
@@ -13858,7 +13858,9 @@
         <v>1100</v>
       </c>
       <c r="J74" s="48"/>
-      <c r="K74" s="24"/>
+      <c r="K74" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L74" s="46"/>
       <c r="M74" s="4" t="s">
         <v>343</v>
@@ -13873,25 +13875,28 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C75" s="19" t="s">
-        <v>366</v>
-      </c>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="8" t="s">
-        <v>274</v>
+        <v>302</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="8">
+        <v>1</v>
+      </c>
+      <c r="E75" s="8">
+        <v>1</v>
+      </c>
+      <c r="F75" s="49">
+        <f>Patient!C6*IF(Patient!C2="Male",D75,E75)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H75" s="16" t="s">
-        <v>263</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H75" s="16"/>
       <c r="I75" s="16" t="s">
         <v>1100</v>
       </c>
@@ -13917,12 +13922,12 @@
         <v>191</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="8" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>83</v>
@@ -13947,37 +13952,32 @@
         <v>344</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="24.75">
+    <row r="77" spans="1:16">
       <c r="A77" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D77" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="E77" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F77" s="49" t="e">
-        <f>Patient!C7*IF(Patient!#REF!="Male",D77,E77)</f>
-        <v>#REF!</v>
+        <v>191</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="8" t="s">
+        <v>317</v>
       </c>
       <c r="G77" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H77" s="16"/>
+        <v>83</v>
+      </c>
+      <c r="H77" s="16" t="s">
+        <v>263</v>
+      </c>
       <c r="I77" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J77" s="48"/>
-      <c r="K77" s="44" t="s">
-        <v>383</v>
-      </c>
+      <c r="K77" s="24"/>
       <c r="L77" s="46"/>
       <c r="M77" s="4" t="s">
         <v>343</v>
@@ -13990,25 +13990,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" ht="24.75">
       <c r="A78" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D78" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="E78" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="F78" s="49">
-        <f>Patient!C6*IF(Patient!C20="Male",D78,E78)/60</f>
-        <v>93.333333333333329</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D78,E78)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G78" s="16" t="s">
         <v>266</v>
@@ -14018,7 +14018,9 @@
         <v>1100</v>
       </c>
       <c r="J78" s="48"/>
-      <c r="K78" s="24"/>
+      <c r="K78" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L78" s="46"/>
       <c r="M78" s="4" t="s">
         <v>343</v>
@@ -14033,32 +14035,33 @@
     </row>
     <row r="79" spans="1:16">
       <c r="A79" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="8" t="s">
-        <v>274</v>
+        <v>302</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="8">
+        <v>1</v>
+      </c>
+      <c r="E79" s="8">
+        <v>1</v>
+      </c>
+      <c r="F79" s="49">
+        <f>Patient!C6*IF(Patient!C20="Male",D79,E79)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G79" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H79" s="16" t="s">
-        <v>263</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H79" s="16"/>
       <c r="I79" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J79" s="48"/>
-      <c r="K79" s="24" t="s">
-        <v>406</v>
-      </c>
+      <c r="K79" s="24"/>
       <c r="L79" s="46"/>
       <c r="M79" s="4" t="s">
         <v>343</v>
@@ -14071,36 +14074,33 @@
         <v>344</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="24.75">
+    <row r="80" spans="1:16">
       <c r="A80" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D80" s="8">
-        <v>5.5E-2</v>
-      </c>
-      <c r="E80" s="8">
-        <v>5.5E-2</v>
-      </c>
-      <c r="F80" s="49">
-        <f>Patient!C7*IF(Patient!C22="Male",D80,E80)</f>
-        <v>303.03100666185702</v>
+        <v>191</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H80" s="16"/>
+        <v>83</v>
+      </c>
+      <c r="H80" s="16" t="s">
+        <v>263</v>
+      </c>
       <c r="I80" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J80" s="48"/>
-      <c r="K80" s="44" t="s">
-        <v>383</v>
+      <c r="K80" s="24" t="s">
+        <v>406</v>
       </c>
       <c r="L80" s="46"/>
       <c r="M80" s="4" t="s">
@@ -14114,25 +14114,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" ht="24.75">
       <c r="A81" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D81" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E81" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F81" s="49">
-        <f>Patient!C6*IF(Patient!C23="Male",D81,E81)/60</f>
-        <v>93.333333333333329</v>
+        <f>Patient!C7*IF(Patient!C22="Male",D81,E81)</f>
+        <v>303.03100666185702</v>
       </c>
       <c r="G81" s="16" t="s">
         <v>266</v>
@@ -14142,7 +14142,9 @@
         <v>1100</v>
       </c>
       <c r="J81" s="48"/>
-      <c r="K81" s="24"/>
+      <c r="K81" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L81" s="46"/>
       <c r="M81" s="4" t="s">
         <v>343</v>
@@ -14155,34 +14157,35 @@
         <v>344</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="36.75">
+    <row r="82" spans="1:16">
       <c r="A82" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="8" t="s">
-        <v>274</v>
+        <v>302</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="8">
+        <v>1</v>
+      </c>
+      <c r="E82" s="8">
+        <v>1</v>
+      </c>
+      <c r="F82" s="49">
+        <f>Patient!C6*IF(Patient!C23="Male",D82,E82)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G82" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H82" s="16" t="s">
-        <v>263</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H82" s="16"/>
       <c r="I82" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J82" s="48"/>
-      <c r="K82" s="24" t="s">
-        <v>410</v>
-      </c>
+      <c r="K82" s="24"/>
       <c r="L82" s="46"/>
       <c r="M82" s="4" t="s">
         <v>343</v>
@@ -14197,34 +14200,31 @@
     </row>
     <row r="83" spans="1:16" ht="36.75">
       <c r="A83" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D83" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="E83" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F83" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D83,E83)</f>
-        <v>110.19309333158436</v>
+        <v>191</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H83" s="16"/>
+        <v>83</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>263</v>
+      </c>
       <c r="I83" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J83" s="48"/>
-      <c r="K83" s="44" t="s">
-        <v>362</v>
+      <c r="K83" s="24" t="s">
+        <v>410</v>
       </c>
       <c r="L83" s="46"/>
       <c r="M83" s="4" t="s">
@@ -14238,28 +14238,28 @@
         <v>344</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" ht="36.75">
       <c r="A84" s="11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D84" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E84" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F84" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D84,E84)/60</f>
-        <v>1.4</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D84,E84)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G84" s="16" t="s">
-        <v>413</v>
+        <v>266</v>
       </c>
       <c r="H84" s="16"/>
       <c r="I84" s="16" t="s">
@@ -14267,35 +14267,42 @@
       </c>
       <c r="J84" s="48"/>
       <c r="K84" s="44" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L84" s="46"/>
       <c r="M84" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
+      <c r="O84" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="P84" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="60.75">
+    <row r="85" spans="1:16">
       <c r="A85" s="11" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>366</v>
-      </c>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="8" t="s">
-        <v>415</v>
+        <v>302</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D85" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E85" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F85" s="49">
+        <f>Patient!C6*IF(Patient!C2="Male",D85,E85)/60</f>
+        <v>1.4</v>
       </c>
       <c r="G85" s="16" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H85" s="16"/>
       <c r="I85" s="16" t="s">
@@ -14303,21 +14310,19 @@
       </c>
       <c r="J85" s="48"/>
       <c r="K85" s="44" t="s">
-        <v>417</v>
+        <v>364</v>
       </c>
       <c r="L85" s="46"/>
       <c r="M85" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N85" s="4"/>
-      <c r="O85" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O85" s="4"/>
       <c r="P85" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="24">
+    <row r="86" spans="1:16" ht="60.75">
       <c r="A86" s="11" t="s">
         <v>414</v>
       </c>
@@ -14325,12 +14330,12 @@
         <v>17</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D86" s="19"/>
       <c r="E86" s="19"/>
       <c r="F86" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G86" s="16" t="s">
         <v>416</v>
@@ -14340,7 +14345,9 @@
         <v>1100</v>
       </c>
       <c r="J86" s="48"/>
-      <c r="K86" s="24"/>
+      <c r="K86" s="44" t="s">
+        <v>417</v>
+      </c>
       <c r="L86" s="46"/>
       <c r="M86" s="4" t="s">
         <v>343</v>
@@ -14353,32 +14360,30 @@
         <v>344</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="36.75">
+    <row r="87" spans="1:16" ht="24">
       <c r="A87" s="11" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>191</v>
+        <v>17</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D87" s="19"/>
       <c r="E87" s="19"/>
       <c r="F87" s="8" t="s">
-        <v>277</v>
+        <v>418</v>
       </c>
       <c r="G87" s="16" t="s">
-        <v>275</v>
+        <v>416</v>
       </c>
       <c r="H87" s="16"/>
       <c r="I87" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J87" s="48"/>
-      <c r="K87" s="24" t="s">
-        <v>278</v>
-      </c>
+      <c r="K87" s="24"/>
       <c r="L87" s="46"/>
       <c r="M87" s="4" t="s">
         <v>343</v>
@@ -14391,7 +14396,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" ht="36.75">
       <c r="A88" s="11" t="s">
         <v>419</v>
       </c>
@@ -14399,12 +14404,12 @@
         <v>191</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="19"/>
       <c r="F88" s="8" t="s">
-        <v>317</v>
+        <v>277</v>
       </c>
       <c r="G88" s="16" t="s">
         <v>275</v>
@@ -14414,7 +14419,9 @@
         <v>1100</v>
       </c>
       <c r="J88" s="48"/>
-      <c r="K88" s="24"/>
+      <c r="K88" s="24" t="s">
+        <v>278</v>
+      </c>
       <c r="L88" s="46"/>
       <c r="M88" s="4" t="s">
         <v>343</v>
@@ -14429,21 +14436,21 @@
     </row>
     <row r="89" spans="1:16">
       <c r="A89" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8">
-        <v>94.7</v>
+        <v>191</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="8" t="s">
+        <v>317</v>
       </c>
       <c r="G89" s="16" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="H89" s="16"/>
       <c r="I89" s="16" t="s">
@@ -14463,33 +14470,30 @@
         <v>344</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="24.75">
+    <row r="90" spans="1:16">
       <c r="A90" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
-      <c r="F90" s="6">
-        <f>F46*0.5</f>
-        <v>55.096546665792182</v>
-      </c>
-      <c r="G90" s="25" t="s">
-        <v>374</v>
+      <c r="F90" s="8">
+        <v>94.7</v>
+      </c>
+      <c r="G90" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="H90" s="16"/>
       <c r="I90" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J90" s="48"/>
-      <c r="K90" s="44" t="s">
-        <v>375</v>
-      </c>
+      <c r="K90" s="24"/>
       <c r="L90" s="46"/>
       <c r="M90" s="4" t="s">
         <v>343</v>
@@ -14504,30 +14508,30 @@
     </row>
     <row r="91" spans="1:16" ht="24.75">
       <c r="A91" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
-      <c r="F91" s="47">
+      <c r="F91" s="6">
         <f>F47*0.5</f>
-        <v>8.8666666666666671</v>
-      </c>
-      <c r="G91" s="16" t="s">
-        <v>266</v>
+        <v>55.096546665792182</v>
+      </c>
+      <c r="G91" s="25" t="s">
+        <v>374</v>
       </c>
       <c r="H91" s="16"/>
       <c r="I91" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J91" s="48"/>
-      <c r="K91" s="24" t="s">
-        <v>377</v>
+      <c r="K91" s="44" t="s">
+        <v>375</v>
       </c>
       <c r="L91" s="46"/>
       <c r="M91" s="4" t="s">
@@ -14541,25 +14545,21 @@
         <v>344</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="36.75">
+    <row r="92" spans="1:16" ht="24.75">
       <c r="A92" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D92" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="E92" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="F92" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D92,E92)</f>
-        <v>220.38618666316873</v>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="47">
+        <f>F48*0.5</f>
+        <v>8.8666666666666671</v>
       </c>
       <c r="G92" s="16" t="s">
         <v>266</v>
@@ -14569,8 +14569,8 @@
         <v>1100</v>
       </c>
       <c r="J92" s="48"/>
-      <c r="K92" s="44" t="s">
-        <v>362</v>
+      <c r="K92" s="24" t="s">
+        <v>377</v>
       </c>
       <c r="L92" s="46"/>
       <c r="M92" s="4" t="s">
@@ -14584,28 +14584,28 @@
         <v>344</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" ht="36.75">
       <c r="A93" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D93" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E93" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F93" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D93,E93)/60</f>
-        <v>4.9000000000000004</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D93,E93)</f>
+        <v>220.38618666316873</v>
       </c>
       <c r="G93" s="16" t="s">
-        <v>380</v>
+        <v>266</v>
       </c>
       <c r="H93" s="16"/>
       <c r="I93" s="16" t="s">
@@ -14613,40 +14613,42 @@
       </c>
       <c r="J93" s="48"/>
       <c r="K93" s="44" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="L93" s="46"/>
       <c r="M93" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
+      <c r="O93" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="P93" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="24.75">
+    <row r="94" spans="1:16">
       <c r="A94" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D94" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E94" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F94" s="49">
-        <f>Patient!C9*Patient!C7*IF(Patient!C36="Male",D94,E94)</f>
-        <v>99.173783998425932</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D94,E94)/60</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G94" s="16" t="s">
-        <v>266</v>
+        <v>380</v>
       </c>
       <c r="H94" s="16"/>
       <c r="I94" s="16" t="s">
@@ -14654,39 +14656,37 @@
       </c>
       <c r="J94" s="48"/>
       <c r="K94" s="44" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L94" s="46"/>
       <c r="M94" s="4" t="s">
         <v>343</v>
       </c>
       <c r="N94" s="4"/>
-      <c r="O94" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="O94" s="4"/>
       <c r="P94" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" ht="24.75">
       <c r="A95" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D95" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E95" s="8">
-        <v>1</v>
-      </c>
-      <c r="F95" s="8">
-        <f>Patient!C9*Patient!C6*IF(Patient!C37="Male",D95,E95)/60</f>
-        <v>56</v>
+        <v>0.03</v>
+      </c>
+      <c r="F95" s="49">
+        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D95,E95)</f>
+        <v>99.173783998425932</v>
       </c>
       <c r="G95" s="16" t="s">
         <v>266</v>
@@ -14696,7 +14696,9 @@
         <v>1100</v>
       </c>
       <c r="J95" s="48"/>
-      <c r="K95" s="24"/>
+      <c r="K95" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L95" s="46"/>
       <c r="M95" s="4" t="s">
         <v>343</v>
@@ -14709,25 +14711,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="24.75">
+    <row r="96" spans="1:16">
       <c r="A96" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D96" s="8">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="E96" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F96" s="49">
-        <f>Patient!C9*Patient!C7*IF(Patient!C38="Male",D96,E96)</f>
-        <v>66.115855998950622</v>
+        <v>1</v>
+      </c>
+      <c r="F96" s="8">
+        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D96,E96)/60</f>
+        <v>56</v>
       </c>
       <c r="G96" s="16" t="s">
         <v>266</v>
@@ -14737,9 +14739,7 @@
         <v>1100</v>
       </c>
       <c r="J96" s="48"/>
-      <c r="K96" s="44" t="s">
-        <v>383</v>
-      </c>
+      <c r="K96" s="24"/>
       <c r="L96" s="46"/>
       <c r="M96" s="4" t="s">
         <v>343</v>
@@ -14752,25 +14752,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" ht="24.75">
       <c r="A97" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D97" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="E97" s="8">
-        <v>1</v>
-      </c>
-      <c r="F97" s="8">
-        <f>Patient!C9*Patient!C6*IF(Patient!C39="Male",D97,E97)/60</f>
-        <v>56</v>
+        <v>0.02</v>
+      </c>
+      <c r="F97" s="49">
+        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D97,E97)</f>
+        <v>66.115855998950622</v>
       </c>
       <c r="G97" s="16" t="s">
         <v>266</v>
@@ -14780,7 +14780,9 @@
         <v>1100</v>
       </c>
       <c r="J97" s="48"/>
-      <c r="K97" s="24"/>
+      <c r="K97" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L97" s="46"/>
       <c r="M97" s="4" t="s">
         <v>343</v>
@@ -14793,25 +14795,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="24.75">
+    <row r="98" spans="1:16">
       <c r="A98" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D98" s="8">
-        <v>5.5E-2</v>
+        <v>1</v>
       </c>
       <c r="E98" s="8">
-        <v>5.5E-2</v>
-      </c>
-      <c r="F98" s="49">
-        <f>Patient!C9*Patient!C7*IF(Patient!C40="Male",D98,E98)</f>
-        <v>181.8186039971142</v>
+        <v>1</v>
+      </c>
+      <c r="F98" s="8">
+        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D98,E98)/60</f>
+        <v>56</v>
       </c>
       <c r="G98" s="16" t="s">
         <v>266</v>
@@ -14820,10 +14822,8 @@
       <c r="I98" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J98" s="16"/>
-      <c r="K98" s="44" t="s">
-        <v>383</v>
-      </c>
+      <c r="J98" s="48"/>
+      <c r="K98" s="24"/>
       <c r="L98" s="46"/>
       <c r="M98" s="4" t="s">
         <v>343</v>
@@ -14836,25 +14836,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" ht="24.75">
       <c r="A99" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D99" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E99" s="8">
-        <v>1</v>
-      </c>
-      <c r="F99" s="8">
-        <f>Patient!C9*Patient!C6*IF(Patient!C41="Male",D99,E99)/60</f>
-        <v>56</v>
+        <v>5.5E-2</v>
+      </c>
+      <c r="F99" s="49">
+        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D99,E99)</f>
+        <v>181.8186039971142</v>
       </c>
       <c r="G99" s="16" t="s">
         <v>266</v>
@@ -14864,7 +14864,9 @@
         <v>1100</v>
       </c>
       <c r="J99" s="16"/>
-      <c r="K99" s="24"/>
+      <c r="K99" s="44" t="s">
+        <v>383</v>
+      </c>
       <c r="L99" s="46"/>
       <c r="M99" s="4" t="s">
         <v>343</v>
@@ -14877,25 +14879,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="24.75">
+    <row r="100" spans="1:16">
       <c r="A100" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D100" s="8">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E100" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="F100" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D100,E100)</f>
-        <v>165.28963999737655</v>
+        <v>1</v>
+      </c>
+      <c r="F100" s="8">
+        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D100,E100)/60</f>
+        <v>56</v>
       </c>
       <c r="G100" s="16" t="s">
         <v>266</v>
@@ -14905,9 +14907,7 @@
         <v>1100</v>
       </c>
       <c r="J100" s="16"/>
-      <c r="K100" s="44" t="s">
-        <v>390</v>
-      </c>
+      <c r="K100" s="24"/>
       <c r="L100" s="46"/>
       <c r="M100" s="4" t="s">
         <v>343</v>
@@ -14920,25 +14920,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" ht="24.75">
       <c r="A101" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D101" s="8">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E101" s="8">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F101" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D101,E101)/60</f>
-        <v>4.666666666666667</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D101,E101)</f>
+        <v>165.28963999737655</v>
       </c>
       <c r="G101" s="16" t="s">
         <v>266</v>
@@ -14948,7 +14948,9 @@
         <v>1100</v>
       </c>
       <c r="J101" s="16"/>
-      <c r="K101" s="24"/>
+      <c r="K101" s="44" t="s">
+        <v>390</v>
+      </c>
       <c r="L101" s="46"/>
       <c r="M101" s="4" t="s">
         <v>343</v>
@@ -14963,23 +14965,23 @@
     </row>
     <row r="102" spans="1:16">
       <c r="A102" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D102" s="8">
-        <v>3.7999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E102" s="8">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="F102" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D102,E102)</f>
-        <v>209.36687733001028</v>
+        <v>0.05</v>
+      </c>
+      <c r="F102" s="49">
+        <f>Patient!C6*IF(Patient!C2="Male",D102,E102)/60</f>
+        <v>4.666666666666667</v>
       </c>
       <c r="G102" s="16" t="s">
         <v>266</v>
@@ -15004,23 +15006,23 @@
     </row>
     <row r="103" spans="1:16">
       <c r="A103" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D103" s="8">
-        <v>0.1</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E103" s="8">
-        <v>0.11</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F103" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D103,E103)/60</f>
-        <v>9.3333333333333339</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D103,E103)</f>
+        <v>209.36687733001028</v>
       </c>
       <c r="G103" s="16" t="s">
         <v>266</v>
@@ -15045,23 +15047,23 @@
     </row>
     <row r="104" spans="1:16">
       <c r="A104" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D104" s="8">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="E104" s="8">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="F104" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D104,E104)</f>
-        <v>55.096546665792182</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D104,E104)/60</f>
+        <v>9.3333333333333339</v>
       </c>
       <c r="G104" s="16" t="s">
         <v>266</v>
@@ -15086,10 +15088,10 @@
     </row>
     <row r="105" spans="1:16">
       <c r="A105" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>44</v>
@@ -15101,20 +15103,18 @@
         <v>0.01</v>
       </c>
       <c r="F105" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D105,E105)/60</f>
-        <v>0.93333333333333335</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D105,E105)</f>
+        <v>55.096546665792182</v>
       </c>
       <c r="G105" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="H105" s="8"/>
+      <c r="H105" s="16"/>
       <c r="I105" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J105" s="8"/>
-      <c r="K105" s="44" t="s">
-        <v>437</v>
-      </c>
+      <c r="J105" s="16"/>
+      <c r="K105" s="24"/>
       <c r="L105" s="46"/>
       <c r="M105" s="4" t="s">
         <v>343</v>
@@ -15129,33 +15129,35 @@
     </row>
     <row r="106" spans="1:16">
       <c r="A106" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D106" s="8">
-        <v>1.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E106" s="8">
-        <v>1.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F106" s="47">
-        <f>Patient!C7*IF(Patient!C2="Male",D106,E106)</f>
-        <v>77.135165332109054</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D106,E106)/60</f>
+        <v>0.93333333333333335</v>
       </c>
       <c r="G106" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="H106" s="16"/>
+      <c r="H106" s="8"/>
       <c r="I106" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J106" s="48"/>
-      <c r="K106" s="24"/>
+      <c r="J106" s="8"/>
+      <c r="K106" s="44" t="s">
+        <v>437</v>
+      </c>
       <c r="L106" s="46"/>
       <c r="M106" s="4" t="s">
         <v>343</v>
@@ -15170,23 +15172,23 @@
     </row>
     <row r="107" spans="1:16">
       <c r="A107" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D107" s="8">
-        <v>0.03</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E107" s="8">
-        <v>0.03</v>
+        <v>1.4E-2</v>
       </c>
       <c r="F107" s="47">
-        <f>Patient!C6*IF(Patient!C2="Male",D107,E107)/60</f>
-        <v>2.8</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D107,E107)</f>
+        <v>77.135165332109054</v>
       </c>
       <c r="G107" s="16" t="s">
         <v>266</v>
@@ -15209,38 +15211,36 @@
         <v>344</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="24.75">
+    <row r="108" spans="1:16">
       <c r="A108" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>17</v>
+        <v>302</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D108" s="8">
-        <v>0.17499999999999999</v>
+        <v>0.03</v>
       </c>
       <c r="E108" s="8">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="F108" s="49">
-        <f>Patient!C7*IF(Patient!C2="Male",D108,E108)</f>
-        <v>964.18956665136318</v>
+        <v>0.03</v>
+      </c>
+      <c r="F108" s="47">
+        <f>Patient!C6*IF(Patient!C2="Male",D108,E108)/60</f>
+        <v>2.8</v>
       </c>
       <c r="G108" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="H108" s="25"/>
+      <c r="H108" s="16"/>
       <c r="I108" s="16" t="s">
         <v>1100</v>
       </c>
-      <c r="J108" s="4"/>
-      <c r="K108" s="44" t="s">
-        <v>390</v>
-      </c>
-      <c r="L108" s="53"/>
+      <c r="J108" s="48"/>
+      <c r="K108" s="24"/>
+      <c r="L108" s="46"/>
       <c r="M108" s="4" t="s">
         <v>343</v>
       </c>
@@ -15252,25 +15252,25 @@
         <v>344</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" ht="24.75">
       <c r="A109" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D109" s="8">
-        <v>1</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="E109" s="8">
-        <v>1</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F109" s="49">
-        <f>Patient!C6*IF(Patient!C2="Male",D109,E109)/60</f>
-        <v>93.333333333333329</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D109,E109)</f>
+        <v>964.18956665136318</v>
       </c>
       <c r="G109" s="16" t="s">
         <v>266</v>
@@ -15280,7 +15280,9 @@
         <v>1100</v>
       </c>
       <c r="J109" s="4"/>
-      <c r="K109" s="31"/>
+      <c r="K109" s="44" t="s">
+        <v>390</v>
+      </c>
       <c r="L109" s="53"/>
       <c r="M109" s="4" t="s">
         <v>343</v>
@@ -15290,6 +15292,47 @@
         <v>63</v>
       </c>
       <c r="P109" s="7" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16">
+      <c r="A110" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D110" s="8">
+        <v>1</v>
+      </c>
+      <c r="E110" s="8">
+        <v>1</v>
+      </c>
+      <c r="F110" s="49">
+        <f>Patient!C6*IF(Patient!C2="Male",D110,E110)/60</f>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="G110" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="H110" s="25"/>
+      <c r="I110" s="16" t="s">
+        <v>1100</v>
+      </c>
+      <c r="J110" s="4"/>
+      <c r="K110" s="31"/>
+      <c r="L110" s="53"/>
+      <c r="M110" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P110" s="7" t="s">
         <v>344</v>
       </c>
     </row>
@@ -17280,7 +17323,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="49">
-        <f>Cardiovascular!F47*60</f>
+        <f>Cardiovascular!F48*60</f>
         <v>1064</v>
       </c>
       <c r="G4" s="17" t="s">

</xml_diff>

<commit_message>
Added two new respiratory ratios.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561DA964-817E-48DB-849F-E31EF93A935E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90BC3F6-9178-4A61-B441-9A1276E6EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="5560" windowWidth="22560" windowHeight="10580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23490" yWindow="3615" windowWidth="27480" windowHeight="23535" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4715" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4728" uniqueCount="1112">
   <si>
     <t>Patient Inputs</t>
   </si>
@@ -3493,6 +3493,21 @@
   </si>
   <si>
     <t>Sex</t>
+  </si>
+  <si>
+    <t>VentilationPerfusionRatio</t>
+  </si>
+  <si>
+    <t>VQRatioOnline</t>
+  </si>
+  <si>
+    <t>PhysiologicDeadSpaceTidalVolumeRatio</t>
+  </si>
+  <si>
+    <t>[0.20, 0.40]</t>
+  </si>
+  <si>
+    <t>cala2004vd</t>
   </si>
 </sst>
 </file>
@@ -4455,13 +4470,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="1025" width="9.1796875" style="1" customWidth="1"/>
+    <col min="5" max="1025" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4699,22 +4714,22 @@
       <selection pane="topRight" activeCell="I2" activeCellId="1" sqref="I10:I11 I2:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" customWidth="1"/>
-    <col min="2" max="3" width="9.1796875" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" style="57" customWidth="1"/>
-    <col min="8" max="8" width="30.7265625" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.1796875" customWidth="1"/>
-    <col min="11" max="11" width="61.453125" style="95" customWidth="1"/>
-    <col min="12" max="12" width="52.453125" customWidth="1"/>
-    <col min="13" max="13" width="24.81640625" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" customWidth="1"/>
-    <col min="15" max="15" width="12.54296875" customWidth="1"/>
-    <col min="16" max="1026" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" customWidth="1"/>
+    <col min="11" max="11" width="61.42578125" style="95" customWidth="1"/>
+    <col min="12" max="12" width="52.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="1026" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="26.25" customHeight="1">
@@ -6923,7 +6938,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" ht="24.75">
       <c r="A55" s="29" t="s">
         <v>1031</v>
       </c>
@@ -7133,7 +7148,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="36.5">
+    <row r="61" spans="1:15" ht="36.75">
       <c r="A61" s="29" t="s">
         <v>1044</v>
       </c>
@@ -7160,7 +7175,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="60.5">
+    <row r="62" spans="1:15" ht="72.75">
       <c r="A62" s="29" t="s">
         <v>1046</v>
       </c>
@@ -7265,7 +7280,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="24">
+    <row r="65" spans="1:15" ht="24.75">
       <c r="A65" s="29" t="s">
         <v>1055</v>
       </c>
@@ -7302,7 +7317,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="36.5">
+    <row r="66" spans="1:15" ht="48.75">
       <c r="A66" s="29" t="s">
         <v>1059</v>
       </c>
@@ -7570,7 +7585,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" ht="24.75">
       <c r="A74" s="29" t="s">
         <v>1077</v>
       </c>
@@ -7774,7 +7789,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="24.5">
+    <row r="80" spans="1:15" ht="36.75">
       <c r="A80" s="29" t="s">
         <v>1084</v>
       </c>
@@ -7805,7 +7820,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="60.5">
+    <row r="81" spans="1:15" ht="72.75">
       <c r="A81" s="29" t="s">
         <v>1086</v>
       </c>
@@ -7910,7 +7925,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="24">
+    <row r="84" spans="1:15" ht="24.75">
       <c r="A84" s="29" t="s">
         <v>1089</v>
       </c>
@@ -7947,7 +7962,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="36.5">
+    <row r="85" spans="1:15" ht="48.75">
       <c r="A85" s="29" t="s">
         <v>1090</v>
       </c>
@@ -8227,27 +8242,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AML77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
       <selection pane="topRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" style="9" customWidth="1"/>
-    <col min="3" max="5" width="16.81640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="33.81640625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="9" customWidth="1"/>
+    <col min="3" max="5" width="16.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48" style="9" customWidth="1"/>
-    <col min="11" max="11" width="49.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="49.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="36" style="1" customWidth="1"/>
-    <col min="13" max="14" width="28.81640625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="9" customWidth="1"/>
-    <col min="16" max="1026" width="9.1796875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="28.85546875" style="9" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="9" customWidth="1"/>
+    <col min="16" max="1026" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="26.25" customHeight="1">
@@ -8991,7 +9006,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="42">
+    <row r="22" spans="1:15" ht="56.25">
       <c r="A22" s="29" t="s">
         <v>118</v>
       </c>
@@ -9026,7 +9041,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="21">
+    <row r="23" spans="1:15" ht="22.5">
       <c r="A23" s="29" t="s">
         <v>123</v>
       </c>
@@ -9312,7 +9327,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="36.5">
+    <row r="31" spans="1:15" ht="36.75">
       <c r="A31" s="11" t="s">
         <v>154</v>
       </c>
@@ -11049,23 +11064,23 @@
       <selection pane="topRight" activeCell="I38" sqref="I38:I110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="9" customWidth="1"/>
-    <col min="3" max="5" width="16.81640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="9" customWidth="1"/>
+    <col min="3" max="5" width="16.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="9" customWidth="1"/>
     <col min="7" max="7" width="29" style="43" customWidth="1"/>
     <col min="8" max="8" width="12" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.7265625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="36.26953125" style="44" customWidth="1"/>
-    <col min="12" max="12" width="29.54296875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="27.54296875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="28.81640625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" style="9" customWidth="1"/>
-    <col min="16" max="16" width="25.1796875" style="1" customWidth="1"/>
-    <col min="17" max="1026" width="9.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="36.28515625" style="44" customWidth="1"/>
+    <col min="12" max="12" width="29.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="9" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="9" customWidth="1"/>
+    <col min="16" max="16" width="25.140625" style="1" customWidth="1"/>
+    <col min="17" max="1026" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -11257,7 +11272,7 @@
       </c>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="48">
+    <row r="6" spans="1:16" ht="60">
       <c r="A6" s="45" t="s">
         <v>260</v>
       </c>
@@ -11749,7 +11764,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" ht="48">
+    <row r="21" spans="1:16" ht="60">
       <c r="A21" s="11" t="s">
         <v>299</v>
       </c>
@@ -11787,7 +11802,7 @@
       </c>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16" s="1" customFormat="1" ht="12">
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="24">
       <c r="A22" s="11" t="s">
         <v>300</v>
       </c>
@@ -12043,7 +12058,7 @@
       </c>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" ht="24">
       <c r="A30" s="11" t="s">
         <v>317</v>
       </c>
@@ -12352,7 +12367,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="24.5">
+    <row r="38" spans="1:16" ht="24.75">
       <c r="A38" s="11" t="s">
         <v>340</v>
       </c>
@@ -12395,7 +12410,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="36.5">
+    <row r="39" spans="1:16" ht="36.75">
       <c r="A39" s="11" t="s">
         <v>344</v>
       </c>
@@ -12804,7 +12819,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="24.5">
+    <row r="49" spans="1:16" ht="24.75">
       <c r="A49" s="11" t="s">
         <v>357</v>
       </c>
@@ -12888,7 +12903,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="24.5">
+    <row r="51" spans="1:16" ht="36.75">
       <c r="A51" s="11" t="s">
         <v>360</v>
       </c>
@@ -13080,7 +13095,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="48.5">
+    <row r="56" spans="1:16" ht="48.75">
       <c r="A56" s="11" t="s">
         <v>370</v>
       </c>
@@ -13160,7 +13175,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="24.5">
+    <row r="58" spans="1:16" ht="24.75">
       <c r="A58" s="11" t="s">
         <v>372</v>
       </c>
@@ -13199,7 +13214,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="24.5">
+    <row r="59" spans="1:16" ht="24.75">
       <c r="A59" s="11" t="s">
         <v>375</v>
       </c>
@@ -13238,7 +13253,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="24.5">
+    <row r="60" spans="1:16" ht="36.75">
       <c r="A60" s="11" t="s">
         <v>377</v>
       </c>
@@ -13322,7 +13337,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" ht="24.75">
       <c r="A62" s="11" t="s">
         <v>381</v>
       </c>
@@ -13406,7 +13421,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" ht="24.75">
       <c r="A64" s="11" t="s">
         <v>384</v>
       </c>
@@ -13490,7 +13505,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" ht="24.75">
       <c r="A66" s="11" t="s">
         <v>386</v>
       </c>
@@ -13574,7 +13589,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" ht="24.75">
       <c r="A68" s="11" t="s">
         <v>388</v>
       </c>
@@ -13830,7 +13845,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" ht="24.75">
       <c r="A74" s="11" t="s">
         <v>399</v>
       </c>
@@ -13990,7 +14005,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" ht="24.75">
       <c r="A78" s="11" t="s">
         <v>402</v>
       </c>
@@ -14114,7 +14129,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" ht="24.75">
       <c r="A81" s="11" t="s">
         <v>406</v>
       </c>
@@ -14198,7 +14213,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="36.5">
+    <row r="83" spans="1:16" ht="36.75">
       <c r="A83" s="11" t="s">
         <v>408</v>
       </c>
@@ -14238,7 +14253,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="24.5">
+    <row r="84" spans="1:16" ht="36.75">
       <c r="A84" s="11" t="s">
         <v>410</v>
       </c>
@@ -14322,7 +14337,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="48.5">
+    <row r="86" spans="1:16" ht="60.75">
       <c r="A86" s="11" t="s">
         <v>413</v>
       </c>
@@ -14396,7 +14411,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="36.5">
+    <row r="88" spans="1:16" ht="36.75">
       <c r="A88" s="11" t="s">
         <v>418</v>
       </c>
@@ -14506,7 +14521,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="24.5">
+    <row r="91" spans="1:16" ht="24.75">
       <c r="A91" s="11" t="s">
         <v>420</v>
       </c>
@@ -14545,7 +14560,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="24.5">
+    <row r="92" spans="1:16" ht="24.75">
       <c r="A92" s="11" t="s">
         <v>421</v>
       </c>
@@ -14584,7 +14599,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="24.5">
+    <row r="93" spans="1:16" ht="36.75">
       <c r="A93" s="11" t="s">
         <v>422</v>
       </c>
@@ -14668,7 +14683,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" ht="24.75">
       <c r="A95" s="11" t="s">
         <v>424</v>
       </c>
@@ -14752,7 +14767,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" ht="24.75">
       <c r="A97" s="11" t="s">
         <v>426</v>
       </c>
@@ -14836,7 +14851,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" ht="24.75">
       <c r="A99" s="11" t="s">
         <v>428</v>
       </c>
@@ -14920,7 +14935,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" ht="24.75">
       <c r="A101" s="11" t="s">
         <v>430</v>
       </c>
@@ -15252,7 +15267,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" ht="24.75">
       <c r="A109" s="11" t="s">
         <v>439</v>
       </c>
@@ -15353,21 +15368,21 @@
       <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="18.54296875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="54" customWidth="1"/>
-    <col min="7" max="8" width="17.26953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7265625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.453125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.26953125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="28.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="1" customWidth="1"/>
-    <col min="16" max="1026" width="9.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="1" customWidth="1"/>
+    <col min="3" max="5" width="18.5703125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="54" customWidth="1"/>
+    <col min="7" max="8" width="17.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="1" customWidth="1"/>
+    <col min="16" max="1026" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1026" ht="24">
@@ -15417,7 +15432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1026" s="106" customFormat="1" ht="60">
+    <row r="2" spans="1:1026" s="106" customFormat="1" ht="72">
       <c r="A2" s="55" t="s">
         <v>441</v>
       </c>
@@ -16478,21 +16493,21 @@
       <selection pane="topRight" activeCell="I11" activeCellId="5" sqref="I3 I4 I7 I8 I9 I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1"/>
-    <col min="7" max="9" width="23.54296875" customWidth="1"/>
-    <col min="10" max="10" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.1796875" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="57" customWidth="1"/>
-    <col min="14" max="14" width="28.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="1" customWidth="1"/>
-    <col min="16" max="1026" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="57" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="1" customWidth="1"/>
+    <col min="16" max="1026" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24">
@@ -16542,7 +16557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="24">
       <c r="A2" s="45" t="s">
         <v>447</v>
       </c>
@@ -16647,7 +16662,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="24">
       <c r="A6" s="45" t="s">
         <v>458</v>
       </c>
@@ -16829,7 +16844,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="24">
       <c r="A12" s="45" t="s">
         <v>474</v>
       </c>
@@ -16869,22 +16884,22 @@
       <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="1" customWidth="1"/>
     <col min="8" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="44.7265625" style="44" customWidth="1"/>
-    <col min="12" max="12" width="6.7265625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.26953125" style="54" customWidth="1"/>
-    <col min="14" max="14" width="28.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="1" customWidth="1"/>
-    <col min="16" max="1026" width="9.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="44.7109375" style="44" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="54" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="1" customWidth="1"/>
+    <col min="16" max="1026" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -16983,19 +16998,19 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.26953125" style="54" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="54" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="54" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="54" customWidth="1"/>
     <col min="3" max="3" width="20" style="54" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="54" customWidth="1"/>
-    <col min="7" max="9" width="17.26953125" style="54" customWidth="1"/>
-    <col min="10" max="11" width="14.7265625" style="54" customWidth="1"/>
-    <col min="12" max="13" width="9.1796875" style="54" customWidth="1"/>
-    <col min="14" max="14" width="28.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="1" customWidth="1"/>
-    <col min="16" max="1026" width="9.1796875" style="54" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="54" customWidth="1"/>
+    <col min="7" max="9" width="17.28515625" style="54" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" style="54" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="54" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="1" customWidth="1"/>
+    <col min="16" max="1026" width="9.140625" style="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24">
@@ -17174,23 +17189,23 @@
       <selection pane="topRight" activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="19.7265625" style="64" customWidth="1"/>
-    <col min="7" max="7" width="24.54296875" style="64" customWidth="1"/>
-    <col min="8" max="8" width="28.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="64" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="64" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="40" style="1" customWidth="1"/>
-    <col min="11" max="11" width="41.81640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="51.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="28.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="1" customWidth="1"/>
-    <col min="16" max="1026" width="9.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="41.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="51.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="1" customWidth="1"/>
+    <col min="16" max="1026" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -17384,7 +17399,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="24">
       <c r="A6" s="11" t="s">
         <v>494</v>
       </c>
@@ -17755,7 +17770,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" ht="24">
       <c r="A17" s="74" t="s">
         <v>520</v>
       </c>
@@ -18008,7 +18023,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" ht="24">
       <c r="A24" s="45" t="s">
         <v>535</v>
       </c>
@@ -18284,7 +18299,7 @@
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" ht="24">
       <c r="A32" s="45" t="s">
         <v>550</v>
       </c>
@@ -18488,7 +18503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" ht="24">
       <c r="A38" s="74" t="s">
         <v>556</v>
       </c>
@@ -18741,7 +18756,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" ht="24">
       <c r="A45" s="45" t="s">
         <v>563</v>
       </c>
@@ -19015,7 +19030,7 @@
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" ht="24">
       <c r="A53" s="45" t="s">
         <v>571</v>
       </c>
@@ -19196,7 +19211,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="36">
+    <row r="58" spans="1:15" ht="48">
       <c r="A58" s="11" t="s">
         <v>579</v>
       </c>
@@ -19231,7 +19246,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="36">
+    <row r="59" spans="1:15" ht="48">
       <c r="A59" s="11" t="s">
         <v>582</v>
       </c>
@@ -19266,7 +19281,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="36">
+    <row r="60" spans="1:15" ht="48">
       <c r="A60" s="11" t="s">
         <v>583</v>
       </c>
@@ -19301,7 +19316,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="36">
+    <row r="61" spans="1:15" ht="48">
       <c r="A61" s="11" t="s">
         <v>586</v>
       </c>
@@ -19336,7 +19351,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="36">
+    <row r="62" spans="1:15" ht="48">
       <c r="A62" s="11" t="s">
         <v>587</v>
       </c>
@@ -19371,7 +19386,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="36">
+    <row r="63" spans="1:15" ht="48">
       <c r="A63" s="11" t="s">
         <v>588</v>
       </c>
@@ -19406,7 +19421,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="36">
+    <row r="64" spans="1:15" ht="48">
       <c r="A64" s="11" t="s">
         <v>589</v>
       </c>
@@ -19441,7 +19456,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="36">
+    <row r="65" spans="1:15" ht="48">
       <c r="A65" s="11" t="s">
         <v>590</v>
       </c>
@@ -19513,7 +19528,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="24">
+    <row r="67" spans="1:15" ht="36">
       <c r="A67" s="11" t="s">
         <v>595</v>
       </c>
@@ -19550,7 +19565,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="36">
+    <row r="68" spans="1:15" ht="48">
       <c r="A68" s="11" t="s">
         <v>596</v>
       </c>
@@ -19585,7 +19600,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="36">
+    <row r="69" spans="1:15" ht="48">
       <c r="A69" s="11" t="s">
         <v>597</v>
       </c>
@@ -19620,7 +19635,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="36">
+    <row r="70" spans="1:15" ht="48">
       <c r="A70" s="11" t="s">
         <v>598</v>
       </c>
@@ -19655,7 +19670,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="36">
+    <row r="71" spans="1:15" ht="48">
       <c r="A71" s="11" t="s">
         <v>599</v>
       </c>
@@ -19690,7 +19705,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="36">
+    <row r="72" spans="1:15" ht="48">
       <c r="A72" s="11" t="s">
         <v>600</v>
       </c>
@@ -19725,7 +19740,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="36">
+    <row r="73" spans="1:15" ht="48">
       <c r="A73" s="11" t="s">
         <v>601</v>
       </c>
@@ -19760,7 +19775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="36">
+    <row r="74" spans="1:15" ht="48">
       <c r="A74" s="11" t="s">
         <v>602</v>
       </c>
@@ -19795,7 +19810,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="36">
+    <row r="75" spans="1:15" ht="48">
       <c r="A75" s="11" t="s">
         <v>603</v>
       </c>
@@ -21057,7 +21072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="24">
+    <row r="109" spans="1:15" ht="36">
       <c r="A109" s="11" t="s">
         <v>671</v>
       </c>
@@ -21166,7 +21181,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="24">
+    <row r="112" spans="1:15" ht="36">
       <c r="A112" s="11" t="s">
         <v>682</v>
       </c>
@@ -22778,29 +22793,29 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:O103"/>
+  <dimension ref="A1:O105"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I72" activeCellId="4" sqref="I96:I103 I90:I93 I86:I87 I80:I81 I72:I75"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="9" customWidth="1"/>
     <col min="3" max="5" width="30" style="9" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="9" customWidth="1"/>
     <col min="7" max="7" width="20" style="43" customWidth="1"/>
-    <col min="8" max="8" width="27.26953125" style="43" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="43" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="43" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" style="43" customWidth="1"/>
-    <col min="11" max="11" width="37.54296875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="37.5703125" style="9" customWidth="1"/>
     <col min="12" max="12" width="52" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24.7265625" style="57" customWidth="1"/>
-    <col min="14" max="14" width="28.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.453125" style="1" customWidth="1"/>
-    <col min="16" max="1026" width="9.1796875" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" style="57" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="1" customWidth="1"/>
+    <col min="16" max="1026" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -22883,7 +22898,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="36">
+    <row r="3" spans="1:15" ht="48">
       <c r="A3" s="11" t="s">
         <v>774</v>
       </c>
@@ -23727,7 +23742,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="48">
+    <row r="29" spans="1:15" ht="60">
       <c r="A29" s="11" t="s">
         <v>828</v>
       </c>
@@ -23985,32 +24000,28 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="96">
+    <row r="37" spans="1:15">
       <c r="A37" s="11" t="s">
-        <v>841</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>770</v>
-      </c>
+        <v>1109</v>
+      </c>
+      <c r="B37" s="17"/>
       <c r="C37" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="5">
-        <v>0</v>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="48" t="s">
+        <v>1110</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>95</v>
+        <v>1111</v>
       </c>
       <c r="H37" s="16"/>
       <c r="I37" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J37" s="16"/>
-      <c r="K37" s="25" t="s">
-        <v>842</v>
-      </c>
+      <c r="K37" s="25"/>
       <c r="L37" s="79"/>
       <c r="M37" s="60" t="s">
         <v>773</v>
@@ -24020,35 +24031,33 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="96">
+    <row r="38" spans="1:15" ht="120">
       <c r="A38" s="11" t="s">
-        <v>843</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>788</v>
+        <v>841</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>770</v>
       </c>
       <c r="C38" s="48" t="s">
         <v>43</v>
       </c>
       <c r="D38" s="48"/>
       <c r="E38" s="48"/>
-      <c r="F38" s="16" t="s">
-        <v>844</v>
+      <c r="F38" s="5">
+        <v>0</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H38" s="16" t="s">
-        <v>845</v>
-      </c>
+      <c r="H38" s="16"/>
       <c r="I38" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J38" s="16"/>
       <c r="K38" s="25" t="s">
-        <v>846</v>
-      </c>
-      <c r="L38" s="83"/>
+        <v>842</v>
+      </c>
+      <c r="L38" s="79"/>
       <c r="M38" s="60" t="s">
         <v>773</v>
       </c>
@@ -24057,12 +24066,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" ht="96">
       <c r="A39" s="11" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>848</v>
+        <v>788</v>
       </c>
       <c r="C39" s="48" t="s">
         <v>43</v>
@@ -24070,7 +24079,7 @@
       <c r="D39" s="48"/>
       <c r="E39" s="48"/>
       <c r="F39" s="16" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>95</v>
@@ -24083,7 +24092,7 @@
       </c>
       <c r="J39" s="16"/>
       <c r="K39" s="25" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="L39" s="83"/>
       <c r="M39" s="60" t="s">
@@ -24094,35 +24103,35 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="24">
+    <row r="40" spans="1:15">
       <c r="A40" s="11" t="s">
-        <v>851</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>852</v>
+        <v>847</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>848</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>780</v>
+        <v>43</v>
       </c>
       <c r="D40" s="48"/>
       <c r="E40" s="48"/>
-      <c r="F40" s="16">
-        <v>3.5</v>
+      <c r="F40" s="16" t="s">
+        <v>849</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H40" s="8" t="s">
-        <v>807</v>
+      <c r="H40" s="16" t="s">
+        <v>845</v>
       </c>
       <c r="I40" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="25" t="s">
-        <v>853</v>
-      </c>
-      <c r="L40" s="53"/>
+        <v>850</v>
+      </c>
+      <c r="L40" s="83"/>
       <c r="M40" s="60" t="s">
         <v>773</v>
       </c>
@@ -24131,23 +24140,35 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
-      <c r="A41" s="45" t="s">
-        <v>854</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>791</v>
-      </c>
-      <c r="C41" s="48"/>
+    <row r="41" spans="1:15" ht="24">
+      <c r="A41" s="11" t="s">
+        <v>851</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>780</v>
+      </c>
       <c r="D41" s="48"/>
       <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
+      <c r="F41" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>807</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>1099</v>
+      </c>
       <c r="J41" s="16"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="79"/>
+      <c r="K41" s="25" t="s">
+        <v>853</v>
+      </c>
+      <c r="L41" s="53"/>
       <c r="M41" s="60" t="s">
         <v>773</v>
       </c>
@@ -24158,7 +24179,7 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="45" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>791</v>
@@ -24181,33 +24202,23 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="36">
-      <c r="A43" s="11" t="s">
-        <v>856</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="C43" s="48" t="s">
-        <v>43</v>
-      </c>
+    <row r="43" spans="1:15">
+      <c r="A43" s="45" t="s">
+        <v>855</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>791</v>
+      </c>
+      <c r="C43" s="48"/>
       <c r="D43" s="48"/>
       <c r="E43" s="48"/>
-      <c r="F43" s="17" t="s">
-        <v>857</v>
-      </c>
-      <c r="G43" s="87" t="s">
-        <v>858</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>859</v>
-      </c>
-      <c r="I43" s="16" t="s">
-        <v>1099</v>
-      </c>
+      <c r="F43" s="48"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
       <c r="J43" s="16"/>
       <c r="K43" s="25"/>
-      <c r="L43" s="88"/>
+      <c r="L43" s="79"/>
       <c r="M43" s="60" t="s">
         <v>773</v>
       </c>
@@ -24216,27 +24227,33 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="45" t="s">
-        <v>860</v>
-      </c>
-      <c r="B44" s="16"/>
+    <row r="44" spans="1:15" ht="36">
+      <c r="A44" s="11" t="s">
+        <v>856</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>281</v>
+      </c>
       <c r="C44" s="48" t="s">
         <v>43</v>
       </c>
       <c r="D44" s="48"/>
       <c r="E44" s="48"/>
-      <c r="F44" s="48">
-        <v>0</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>861</v>
-      </c>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
+      <c r="F44" s="17" t="s">
+        <v>857</v>
+      </c>
+      <c r="G44" s="87" t="s">
+        <v>858</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>859</v>
+      </c>
+      <c r="I44" s="16" t="s">
+        <v>1099</v>
+      </c>
       <c r="J44" s="16"/>
       <c r="K44" s="25"/>
-      <c r="L44" s="79"/>
+      <c r="L44" s="88"/>
       <c r="M44" s="60" t="s">
         <v>773</v>
       </c>
@@ -24247,19 +24264,25 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="45" t="s">
-        <v>862</v>
-      </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="48"/>
+        <v>860</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="48" t="s">
+        <v>43</v>
+      </c>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
+      <c r="F45" s="48">
+        <v>0</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>861</v>
+      </c>
+      <c r="H45" s="16"/>
       <c r="I45" s="16"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="79"/>
       <c r="M45" s="60" t="s">
         <v>773</v>
       </c>
@@ -24269,28 +24292,18 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="11" t="s">
-        <v>863</v>
+      <c r="A46" s="45" t="s">
+        <v>862</v>
       </c>
       <c r="B46" s="14"/>
-      <c r="C46" s="48" t="s">
-        <v>43</v>
-      </c>
+      <c r="C46" s="48"/>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
-      <c r="F46" s="48">
-        <v>4.62</v>
-      </c>
-      <c r="G46" s="48" t="s">
-        <v>14</v>
-      </c>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
       <c r="H46" s="48"/>
-      <c r="I46" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J46" s="48" t="s">
-        <v>864</v>
-      </c>
+      <c r="I46" s="16"/>
+      <c r="J46" s="48"/>
       <c r="K46" s="48"/>
       <c r="L46" s="48"/>
       <c r="M46" s="60" t="s">
@@ -24301,33 +24314,31 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="24">
+    <row r="47" spans="1:15">
       <c r="A47" s="11" t="s">
-        <v>865</v>
-      </c>
-      <c r="B47" s="16"/>
+        <v>863</v>
+      </c>
+      <c r="B47" s="14"/>
       <c r="C47" s="48" t="s">
         <v>43</v>
       </c>
       <c r="D47" s="48"/>
       <c r="E47" s="48"/>
-      <c r="F47" s="16">
-        <v>0.23</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>807</v>
-      </c>
+      <c r="F47" s="48">
+        <v>4.62</v>
+      </c>
+      <c r="G47" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="48"/>
       <c r="I47" s="16" t="s">
         <v>1099</v>
       </c>
-      <c r="J47" s="16"/>
-      <c r="K47" s="25" t="s">
-        <v>866</v>
-      </c>
-      <c r="L47" s="80"/>
+      <c r="J47" s="48" t="s">
+        <v>864</v>
+      </c>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
       <c r="M47" s="60" t="s">
         <v>773</v>
       </c>
@@ -24336,20 +24347,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" ht="24">
       <c r="A48" s="11" t="s">
-        <v>867</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>16</v>
-      </c>
+        <v>865</v>
+      </c>
+      <c r="B48" s="16"/>
       <c r="C48" s="48" t="s">
-        <v>780</v>
+        <v>43</v>
       </c>
       <c r="D48" s="48"/>
       <c r="E48" s="48"/>
-      <c r="F48" s="48">
-        <v>7</v>
+      <c r="F48" s="16">
+        <v>0.23</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>95</v>
@@ -24361,22 +24370,24 @@
         <v>1099</v>
       </c>
       <c r="J48" s="16"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="79"/>
+      <c r="K48" s="25" t="s">
+        <v>866</v>
+      </c>
+      <c r="L48" s="80"/>
       <c r="M48" s="60" t="s">
         <v>773</v>
       </c>
       <c r="N48" s="4"/>
       <c r="O48" s="4" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="11" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>869</v>
+        <v>16</v>
       </c>
       <c r="C49" s="48" t="s">
         <v>780</v>
@@ -24384,7 +24395,7 @@
       <c r="D49" s="48"/>
       <c r="E49" s="48"/>
       <c r="F49" s="48">
-        <v>0.08</v>
+        <v>7</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>95</v>
@@ -24396,21 +24407,19 @@
         <v>1099</v>
       </c>
       <c r="J49" s="16"/>
-      <c r="K49" s="25" t="s">
-        <v>870</v>
-      </c>
+      <c r="K49" s="25"/>
       <c r="L49" s="79"/>
       <c r="M49" s="60" t="s">
         <v>773</v>
       </c>
       <c r="N49" s="4"/>
       <c r="O49" s="4" t="s">
-        <v>92</v>
+        <v>778</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="24">
       <c r="A50" s="11" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>869</v>
@@ -24421,8 +24430,7 @@
       <c r="D50" s="48"/>
       <c r="E50" s="48"/>
       <c r="F50" s="48">
-        <f>0.002*12</f>
-        <v>2.4E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>95</v>
@@ -24435,9 +24443,9 @@
       </c>
       <c r="J50" s="16"/>
       <c r="K50" s="25" t="s">
-        <v>872</v>
-      </c>
-      <c r="L50" s="53"/>
+        <v>870</v>
+      </c>
+      <c r="L50" s="79"/>
       <c r="M50" s="60" t="s">
         <v>773</v>
       </c>
@@ -24446,20 +24454,21 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="36">
+    <row r="51" spans="1:15" ht="24">
       <c r="A51" s="11" t="s">
-        <v>873</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>852</v>
+        <v>871</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>869</v>
       </c>
       <c r="C51" s="48" t="s">
         <v>780</v>
       </c>
       <c r="D51" s="48"/>
       <c r="E51" s="48"/>
-      <c r="F51" s="16">
-        <v>3.3500000000000002E-2</v>
+      <c r="F51" s="48">
+        <f>0.002*12</f>
+        <v>2.4E-2</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>95</v>
@@ -24472,7 +24481,7 @@
       </c>
       <c r="J51" s="16"/>
       <c r="K51" s="25" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="L51" s="53"/>
       <c r="M51" s="60" t="s">
@@ -24483,23 +24492,35 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
-      <c r="A52" s="45" t="s">
-        <v>875</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>813</v>
-      </c>
-      <c r="C52" s="48"/>
+    <row r="52" spans="1:15" ht="36">
+      <c r="A52" s="11" t="s">
+        <v>873</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C52" s="48" t="s">
+        <v>780</v>
+      </c>
       <c r="D52" s="48"/>
       <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
+      <c r="F52" s="16">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>807</v>
+      </c>
+      <c r="I52" s="16" t="s">
+        <v>1099</v>
+      </c>
       <c r="J52" s="16"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="79"/>
+      <c r="K52" s="25" t="s">
+        <v>874</v>
+      </c>
+      <c r="L52" s="53"/>
       <c r="M52" s="60" t="s">
         <v>773</v>
       </c>
@@ -24508,35 +24529,22 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="45.75" customHeight="1">
-      <c r="A53" s="11" t="s">
-        <v>876</v>
+    <row r="53" spans="1:15">
+      <c r="A53" s="45" t="s">
+        <v>875</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>869</v>
-      </c>
-      <c r="C53" s="48" t="s">
-        <v>780</v>
-      </c>
+        <v>813</v>
+      </c>
+      <c r="C53" s="48"/>
       <c r="D53" s="48"/>
       <c r="E53" s="48"/>
-      <c r="F53" s="48">
-        <f>0.007*12</f>
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>807</v>
-      </c>
-      <c r="I53" s="16" t="s">
-        <v>1099</v>
-      </c>
+      <c r="F53" s="48"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
       <c r="J53" s="16"/>
-      <c r="K53" s="25" t="s">
-        <v>877</v>
-      </c>
+      <c r="K53" s="25"/>
       <c r="L53" s="79"/>
       <c r="M53" s="60" t="s">
         <v>773</v>
@@ -24546,22 +24554,35 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
-      <c r="A54" s="45" t="s">
-        <v>878</v>
+    <row r="54" spans="1:15" ht="45.75" customHeight="1">
+      <c r="A54" s="11" t="s">
+        <v>876</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>791</v>
-      </c>
-      <c r="C54" s="48"/>
+        <v>869</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>780</v>
+      </c>
       <c r="D54" s="48"/>
       <c r="E54" s="48"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="16"/>
+      <c r="F54" s="48">
+        <f>0.007*12</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>807</v>
+      </c>
+      <c r="I54" s="16" t="s">
+        <v>1099</v>
+      </c>
       <c r="J54" s="16"/>
-      <c r="K54" s="25"/>
+      <c r="K54" s="25" t="s">
+        <v>877</v>
+      </c>
       <c r="L54" s="79"/>
       <c r="M54" s="60" t="s">
         <v>773</v>
@@ -24572,29 +24593,19 @@
       </c>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="11" t="s">
-        <v>879</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>770</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="48">
-        <v>-1</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>829</v>
-      </c>
-      <c r="I55" s="16" t="s">
-        <v>1100</v>
-      </c>
+      <c r="A55" s="45" t="s">
+        <v>878</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>791</v>
+      </c>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
       <c r="J55" s="16"/>
       <c r="K55" s="25"/>
       <c r="L55" s="79"/>
@@ -24614,12 +24625,12 @@
         <v>770</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="19"/>
       <c r="F56" s="48">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>95</v>
@@ -24643,24 +24654,24 @@
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="11" t="s">
-        <v>880</v>
-      </c>
-      <c r="B57" s="16" t="s">
+        <v>879</v>
+      </c>
+      <c r="B57" s="17" t="s">
         <v>770</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19"/>
       <c r="F57" s="48">
-        <v>5.2</v>
+        <v>1</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>881</v>
+        <v>829</v>
       </c>
       <c r="I57" s="16" t="s">
         <v>1100</v>
@@ -24684,12 +24695,12 @@
         <v>770</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D58" s="19"/>
       <c r="E58" s="19"/>
       <c r="F58" s="48">
-        <v>7.2</v>
+        <v>5.2</v>
       </c>
       <c r="G58" s="16" t="s">
         <v>14</v>
@@ -24713,32 +24724,30 @@
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="11" t="s">
-        <v>882</v>
-      </c>
-      <c r="B59" s="17" t="s">
+        <v>880</v>
+      </c>
+      <c r="B59" s="16" t="s">
         <v>770</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D59" s="19"/>
       <c r="E59" s="19"/>
-      <c r="F59" s="85">
-        <v>-8</v>
+      <c r="F59" s="48">
+        <v>7.2</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H59" s="8" t="s">
-        <v>823</v>
+        <v>14</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>881</v>
       </c>
       <c r="I59" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J59" s="16"/>
-      <c r="K59" s="25" t="s">
-        <v>883</v>
-      </c>
+      <c r="K59" s="25"/>
       <c r="L59" s="79"/>
       <c r="M59" s="60" t="s">
         <v>773</v>
@@ -24748,7 +24757,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" ht="24">
       <c r="A60" s="11" t="s">
         <v>882</v>
       </c>
@@ -24756,12 +24765,12 @@
         <v>770</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
       <c r="F60" s="85">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>95</v>
@@ -24785,31 +24794,33 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" ht="24">
       <c r="A61" s="11" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>770</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
-      <c r="F61" s="86">
-        <v>-5.4</v>
+      <c r="F61" s="85">
+        <v>-5</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H61" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>823</v>
+      </c>
       <c r="I61" s="16" t="s">
         <v>1100</v>
       </c>
       <c r="J61" s="16"/>
       <c r="K61" s="25" t="s">
-        <v>825</v>
+        <v>883</v>
       </c>
       <c r="L61" s="79"/>
       <c r="M61" s="60" t="s">
@@ -24828,12 +24839,12 @@
         <v>770</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
       <c r="F62" s="86">
-        <v>0</v>
+        <v>-5.4</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>14</v>
@@ -24843,7 +24854,9 @@
         <v>1100</v>
       </c>
       <c r="J62" s="16"/>
-      <c r="K62" s="25"/>
+      <c r="K62" s="25" t="s">
+        <v>825</v>
+      </c>
       <c r="L62" s="79"/>
       <c r="M62" s="60" t="s">
         <v>773</v>
@@ -24855,25 +24868,23 @@
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="11" t="s">
-        <v>885</v>
-      </c>
-      <c r="B63" s="16" t="s">
+        <v>884</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>770</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>
-      <c r="F63" s="48">
-        <v>5</v>
+      <c r="F63" s="86">
+        <v>0</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H63" s="16" t="s">
-        <v>881</v>
-      </c>
+      <c r="H63" s="8"/>
       <c r="I63" s="16" t="s">
         <v>1100</v>
       </c>
@@ -24896,12 +24907,12 @@
         <v>770</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D64" s="19"/>
       <c r="E64" s="19"/>
       <c r="F64" s="48">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="G64" s="16" t="s">
         <v>14</v>
@@ -24923,33 +24934,31 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="24">
+    <row r="65" spans="1:15">
       <c r="A65" s="11" t="s">
-        <v>886</v>
-      </c>
-      <c r="B65" s="17" t="s">
+        <v>885</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>770</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D65" s="19"/>
       <c r="E65" s="19"/>
       <c r="F65" s="48">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>771</v>
+        <v>14</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="I65" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J65" s="16" t="s">
-        <v>888</v>
-      </c>
+        <v>1100</v>
+      </c>
+      <c r="J65" s="16"/>
       <c r="K65" s="25"/>
       <c r="L65" s="79"/>
       <c r="M65" s="60" t="s">
@@ -24968,7 +24977,7 @@
         <v>770</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D66" s="19"/>
       <c r="E66" s="19"/>
@@ -24997,31 +25006,33 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" ht="24">
       <c r="A67" s="11" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="B67" s="17" t="s">
         <v>770</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
       <c r="F67" s="48">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>95</v>
+        <v>771</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>829</v>
+        <v>887</v>
       </c>
       <c r="I67" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J67" s="16"/>
+        <v>1099</v>
+      </c>
+      <c r="J67" s="16" t="s">
+        <v>888</v>
+      </c>
       <c r="K67" s="25"/>
       <c r="L67" s="79"/>
       <c r="M67" s="60" t="s">
@@ -25040,12 +25051,12 @@
         <v>770</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D68" s="19"/>
       <c r="E68" s="19"/>
       <c r="F68" s="48">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>95</v>
@@ -25068,157 +25079,147 @@
       </c>
     </row>
     <row r="69" spans="1:15">
-      <c r="A69" s="27" t="s">
-        <v>339</v>
-      </c>
-      <c r="B69" s="2" t="s">
+      <c r="A69" s="11" t="s">
+        <v>889</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>770</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="48">
         <v>1</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="G69" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="H69" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>1098</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L69" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="M69" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="N69" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="O69" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="25.5" customHeight="1">
+      <c r="G69" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H69" s="16" t="s">
+        <v>829</v>
+      </c>
+      <c r="I69" s="16" t="s">
+        <v>1100</v>
+      </c>
+      <c r="J69" s="16"/>
+      <c r="K69" s="25"/>
+      <c r="L69" s="79"/>
+      <c r="M69" s="60" t="s">
+        <v>773</v>
+      </c>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" s="11" t="s">
-        <v>890</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>368</v>
+        <v>1107</v>
+      </c>
+      <c r="B70" s="17"/>
+      <c r="C70" s="48" t="s">
+        <v>43</v>
       </c>
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
-      <c r="F70" s="89" t="s">
-        <v>891</v>
+      <c r="F70" s="48">
+        <v>0.8</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>892</v>
-      </c>
+        <v>1108</v>
+      </c>
+      <c r="H70" s="16"/>
       <c r="I70" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J70" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K70" s="25" t="s">
-        <v>894</v>
-      </c>
+        <v>1099</v>
+      </c>
+      <c r="J70" s="16"/>
+      <c r="K70" s="25"/>
       <c r="L70" s="79"/>
       <c r="M70" s="60" t="s">
-        <v>895</v>
+        <v>773</v>
       </c>
       <c r="N70" s="4"/>
       <c r="O70" s="4" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" ht="24">
-      <c r="A71" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="A71" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G71" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="H71" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L71" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M71" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N71" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O71" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="25.5" customHeight="1">
+      <c r="A72" s="11" t="s">
         <v>890</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B72" s="16" t="s">
         <v>770</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="89" t="s">
-        <v>897</v>
-      </c>
-      <c r="G71" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>892</v>
-      </c>
-      <c r="I71" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J71" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K71" s="25" t="s">
-        <v>894</v>
-      </c>
-      <c r="L71" s="79"/>
-      <c r="M71" s="60" t="s">
-        <v>895</v>
-      </c>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="24">
-      <c r="A72" s="11" t="s">
-        <v>898</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>190</v>
       </c>
       <c r="C72" s="19" t="s">
         <v>368</v>
       </c>
       <c r="D72" s="19"/>
       <c r="E72" s="19"/>
-      <c r="F72" s="16" t="s">
-        <v>899</v>
-      </c>
-      <c r="G72" s="87" t="s">
-        <v>900</v>
+      <c r="F72" s="89" t="s">
+        <v>891</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J72" s="16"/>
+        <v>1100</v>
+      </c>
+      <c r="J72" s="16" t="s">
+        <v>893</v>
+      </c>
       <c r="K72" s="25" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="L72" s="79"/>
       <c r="M72" s="60" t="s">
@@ -25226,47 +25227,51 @@
       </c>
       <c r="N72" s="4"/>
       <c r="O72" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="24">
       <c r="A73" s="11" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>190</v>
+        <v>770</v>
       </c>
       <c r="C73" s="19" t="s">
         <v>365</v>
       </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
-      <c r="F73" s="90">
-        <v>120</v>
-      </c>
-      <c r="G73" s="48" t="s">
-        <v>95</v>
+      <c r="F73" s="89" t="s">
+        <v>897</v>
+      </c>
+      <c r="G73" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>903</v>
+        <v>892</v>
       </c>
       <c r="I73" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J73" s="16"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="53"/>
+        <v>1100</v>
+      </c>
+      <c r="J73" s="16" t="s">
+        <v>893</v>
+      </c>
+      <c r="K73" s="25" t="s">
+        <v>894</v>
+      </c>
+      <c r="L73" s="79"/>
       <c r="M73" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N73" s="4"/>
       <c r="O73" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="24">
       <c r="A74" s="11" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>190</v>
@@ -25276,32 +25281,34 @@
       </c>
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
-      <c r="F74" s="48" t="s">
-        <v>905</v>
-      </c>
-      <c r="G74" s="48" t="s">
-        <v>95</v>
+      <c r="F74" s="16" t="s">
+        <v>899</v>
+      </c>
+      <c r="G74" s="87" t="s">
+        <v>900</v>
       </c>
       <c r="H74" s="16" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="I74" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
+      <c r="K74" s="25" t="s">
+        <v>902</v>
+      </c>
       <c r="L74" s="79"/>
       <c r="M74" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N74" s="4"/>
       <c r="O74" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="30" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" s="11" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B75" s="16" t="s">
         <v>190</v>
@@ -25311,112 +25318,104 @@
       </c>
       <c r="D75" s="19"/>
       <c r="E75" s="19"/>
-      <c r="F75" s="16" t="s">
-        <v>907</v>
-      </c>
-      <c r="G75" s="87" t="s">
-        <v>900</v>
+      <c r="F75" s="90">
+        <v>120</v>
+      </c>
+      <c r="G75" s="48" t="s">
+        <v>95</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="I75" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J75" s="16"/>
-      <c r="K75" s="25" t="s">
-        <v>908</v>
-      </c>
-      <c r="L75" s="79"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="53"/>
       <c r="M75" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N75" s="4"/>
       <c r="O75" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="24">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="11" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>770</v>
+        <v>190</v>
       </c>
       <c r="C76" s="19" t="s">
         <v>368</v>
       </c>
       <c r="D76" s="19"/>
       <c r="E76" s="19"/>
-      <c r="F76" s="48">
-        <v>1028.2</v>
-      </c>
-      <c r="G76" s="16" t="s">
-        <v>14</v>
+      <c r="F76" s="48" t="s">
+        <v>905</v>
+      </c>
+      <c r="G76" s="48" t="s">
+        <v>95</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>881</v>
+        <v>906</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J76" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K76" s="25" t="s">
-        <v>910</v>
-      </c>
-      <c r="L76" s="53"/>
+        <v>1099</v>
+      </c>
+      <c r="J76" s="16"/>
+      <c r="K76" s="16"/>
+      <c r="L76" s="79"/>
       <c r="M76" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N76" s="4"/>
       <c r="O76" s="4" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="30" customHeight="1">
       <c r="A77" s="11" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>770</v>
+        <v>190</v>
       </c>
       <c r="C77" s="19" t="s">
         <v>365</v>
       </c>
       <c r="D77" s="19"/>
       <c r="E77" s="19"/>
-      <c r="F77" s="48">
-        <v>1025.7</v>
-      </c>
-      <c r="G77" s="16" t="s">
-        <v>14</v>
+      <c r="F77" s="16" t="s">
+        <v>907</v>
+      </c>
+      <c r="G77" s="87" t="s">
+        <v>900</v>
       </c>
       <c r="H77" s="16" t="s">
-        <v>881</v>
+        <v>901</v>
       </c>
       <c r="I77" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J77" s="16" t="s">
-        <v>893</v>
-      </c>
+        <v>1099</v>
+      </c>
+      <c r="J77" s="16"/>
       <c r="K77" s="25" t="s">
-        <v>910</v>
-      </c>
-      <c r="L77" s="53"/>
+        <v>908</v>
+      </c>
+      <c r="L77" s="79"/>
       <c r="M77" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N77" s="4"/>
       <c r="O77" s="4" t="s">
-        <v>896</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="24">
       <c r="A78" s="11" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B78" s="16" t="s">
         <v>770</v>
@@ -25455,7 +25454,7 @@
     </row>
     <row r="79" spans="1:15" ht="24">
       <c r="A79" s="11" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B79" s="16" t="s">
         <v>770</v>
@@ -25492,161 +25491,161 @@
         <v>896</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" ht="24">
       <c r="A80" s="11" t="s">
-        <v>912</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>852</v>
-      </c>
-      <c r="C80" s="48" t="s">
-        <v>913</v>
-      </c>
-      <c r="D80" s="48"/>
-      <c r="E80" s="48"/>
-      <c r="F80" s="91">
-        <v>0.03</v>
-      </c>
-      <c r="G80" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>807</v>
+        <v>911</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>770</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="48">
+        <v>1028.2</v>
+      </c>
+      <c r="G80" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="16" t="s">
+        <v>881</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J80" s="16"/>
-      <c r="K80" s="4" t="s">
-        <v>914</v>
-      </c>
-      <c r="L80" s="92"/>
+        <v>1100</v>
+      </c>
+      <c r="J80" s="16" t="s">
+        <v>893</v>
+      </c>
+      <c r="K80" s="25" t="s">
+        <v>910</v>
+      </c>
+      <c r="L80" s="53"/>
       <c r="M80" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N80" s="4"/>
       <c r="O80" s="4" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="24">
       <c r="A81" s="11" t="s">
-        <v>912</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>852</v>
-      </c>
-      <c r="C81" s="48" t="s">
-        <v>915</v>
-      </c>
-      <c r="D81" s="48"/>
-      <c r="E81" s="48"/>
-      <c r="F81" s="4">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="G81" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>807</v>
+        <v>911</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>770</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="48">
+        <v>1025.7</v>
+      </c>
+      <c r="G81" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="16" t="s">
+        <v>881</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J81" s="16"/>
-      <c r="K81" s="4" t="s">
-        <v>916</v>
-      </c>
-      <c r="L81" s="92"/>
+        <v>1100</v>
+      </c>
+      <c r="J81" s="16" t="s">
+        <v>893</v>
+      </c>
+      <c r="K81" s="25" t="s">
+        <v>910</v>
+      </c>
+      <c r="L81" s="53"/>
       <c r="M81" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N81" s="4"/>
       <c r="O81" s="4" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="24">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" s="11" t="s">
-        <v>917</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>368</v>
-      </c>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="16" t="s">
-        <v>918</v>
-      </c>
-      <c r="G82" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="H82" s="16" t="s">
-        <v>920</v>
+        <v>912</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C82" s="48" t="s">
+        <v>913</v>
+      </c>
+      <c r="D82" s="48"/>
+      <c r="E82" s="48"/>
+      <c r="F82" s="91">
+        <v>0.03</v>
+      </c>
+      <c r="G82" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I82" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J82" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K82" s="25" t="s">
-        <v>921</v>
-      </c>
-      <c r="L82" s="79"/>
+        <v>1099</v>
+      </c>
+      <c r="J82" s="16"/>
+      <c r="K82" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="L82" s="92"/>
       <c r="M82" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N82" s="4"/>
       <c r="O82" s="4" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="24">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" s="11" t="s">
-        <v>917</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="D83" s="19"/>
-      <c r="E83" s="19"/>
-      <c r="F83" s="16" t="s">
-        <v>922</v>
-      </c>
-      <c r="G83" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="H83" s="16" t="s">
-        <v>920</v>
+        <v>912</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C83" s="48" t="s">
+        <v>915</v>
+      </c>
+      <c r="D83" s="48"/>
+      <c r="E83" s="48"/>
+      <c r="F83" s="4">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G83" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I83" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J83" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K83" s="25" t="s">
-        <v>921</v>
-      </c>
-      <c r="L83" s="79"/>
+        <v>1099</v>
+      </c>
+      <c r="J83" s="16"/>
+      <c r="K83" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="L83" s="92"/>
       <c r="M83" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N83" s="4"/>
       <c r="O83" s="4" t="s">
-        <v>896</v>
+        <v>778</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="24">
       <c r="A84" s="11" t="s">
-        <v>923</v>
+        <v>917</v>
       </c>
       <c r="B84" s="16" t="s">
         <v>770</v>
@@ -25672,7 +25671,7 @@
         <v>893</v>
       </c>
       <c r="K84" s="25" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="L84" s="79"/>
       <c r="M84" s="60" t="s">
@@ -25685,7 +25684,7 @@
     </row>
     <row r="85" spans="1:15" ht="24">
       <c r="A85" s="11" t="s">
-        <v>923</v>
+        <v>917</v>
       </c>
       <c r="B85" s="16" t="s">
         <v>770</v>
@@ -25711,7 +25710,7 @@
         <v>893</v>
       </c>
       <c r="K85" s="25" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="L85" s="79"/>
       <c r="M85" s="60" t="s">
@@ -25724,31 +25723,33 @@
     </row>
     <row r="86" spans="1:15" ht="24">
       <c r="A86" s="11" t="s">
-        <v>925</v>
-      </c>
-      <c r="B86" s="17" t="s">
-        <v>852</v>
-      </c>
-      <c r="C86" s="48" t="s">
-        <v>913</v>
-      </c>
-      <c r="D86" s="48"/>
-      <c r="E86" s="48"/>
-      <c r="F86" s="4">
-        <v>1.26E-2</v>
-      </c>
-      <c r="G86" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H86" s="8" t="s">
-        <v>807</v>
+        <v>923</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>770</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="16" t="s">
+        <v>918</v>
+      </c>
+      <c r="G86" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="H86" s="16" t="s">
+        <v>920</v>
       </c>
       <c r="I86" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J86" s="16"/>
-      <c r="K86" s="16" t="s">
-        <v>926</v>
+        <v>1100</v>
+      </c>
+      <c r="J86" s="16" t="s">
+        <v>893</v>
+      </c>
+      <c r="K86" s="25" t="s">
+        <v>924</v>
       </c>
       <c r="L86" s="79"/>
       <c r="M86" s="60" t="s">
@@ -25756,36 +25757,38 @@
       </c>
       <c r="N86" s="4"/>
       <c r="O86" s="4" t="s">
-        <v>92</v>
+        <v>896</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="24">
       <c r="A87" s="11" t="s">
-        <v>925</v>
-      </c>
-      <c r="B87" s="17" t="s">
-        <v>852</v>
-      </c>
-      <c r="C87" s="48" t="s">
-        <v>915</v>
-      </c>
-      <c r="D87" s="48"/>
-      <c r="E87" s="48"/>
-      <c r="F87" s="4">
-        <v>1.5800000000000002E-2</v>
-      </c>
-      <c r="G87" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H87" s="8" t="s">
-        <v>807</v>
+        <v>923</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>770</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="16" t="s">
+        <v>922</v>
+      </c>
+      <c r="G87" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="H87" s="16" t="s">
+        <v>920</v>
       </c>
       <c r="I87" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16" t="s">
-        <v>927</v>
+        <v>1100</v>
+      </c>
+      <c r="J87" s="16" t="s">
+        <v>893</v>
+      </c>
+      <c r="K87" s="25" t="s">
+        <v>924</v>
       </c>
       <c r="L87" s="79"/>
       <c r="M87" s="60" t="s">
@@ -25793,108 +25796,110 @@
       </c>
       <c r="N87" s="4"/>
       <c r="O87" s="4" t="s">
-        <v>92</v>
+        <v>896</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="24">
       <c r="A88" s="11" t="s">
-        <v>928</v>
-      </c>
-      <c r="B88" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="C88" s="19" t="s">
-        <v>368</v>
-      </c>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="16" t="s">
-        <v>918</v>
-      </c>
-      <c r="G88" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="H88" s="16" t="s">
-        <v>920</v>
+        <v>925</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C88" s="48" t="s">
+        <v>913</v>
+      </c>
+      <c r="D88" s="48"/>
+      <c r="E88" s="48"/>
+      <c r="F88" s="4">
+        <v>1.26E-2</v>
+      </c>
+      <c r="G88" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I88" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J88" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K88" s="25"/>
+        <v>1099</v>
+      </c>
+      <c r="J88" s="16"/>
+      <c r="K88" s="16" t="s">
+        <v>926</v>
+      </c>
       <c r="L88" s="79"/>
       <c r="M88" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N88" s="4"/>
       <c r="O88" s="4" t="s">
-        <v>896</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="24">
       <c r="A89" s="11" t="s">
-        <v>928</v>
-      </c>
-      <c r="B89" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="16" t="s">
-        <v>922</v>
-      </c>
-      <c r="G89" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="H89" s="16" t="s">
-        <v>920</v>
+        <v>925</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C89" s="48" t="s">
+        <v>915</v>
+      </c>
+      <c r="D89" s="48"/>
+      <c r="E89" s="48"/>
+      <c r="F89" s="4">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G89" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I89" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J89" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K89" s="25"/>
+        <v>1099</v>
+      </c>
+      <c r="J89" s="16"/>
+      <c r="K89" s="16" t="s">
+        <v>927</v>
+      </c>
       <c r="L89" s="79"/>
       <c r="M89" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N89" s="4"/>
       <c r="O89" s="4" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" ht="36">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="24">
       <c r="A90" s="11" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C90" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="D90" s="48"/>
-      <c r="E90" s="48"/>
-      <c r="F90" s="93" t="s">
-        <v>930</v>
-      </c>
-      <c r="G90" s="87" t="s">
-        <v>931</v>
+        <v>770</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="16" t="s">
+        <v>918</v>
+      </c>
+      <c r="G90" s="16" t="s">
+        <v>919</v>
       </c>
       <c r="H90" s="16" t="s">
-        <v>932</v>
+        <v>920</v>
       </c>
       <c r="I90" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J90" s="16"/>
+        <v>1100</v>
+      </c>
+      <c r="J90" s="16" t="s">
+        <v>893</v>
+      </c>
       <c r="K90" s="25"/>
       <c r="L90" s="79"/>
       <c r="M90" s="60" t="s">
@@ -25902,109 +25907,107 @@
       </c>
       <c r="N90" s="4"/>
       <c r="O90" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" ht="39" customHeight="1">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="24">
       <c r="A91" s="11" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C91" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="D91" s="48"/>
-      <c r="E91" s="48"/>
+        <v>770</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
       <c r="F91" s="16" t="s">
-        <v>934</v>
-      </c>
-      <c r="G91" s="87" t="s">
-        <v>935</v>
+        <v>922</v>
+      </c>
+      <c r="G91" s="16" t="s">
+        <v>919</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>936</v>
+        <v>920</v>
       </c>
       <c r="I91" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J91" s="16"/>
-      <c r="K91"/>
+        <v>1100</v>
+      </c>
+      <c r="J91" s="16" t="s">
+        <v>893</v>
+      </c>
+      <c r="K91" s="25"/>
       <c r="L91" s="79"/>
       <c r="M91" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N91" s="4"/>
       <c r="O91" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" ht="24">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="36">
       <c r="A92" s="11" t="s">
-        <v>937</v>
-      </c>
-      <c r="B92" s="17" t="s">
-        <v>852</v>
+        <v>929</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>190</v>
       </c>
       <c r="C92" s="48" t="s">
-        <v>913</v>
+        <v>43</v>
       </c>
       <c r="D92" s="48"/>
       <c r="E92" s="48"/>
-      <c r="F92" s="4">
-        <v>1.54E-2</v>
-      </c>
-      <c r="G92" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>807</v>
+      <c r="F92" s="93" t="s">
+        <v>930</v>
+      </c>
+      <c r="G92" s="87" t="s">
+        <v>931</v>
+      </c>
+      <c r="H92" s="16" t="s">
+        <v>932</v>
       </c>
       <c r="I92" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J92" s="16"/>
-      <c r="K92" s="16" t="s">
-        <v>926</v>
-      </c>
+      <c r="K92" s="25"/>
       <c r="L92" s="79"/>
       <c r="M92" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N92" s="4"/>
       <c r="O92" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" ht="24">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="39" customHeight="1">
       <c r="A93" s="11" t="s">
-        <v>937</v>
-      </c>
-      <c r="B93" s="17" t="s">
-        <v>852</v>
+        <v>933</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>190</v>
       </c>
       <c r="C93" s="48" t="s">
-        <v>915</v>
+        <v>43</v>
       </c>
       <c r="D93" s="48"/>
       <c r="E93" s="48"/>
-      <c r="F93" s="4">
-        <v>1.9300000000000001E-2</v>
-      </c>
-      <c r="G93" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H93" s="8" t="s">
-        <v>807</v>
+      <c r="F93" s="16" t="s">
+        <v>934</v>
+      </c>
+      <c r="G93" s="87" t="s">
+        <v>935</v>
+      </c>
+      <c r="H93" s="16" t="s">
+        <v>936</v>
       </c>
       <c r="I93" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J93" s="16"/>
-      <c r="K93" s="16" t="s">
-        <v>927</v>
-      </c>
+      <c r="K93"/>
       <c r="L93" s="79"/>
       <c r="M93" s="60" t="s">
         <v>895</v>
@@ -26016,103 +26019,105 @@
     </row>
     <row r="94" spans="1:15" ht="24">
       <c r="A94" s="11" t="s">
-        <v>938</v>
-      </c>
-      <c r="B94" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="C94" s="19" t="s">
-        <v>368</v>
-      </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="16" t="s">
-        <v>918</v>
-      </c>
-      <c r="G94" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="H94" s="16" t="s">
-        <v>920</v>
+        <v>937</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C94" s="48" t="s">
+        <v>913</v>
+      </c>
+      <c r="D94" s="48"/>
+      <c r="E94" s="48"/>
+      <c r="F94" s="4">
+        <v>1.54E-2</v>
+      </c>
+      <c r="G94" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H94" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I94" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J94" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K94" s="25"/>
+        <v>1099</v>
+      </c>
+      <c r="J94" s="16"/>
+      <c r="K94" s="16" t="s">
+        <v>926</v>
+      </c>
       <c r="L94" s="79"/>
       <c r="M94" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N94" s="4"/>
       <c r="O94" s="4" t="s">
-        <v>896</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="24">
       <c r="A95" s="11" t="s">
-        <v>938</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>770</v>
-      </c>
-      <c r="C95" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="16" t="s">
-        <v>922</v>
-      </c>
-      <c r="G95" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="H95" s="16" t="s">
-        <v>920</v>
+        <v>937</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C95" s="48" t="s">
+        <v>915</v>
+      </c>
+      <c r="D95" s="48"/>
+      <c r="E95" s="48"/>
+      <c r="F95" s="4">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="G95" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H95" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I95" s="16" t="s">
-        <v>1100</v>
-      </c>
-      <c r="J95" s="16" t="s">
-        <v>893</v>
-      </c>
-      <c r="K95" s="25"/>
+        <v>1099</v>
+      </c>
+      <c r="J95" s="16"/>
+      <c r="K95" s="16" t="s">
+        <v>927</v>
+      </c>
       <c r="L95" s="79"/>
       <c r="M95" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N95" s="4"/>
       <c r="O95" s="4" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" ht="36">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="24">
       <c r="A96" s="11" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C96" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="D96" s="48"/>
-      <c r="E96" s="48"/>
-      <c r="F96" s="93" t="s">
-        <v>930</v>
-      </c>
-      <c r="G96" s="87" t="s">
-        <v>931</v>
+        <v>770</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="16" t="s">
+        <v>918</v>
+      </c>
+      <c r="G96" s="16" t="s">
+        <v>919</v>
       </c>
       <c r="H96" s="16" t="s">
-        <v>932</v>
+        <v>920</v>
       </c>
       <c r="I96" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J96" s="16"/>
+        <v>1100</v>
+      </c>
+      <c r="J96" s="16" t="s">
+        <v>893</v>
+      </c>
       <c r="K96" s="25"/>
       <c r="L96" s="79"/>
       <c r="M96" s="60" t="s">
@@ -26120,34 +26125,36 @@
       </c>
       <c r="N96" s="4"/>
       <c r="O96" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="36.75" customHeight="1">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="24">
       <c r="A97" s="11" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C97" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="D97" s="48"/>
-      <c r="E97" s="48"/>
+        <v>770</v>
+      </c>
+      <c r="C97" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
       <c r="F97" s="16" t="s">
-        <v>934</v>
-      </c>
-      <c r="G97" s="87" t="s">
-        <v>935</v>
+        <v>922</v>
+      </c>
+      <c r="G97" s="16" t="s">
+        <v>919</v>
       </c>
       <c r="H97" s="16" t="s">
-        <v>936</v>
+        <v>920</v>
       </c>
       <c r="I97" s="16" t="s">
-        <v>1099</v>
-      </c>
-      <c r="J97" s="16"/>
+        <v>1100</v>
+      </c>
+      <c r="J97" s="16" t="s">
+        <v>893</v>
+      </c>
       <c r="K97" s="25"/>
       <c r="L97" s="79"/>
       <c r="M97" s="60" t="s">
@@ -26155,110 +26162,106 @@
       </c>
       <c r="N97" s="4"/>
       <c r="O97" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="36">
       <c r="A98" s="11" t="s">
-        <v>941</v>
-      </c>
-      <c r="B98" s="17" t="s">
-        <v>852</v>
+        <v>939</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>190</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>780</v>
+        <v>43</v>
       </c>
       <c r="D98" s="48"/>
       <c r="E98" s="48"/>
-      <c r="F98" s="94">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="G98" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H98" s="8" t="s">
-        <v>807</v>
+      <c r="F98" s="93" t="s">
+        <v>930</v>
+      </c>
+      <c r="G98" s="87" t="s">
+        <v>931</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>932</v>
       </c>
       <c r="I98" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J98" s="16"/>
-      <c r="K98" s="16" t="s">
-        <v>942</v>
-      </c>
+      <c r="K98" s="25"/>
       <c r="L98" s="79"/>
       <c r="M98" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N98" s="4"/>
       <c r="O98" s="4" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" ht="36.75" customHeight="1">
       <c r="A99" s="11" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="B99" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="C99" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19"/>
+      <c r="C99" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D99" s="48"/>
+      <c r="E99" s="48"/>
       <c r="F99" s="16" t="s">
-        <v>944</v>
+        <v>934</v>
       </c>
       <c r="G99" s="87" t="s">
-        <v>95</v>
+        <v>935</v>
       </c>
       <c r="H99" s="16" t="s">
-        <v>945</v>
+        <v>936</v>
       </c>
       <c r="I99" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J99" s="16"/>
-      <c r="K99" s="25" t="s">
-        <v>946</v>
-      </c>
+      <c r="K99" s="25"/>
       <c r="L99" s="79"/>
       <c r="M99" s="60" t="s">
         <v>895</v>
       </c>
       <c r="N99" s="4"/>
       <c r="O99" s="4" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:15">
       <c r="A100" s="11" t="s">
-        <v>947</v>
-      </c>
-      <c r="B100" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C100" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D100" s="19"/>
-      <c r="E100" s="19"/>
-      <c r="F100" s="48" t="s">
-        <v>948</v>
+        <v>941</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C100" s="48" t="s">
+        <v>780</v>
+      </c>
+      <c r="D100" s="48"/>
+      <c r="E100" s="48"/>
+      <c r="F100" s="94">
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="G100" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="H100" s="16" t="s">
-        <v>945</v>
+      <c r="H100" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I100" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J100" s="16"/>
-      <c r="K100" s="25" t="s">
-        <v>946</v>
+      <c r="K100" s="16" t="s">
+        <v>942</v>
       </c>
       <c r="L100" s="79"/>
       <c r="M100" s="60" t="s">
@@ -26266,36 +26269,36 @@
       </c>
       <c r="N100" s="4"/>
       <c r="O100" s="4" t="s">
-        <v>92</v>
+        <v>778</v>
       </c>
     </row>
     <row r="101" spans="1:15">
       <c r="A101" s="11" t="s">
-        <v>949</v>
-      </c>
-      <c r="B101" s="17" t="s">
-        <v>852</v>
-      </c>
-      <c r="C101" s="48" t="s">
-        <v>780</v>
-      </c>
-      <c r="D101" s="48"/>
-      <c r="E101" s="48"/>
-      <c r="F101" s="82">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="G101" s="48" t="s">
+        <v>943</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C101" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="16" t="s">
+        <v>944</v>
+      </c>
+      <c r="G101" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="H101" s="8" t="s">
-        <v>807</v>
+      <c r="H101" s="16" t="s">
+        <v>945</v>
       </c>
       <c r="I101" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J101" s="16"/>
-      <c r="K101" s="16" t="s">
-        <v>950</v>
+      <c r="K101" s="25" t="s">
+        <v>946</v>
       </c>
       <c r="L101" s="79"/>
       <c r="M101" s="60" t="s">
@@ -26303,12 +26306,12 @@
       </c>
       <c r="N101" s="4"/>
       <c r="O101" s="4" t="s">
-        <v>778</v>
+        <v>113</v>
       </c>
     </row>
     <row r="102" spans="1:15">
       <c r="A102" s="11" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="B102" s="16" t="s">
         <v>190</v>
@@ -26318,10 +26321,10 @@
       </c>
       <c r="D102" s="19"/>
       <c r="E102" s="19"/>
-      <c r="F102" s="16" t="s">
-        <v>944</v>
-      </c>
-      <c r="G102" s="87" t="s">
+      <c r="F102" s="48" t="s">
+        <v>948</v>
+      </c>
+      <c r="G102" s="48" t="s">
         <v>95</v>
       </c>
       <c r="H102" s="16" t="s">
@@ -26340,36 +26343,36 @@
       </c>
       <c r="N102" s="4"/>
       <c r="O102" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" ht="14.25" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
       <c r="A103" s="11" t="s">
-        <v>952</v>
-      </c>
-      <c r="B103" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C103" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="48" t="s">
-        <v>948</v>
+        <v>949</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="C103" s="48" t="s">
+        <v>780</v>
+      </c>
+      <c r="D103" s="48"/>
+      <c r="E103" s="48"/>
+      <c r="F103" s="82">
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="G103" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="H103" s="16" t="s">
-        <v>945</v>
+      <c r="H103" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="I103" s="16" t="s">
         <v>1099</v>
       </c>
       <c r="J103" s="16"/>
-      <c r="K103" s="25" t="s">
-        <v>946</v>
+      <c r="K103" s="16" t="s">
+        <v>950</v>
       </c>
       <c r="L103" s="79"/>
       <c r="M103" s="60" t="s">
@@ -26377,6 +26380,80 @@
       </c>
       <c r="N103" s="4"/>
       <c r="O103" s="4" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
+      <c r="A104" s="11" t="s">
+        <v>951</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C104" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="16" t="s">
+        <v>944</v>
+      </c>
+      <c r="G104" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="H104" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="I104" s="16" t="s">
+        <v>1099</v>
+      </c>
+      <c r="J104" s="16"/>
+      <c r="K104" s="25" t="s">
+        <v>946</v>
+      </c>
+      <c r="L104" s="79"/>
+      <c r="M104" s="60" t="s">
+        <v>895</v>
+      </c>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A105" s="11" t="s">
+        <v>952</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C105" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="48" t="s">
+        <v>948</v>
+      </c>
+      <c r="G105" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="H105" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="I105" s="16" t="s">
+        <v>1099</v>
+      </c>
+      <c r="J105" s="16"/>
+      <c r="K105" s="25" t="s">
+        <v>946</v>
+      </c>
+      <c r="L105" s="79"/>
+      <c r="M105" s="60" t="s">
+        <v>895</v>
+      </c>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update new respiratory validation value.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90BC3F6-9178-4A61-B441-9A1276E6EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87100431-5CC4-4BE7-8FFE-FEE2BA989BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23490" yWindow="3615" windowWidth="27480" windowHeight="23535" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4728" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4729" uniqueCount="1113">
   <si>
     <t>Patient Inputs</t>
   </si>
@@ -3508,6 +3508,9 @@
   </si>
   <si>
     <t>cala2004vd</t>
+  </si>
+  <si>
+    <t>[0.8, 1.0]</t>
   </si>
 </sst>
 </file>
@@ -22795,9 +22798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G37" sqref="G37"/>
+      <selection pane="topRight" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25123,8 +25126,8 @@
       </c>
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
-      <c r="F70" s="48">
-        <v>0.8</v>
+      <c r="F70" s="48" t="s">
+        <v>1112</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>1108</v>

</xml_diff>